<commit_message>
Design Figure Mock-Ups & Note Added to Critical Item (Master File)
</commit_message>
<xml_diff>
--- a/Writeups/Exp.1_Master.xlsx
+++ b/Writeups/Exp.1_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\Social.Influence_Speech.Perception\SI.SP\Writeups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A69D6EF-9415-4449-A1F1-B227D2787B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40260C03-AA70-408E-8AAB-F397728AE770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{6F4FE53E-24C5-4985-9E6F-6A265A63BA90}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6F4FE53E-24C5-4985-9E6F-6A265A63BA90}"/>
   </bookViews>
   <sheets>
     <sheet name="Exposure Phase" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="201">
   <si>
     <t>Critical Items</t>
   </si>
@@ -1135,12 +1135,42 @@
   <si>
     <t>Shifted ?sh</t>
   </si>
+  <si>
+    <t>Needs Work!!</t>
+  </si>
+  <si>
+    <t>Version 1</t>
+  </si>
+  <si>
+    <t>Version 2</t>
+  </si>
+  <si>
+    <t>Version 3</t>
+  </si>
+  <si>
+    <t>Version 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Word </t>
+  </si>
+  <si>
+    <t>Same</t>
+  </si>
+  <si>
+    <t>Opposite</t>
+  </si>
+  <si>
+    <t>^^ Compared to the ear and gender of the attended talker</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1229,6 +1259,12 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Sylfaen"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Sylfaen"/>
       <family val="1"/>
@@ -1524,7 +1560,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="55">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -2192,11 +2228,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="338">
+  <cellXfs count="355">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2841,51 +2912,132 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2902,98 +3054,59 @@
       <alignment horizontal="left" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3006,6 +3119,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="44" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="44" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="44" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3045,52 +3170,49 @@
     <xf numFmtId="0" fontId="3" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="44" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="44" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="44" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="37" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3101,8 +3223,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD1DFA9"/>
       <color rgb="FFB5CC76"/>
-      <color rgb="FFD1DFA9"/>
       <color rgb="FFFFDAA3"/>
       <color rgb="FF77CEF9"/>
       <color rgb="FFB2E3FC"/>
@@ -4758,7 +4880,7 @@
   </sheetPr>
   <dimension ref="A1:AH718"/>
   <sheetViews>
-    <sheetView zoomScale="65" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AL19" sqref="AL19"/>
     </sheetView>
   </sheetViews>
@@ -4803,14 +4925,14 @@
       <c r="AB1" s="5"/>
     </row>
     <row r="2" spans="1:34" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="260" t="s">
+      <c r="B2" s="268" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="260"/>
-      <c r="D2" s="260"/>
-      <c r="E2" s="260"/>
-      <c r="F2" s="260"/>
-      <c r="G2" s="260"/>
+      <c r="C2" s="268"/>
+      <c r="D2" s="268"/>
+      <c r="E2" s="268"/>
+      <c r="F2" s="268"/>
+      <c r="G2" s="268"/>
       <c r="H2" s="20"/>
       <c r="I2" s="13" t="s">
         <v>179</v>
@@ -4820,40 +4942,40 @@
         <v>17</v>
       </c>
       <c r="L2" s="20"/>
-      <c r="M2" s="260" t="s">
+      <c r="M2" s="268" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="260"/>
-      <c r="O2" s="260"/>
-      <c r="P2" s="260"/>
-      <c r="Q2" s="260"/>
-      <c r="R2" s="260"/>
-      <c r="S2" s="260"/>
-      <c r="T2" s="260"/>
-      <c r="U2" s="260"/>
-      <c r="V2" s="260"/>
-      <c r="W2" s="260"/>
-      <c r="X2" s="260"/>
-      <c r="Y2" s="260"/>
-      <c r="Z2" s="260"/>
-      <c r="AA2" s="260"/>
-      <c r="AB2" s="260"/>
+      <c r="N2" s="268"/>
+      <c r="O2" s="268"/>
+      <c r="P2" s="268"/>
+      <c r="Q2" s="268"/>
+      <c r="R2" s="268"/>
+      <c r="S2" s="268"/>
+      <c r="T2" s="268"/>
+      <c r="U2" s="268"/>
+      <c r="V2" s="268"/>
+      <c r="W2" s="268"/>
+      <c r="X2" s="268"/>
+      <c r="Y2" s="268"/>
+      <c r="Z2" s="268"/>
+      <c r="AA2" s="268"/>
+      <c r="AB2" s="268"/>
     </row>
     <row r="3" spans="1:34" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="261" t="s">
+      <c r="B3" s="269" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="262"/>
-      <c r="D3" s="262"/>
-      <c r="E3" s="262"/>
-      <c r="F3" s="262"/>
-      <c r="G3" s="263"/>
+      <c r="C3" s="270"/>
+      <c r="D3" s="270"/>
+      <c r="E3" s="270"/>
+      <c r="F3" s="270"/>
+      <c r="G3" s="271"/>
       <c r="H3" s="28"/>
-      <c r="I3" s="264" t="s">
+      <c r="I3" s="272" t="s">
         <v>25</v>
       </c>
       <c r="J3" s="28"/>
-      <c r="K3" s="264" t="s">
+      <c r="K3" s="272" t="s">
         <v>27</v>
       </c>
       <c r="L3" s="3"/>
@@ -4861,26 +4983,26 @@
         <v>21</v>
       </c>
       <c r="N3" s="251"/>
-      <c r="O3" s="254" t="s">
+      <c r="O3" s="276" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="254"/>
-      <c r="Q3" s="254"/>
-      <c r="R3" s="254"/>
+      <c r="P3" s="276"/>
+      <c r="Q3" s="276"/>
+      <c r="R3" s="276"/>
       <c r="S3" s="191"/>
-      <c r="T3" s="254" t="s">
+      <c r="T3" s="276" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="254"/>
-      <c r="V3" s="254"/>
-      <c r="W3" s="254"/>
+      <c r="U3" s="276"/>
+      <c r="V3" s="276"/>
+      <c r="W3" s="276"/>
       <c r="X3" s="190"/>
-      <c r="Y3" s="254" t="s">
+      <c r="Y3" s="276" t="s">
         <v>14</v>
       </c>
-      <c r="Z3" s="254"/>
-      <c r="AA3" s="254"/>
-      <c r="AB3" s="255"/>
+      <c r="Z3" s="276"/>
+      <c r="AA3" s="276"/>
+      <c r="AB3" s="277"/>
     </row>
     <row r="4" spans="1:34" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D4" s="4"/>
@@ -4888,34 +5010,34 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="265"/>
+      <c r="I4" s="274"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="256"/>
+      <c r="K4" s="273"/>
       <c r="L4" s="5"/>
-      <c r="M4" s="256" t="s">
+      <c r="M4" s="273" t="s">
         <v>180</v>
       </c>
       <c r="N4" s="193"/>
-      <c r="O4" s="266" t="s">
+      <c r="O4" s="275" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="266"/>
-      <c r="Q4" s="266"/>
-      <c r="R4" s="266"/>
+      <c r="P4" s="275"/>
+      <c r="Q4" s="275"/>
+      <c r="R4" s="275"/>
       <c r="S4" s="192"/>
-      <c r="T4" s="266" t="s">
+      <c r="T4" s="275" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="266"/>
-      <c r="V4" s="266"/>
-      <c r="W4" s="266"/>
+      <c r="U4" s="275"/>
+      <c r="V4" s="275"/>
+      <c r="W4" s="275"/>
       <c r="X4" s="193"/>
-      <c r="Y4" s="266" t="s">
+      <c r="Y4" s="275" t="s">
         <v>30</v>
       </c>
-      <c r="Z4" s="266"/>
-      <c r="AA4" s="266"/>
-      <c r="AB4" s="266"/>
+      <c r="Z4" s="275"/>
+      <c r="AA4" s="275"/>
+      <c r="AB4" s="275"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="C5" s="4" t="s">
@@ -4934,10 +5056,10 @@
         <v>3</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="265"/>
+      <c r="I5" s="274"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="256"/>
-      <c r="M5" s="256"/>
+      <c r="K5" s="273"/>
+      <c r="M5" s="273"/>
       <c r="N5" s="194"/>
       <c r="O5" s="7" t="s">
         <v>18</v>
@@ -5007,10 +5129,10 @@
       <c r="AA6" s="10"/>
       <c r="AB6" s="9"/>
       <c r="AE6" s="33"/>
-      <c r="AF6" s="257" t="s">
+      <c r="AF6" s="266" t="s">
         <v>28</v>
       </c>
-      <c r="AG6" s="258"/>
+      <c r="AG6" s="278"/>
       <c r="AH6" s="32"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.35">
@@ -5082,8 +5204,8 @@
         <v>9</v>
       </c>
       <c r="AE7" s="34"/>
-      <c r="AF7" s="257"/>
-      <c r="AG7" s="258"/>
+      <c r="AF7" s="266"/>
+      <c r="AG7" s="278"/>
       <c r="AH7" s="32"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.35">
@@ -5136,8 +5258,8 @@
         <v>8</v>
       </c>
       <c r="AE8" s="34"/>
-      <c r="AF8" s="257"/>
-      <c r="AG8" s="258"/>
+      <c r="AF8" s="266"/>
+      <c r="AG8" s="278"/>
       <c r="AH8" s="32"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.35">
@@ -5168,8 +5290,8 @@
       <c r="AA9" s="12"/>
       <c r="AB9" s="14"/>
       <c r="AE9" s="34"/>
-      <c r="AF9" s="257"/>
-      <c r="AG9" s="258"/>
+      <c r="AF9" s="266"/>
+      <c r="AG9" s="278"/>
       <c r="AH9" s="32"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.35">
@@ -5228,8 +5350,8 @@
         <v>9</v>
       </c>
       <c r="AE10" s="34"/>
-      <c r="AF10" s="257"/>
-      <c r="AG10" s="258"/>
+      <c r="AF10" s="266"/>
+      <c r="AG10" s="278"/>
       <c r="AH10" s="32"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.35">
@@ -5272,8 +5394,8 @@
         <v>8</v>
       </c>
       <c r="AE11" s="35"/>
-      <c r="AF11" s="257"/>
-      <c r="AG11" s="258"/>
+      <c r="AF11" s="266"/>
+      <c r="AG11" s="278"/>
       <c r="AH11" s="32"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.35">
@@ -5580,10 +5702,10 @@
       <c r="AA18" s="9"/>
       <c r="AB18" s="9"/>
       <c r="AE18" s="37"/>
-      <c r="AF18" s="257" t="s">
+      <c r="AF18" s="266" t="s">
         <v>28</v>
       </c>
-      <c r="AG18" s="259"/>
+      <c r="AG18" s="267"/>
     </row>
     <row r="19" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B19" s="11">
@@ -5654,8 +5776,8 @@
         <v>9</v>
       </c>
       <c r="AE19" s="2"/>
-      <c r="AF19" s="257"/>
-      <c r="AG19" s="259"/>
+      <c r="AF19" s="266"/>
+      <c r="AG19" s="267"/>
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B20" s="20"/>
@@ -5707,8 +5829,8 @@
         <v>8</v>
       </c>
       <c r="AE20" s="2"/>
-      <c r="AF20" s="257"/>
-      <c r="AG20" s="259"/>
+      <c r="AF20" s="266"/>
+      <c r="AG20" s="267"/>
     </row>
     <row r="21" spans="2:33" x14ac:dyDescent="0.35">
       <c r="C21" s="23"/>
@@ -5738,8 +5860,8 @@
       <c r="AA21" s="12"/>
       <c r="AB21" s="14"/>
       <c r="AE21" s="2"/>
-      <c r="AF21" s="257"/>
-      <c r="AG21" s="259"/>
+      <c r="AF21" s="266"/>
+      <c r="AG21" s="267"/>
     </row>
     <row r="22" spans="2:33" x14ac:dyDescent="0.35">
       <c r="C22" s="23"/>
@@ -5797,8 +5919,8 @@
         <v>9</v>
       </c>
       <c r="AE22" s="2"/>
-      <c r="AF22" s="257"/>
-      <c r="AG22" s="259"/>
+      <c r="AF22" s="266"/>
+      <c r="AG22" s="267"/>
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.35">
       <c r="C23" s="23"/>
@@ -5839,8 +5961,8 @@
         <v>8</v>
       </c>
       <c r="AE23" s="36"/>
-      <c r="AF23" s="257"/>
-      <c r="AG23" s="259"/>
+      <c r="AF23" s="266"/>
+      <c r="AG23" s="267"/>
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B24" s="11"/>
@@ -23072,8 +23194,8 @@
   </sheetPr>
   <dimension ref="B2:AO41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="144" workbookViewId="0">
-      <selection activeCell="AP5" sqref="AP5:AT27"/>
+    <sheetView topLeftCell="H1" zoomScale="73" zoomScaleNormal="144" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -23122,11 +23244,11 @@
       <c r="C3" s="189" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="287" t="s">
+      <c r="D3" s="280" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="274"/>
-      <c r="F3" s="274"/>
+      <c r="E3" s="281"/>
+      <c r="F3" s="281"/>
       <c r="G3" s="79"/>
       <c r="H3" s="188" t="s">
         <v>76</v>
@@ -23134,46 +23256,46 @@
       <c r="I3" s="189" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="287" t="s">
+      <c r="J3" s="280" t="s">
         <v>79</v>
       </c>
-      <c r="K3" s="274"/>
-      <c r="L3" s="274"/>
-      <c r="N3" s="289" t="s">
+      <c r="K3" s="281"/>
+      <c r="L3" s="281"/>
+      <c r="N3" s="282" t="s">
         <v>80</v>
       </c>
-      <c r="O3" s="289"/>
+      <c r="O3" s="282"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="289" t="s">
+      <c r="Q3" s="282" t="s">
         <v>81</v>
       </c>
-      <c r="R3" s="289"/>
+      <c r="R3" s="282"/>
       <c r="S3" s="19"/>
       <c r="T3" s="179"/>
       <c r="U3" s="179"/>
-      <c r="V3" s="269" t="s">
+      <c r="V3" s="296" t="s">
         <v>80</v>
       </c>
-      <c r="W3" s="269"/>
-      <c r="X3" s="269"/>
+      <c r="W3" s="296"/>
+      <c r="X3" s="296"/>
       <c r="Y3" s="179"/>
       <c r="Z3" s="179"/>
-      <c r="AB3" s="267" t="s">
+      <c r="AB3" s="279" t="s">
         <v>157</v>
       </c>
-      <c r="AC3" s="267"/>
-      <c r="AD3" s="267"/>
-      <c r="AE3" s="267"/>
-      <c r="AF3" s="267"/>
-      <c r="AG3" s="267"/>
-      <c r="AH3" s="267"/>
-      <c r="AI3" s="267"/>
-      <c r="AJ3" s="267"/>
-      <c r="AL3" s="267" t="s">
+      <c r="AC3" s="279"/>
+      <c r="AD3" s="279"/>
+      <c r="AE3" s="279"/>
+      <c r="AF3" s="279"/>
+      <c r="AG3" s="279"/>
+      <c r="AH3" s="279"/>
+      <c r="AI3" s="279"/>
+      <c r="AJ3" s="279"/>
+      <c r="AL3" s="279" t="s">
         <v>32</v>
       </c>
-      <c r="AM3" s="267"/>
-      <c r="AN3" s="267"/>
+      <c r="AM3" s="279"/>
+      <c r="AN3" s="279"/>
     </row>
     <row r="4" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="97" t="s">
@@ -23182,9 +23304,9 @@
       <c r="C4" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="287"/>
-      <c r="E4" s="274"/>
-      <c r="F4" s="274"/>
+      <c r="D4" s="280"/>
+      <c r="E4" s="281"/>
+      <c r="F4" s="281"/>
       <c r="G4" s="79"/>
       <c r="H4" s="97" t="s">
         <v>82</v>
@@ -23192,9 +23314,9 @@
       <c r="I4" s="93" t="s">
         <v>84</v>
       </c>
-      <c r="J4" s="287"/>
-      <c r="K4" s="274"/>
-      <c r="L4" s="274"/>
+      <c r="J4" s="280"/>
+      <c r="K4" s="281"/>
+      <c r="L4" s="281"/>
       <c r="N4" s="86" t="s">
         <v>76</v>
       </c>
@@ -23214,11 +23336,11 @@
       <c r="W4" s="116"/>
       <c r="X4" s="117"/>
       <c r="Z4" s="179"/>
-      <c r="AL4" s="275" t="s">
+      <c r="AL4" s="295" t="s">
         <v>160</v>
       </c>
-      <c r="AM4" s="275"/>
-      <c r="AN4" s="275"/>
+      <c r="AM4" s="295"/>
+      <c r="AN4" s="295"/>
     </row>
     <row r="5" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="94" t="s">
@@ -23227,11 +23349,11 @@
       <c r="C5" s="98" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="287" t="s">
+      <c r="D5" s="280" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="274"/>
-      <c r="F5" s="274"/>
+      <c r="E5" s="281"/>
+      <c r="F5" s="281"/>
       <c r="G5" s="79"/>
       <c r="H5" s="94" t="s">
         <v>87</v>
@@ -23239,9 +23361,9 @@
       <c r="I5" s="98" t="s">
         <v>90</v>
       </c>
-      <c r="J5" s="287"/>
-      <c r="K5" s="274"/>
-      <c r="L5" s="274"/>
+      <c r="J5" s="280"/>
+      <c r="K5" s="281"/>
+      <c r="L5" s="281"/>
       <c r="N5" s="154" t="s">
         <v>149</v>
       </c>
@@ -23256,7 +23378,7 @@
         <v>149</v>
       </c>
       <c r="S5" s="19"/>
-      <c r="T5" s="271" t="s">
+      <c r="T5" s="298" t="s">
         <v>149</v>
       </c>
       <c r="U5" s="118"/>
@@ -23268,24 +23390,24 @@
         <v>84</v>
       </c>
       <c r="Y5" s="121"/>
-      <c r="Z5" s="273" t="s">
+      <c r="Z5" s="300" t="s">
         <v>150</v>
       </c>
       <c r="AA5" s="179"/>
-      <c r="AB5" s="267" t="s">
+      <c r="AB5" s="279" t="s">
         <v>189</v>
       </c>
-      <c r="AC5" s="267"/>
-      <c r="AD5" s="267"/>
-      <c r="AE5" s="267"/>
-      <c r="AF5" s="267"/>
-      <c r="AG5" s="267"/>
-      <c r="AH5" s="267"/>
-      <c r="AI5" s="267"/>
-      <c r="AJ5" s="267"/>
-      <c r="AL5" s="275"/>
-      <c r="AM5" s="275"/>
-      <c r="AN5" s="275"/>
+      <c r="AC5" s="279"/>
+      <c r="AD5" s="279"/>
+      <c r="AE5" s="279"/>
+      <c r="AF5" s="279"/>
+      <c r="AG5" s="279"/>
+      <c r="AH5" s="279"/>
+      <c r="AI5" s="279"/>
+      <c r="AJ5" s="279"/>
+      <c r="AL5" s="295"/>
+      <c r="AM5" s="295"/>
+      <c r="AN5" s="295"/>
       <c r="AO5" s="19"/>
     </row>
     <row r="6" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -23305,9 +23427,9 @@
       <c r="I6" s="95" t="s">
         <v>95</v>
       </c>
-      <c r="J6" s="287"/>
-      <c r="K6" s="274"/>
-      <c r="L6" s="274"/>
+      <c r="J6" s="280"/>
+      <c r="K6" s="281"/>
+      <c r="L6" s="281"/>
       <c r="N6" s="119" t="s">
         <v>82</v>
       </c>
@@ -23321,7 +23443,7 @@
         <v>85</v>
       </c>
       <c r="S6" s="19"/>
-      <c r="T6" s="272"/>
+      <c r="T6" s="299"/>
       <c r="U6" s="122"/>
       <c r="V6" s="80" t="s">
         <v>91</v>
@@ -23331,12 +23453,12 @@
         <v>101</v>
       </c>
       <c r="Y6" s="124"/>
-      <c r="Z6" s="273"/>
+      <c r="Z6" s="300"/>
       <c r="AA6" s="179"/>
       <c r="AB6" s="177" t="s">
         <v>86</v>
       </c>
-      <c r="AC6" s="328" t="s">
+      <c r="AC6" s="256" t="s">
         <v>77</v>
       </c>
       <c r="AD6" s="169" t="s">
@@ -23352,15 +23474,15 @@
       <c r="AH6" s="164" t="s">
         <v>77</v>
       </c>
-      <c r="AI6" s="328" t="s">
+      <c r="AI6" s="256" t="s">
         <v>76</v>
       </c>
       <c r="AJ6" s="171" t="s">
         <v>86</v>
       </c>
-      <c r="AL6" s="275"/>
-      <c r="AM6" s="275"/>
-      <c r="AN6" s="275"/>
+      <c r="AL6" s="295"/>
+      <c r="AM6" s="295"/>
+      <c r="AN6" s="295"/>
       <c r="AO6" s="19"/>
     </row>
     <row r="7" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -23370,11 +23492,11 @@
       <c r="C7" s="98" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="287" t="s">
+      <c r="D7" s="280" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="274"/>
-      <c r="F7" s="274"/>
+      <c r="E7" s="281"/>
+      <c r="F7" s="281"/>
       <c r="G7" s="79"/>
       <c r="H7" s="94" t="s">
         <v>98</v>
@@ -23382,9 +23504,9 @@
       <c r="I7" s="98" t="s">
         <v>100</v>
       </c>
-      <c r="J7" s="287"/>
-      <c r="K7" s="274"/>
-      <c r="L7" s="274"/>
+      <c r="J7" s="280"/>
+      <c r="K7" s="281"/>
+      <c r="L7" s="281"/>
       <c r="N7" s="80" t="s">
         <v>91</v>
       </c>
@@ -23398,7 +23520,7 @@
         <v>90</v>
       </c>
       <c r="S7" s="19"/>
-      <c r="T7" s="272"/>
+      <c r="T7" s="299"/>
       <c r="U7" s="122"/>
       <c r="V7" s="105" t="s">
         <v>93</v>
@@ -23408,12 +23530,12 @@
         <v>95</v>
       </c>
       <c r="Y7" s="124"/>
-      <c r="Z7" s="273"/>
+      <c r="Z7" s="300"/>
       <c r="AA7" s="140"/>
-      <c r="AB7" s="330" t="s">
+      <c r="AB7" s="258" t="s">
         <v>92</v>
       </c>
-      <c r="AC7" s="333" t="s">
+      <c r="AC7" s="261" t="s">
         <v>92</v>
       </c>
       <c r="AD7" s="168"/>
@@ -23425,11 +23547,11 @@
       <c r="AH7" s="165" t="s">
         <v>92</v>
       </c>
-      <c r="AI7" s="333"/>
-      <c r="AJ7" s="335"/>
-      <c r="AL7" s="275"/>
-      <c r="AM7" s="275"/>
-      <c r="AN7" s="275"/>
+      <c r="AI7" s="261"/>
+      <c r="AJ7" s="263"/>
+      <c r="AL7" s="295"/>
+      <c r="AM7" s="295"/>
+      <c r="AN7" s="295"/>
       <c r="AO7" s="19"/>
     </row>
     <row r="8" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -23439,9 +23561,9 @@
       <c r="C8" s="95" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="287"/>
-      <c r="E8" s="274"/>
-      <c r="F8" s="274"/>
+      <c r="D8" s="280"/>
+      <c r="E8" s="281"/>
+      <c r="F8" s="281"/>
       <c r="G8" s="41"/>
       <c r="H8" s="99" t="s">
         <v>104</v>
@@ -23449,11 +23571,11 @@
       <c r="I8" s="95" t="s">
         <v>106</v>
       </c>
-      <c r="J8" s="288" t="s">
+      <c r="J8" s="294" t="s">
         <v>107</v>
       </c>
-      <c r="K8" s="267"/>
-      <c r="L8" s="267"/>
+      <c r="K8" s="279"/>
+      <c r="L8" s="279"/>
       <c r="N8" s="105" t="s">
         <v>93</v>
       </c>
@@ -23467,7 +23589,7 @@
         <v>97</v>
       </c>
       <c r="S8" s="19"/>
-      <c r="T8" s="272"/>
+      <c r="T8" s="299"/>
       <c r="U8" s="122"/>
       <c r="V8" s="80" t="s">
         <v>102</v>
@@ -23477,7 +23599,7 @@
         <v>112</v>
       </c>
       <c r="Y8" s="124"/>
-      <c r="Z8" s="273"/>
+      <c r="Z8" s="300"/>
       <c r="AA8" s="140"/>
       <c r="AB8" s="172" t="s">
         <v>92</v>
@@ -23485,20 +23607,20 @@
       <c r="AC8" s="164" t="s">
         <v>92</v>
       </c>
-      <c r="AD8" s="333"/>
-      <c r="AE8" s="331"/>
+      <c r="AD8" s="261"/>
+      <c r="AE8" s="259"/>
       <c r="AF8" s="19"/>
-      <c r="AG8" s="336" t="s">
+      <c r="AG8" s="264" t="s">
         <v>92</v>
       </c>
-      <c r="AH8" s="333" t="s">
+      <c r="AH8" s="261" t="s">
         <v>92</v>
       </c>
       <c r="AI8" s="169"/>
       <c r="AJ8" s="175"/>
-      <c r="AL8" s="275"/>
-      <c r="AM8" s="275"/>
-      <c r="AN8" s="275"/>
+      <c r="AL8" s="295"/>
+      <c r="AM8" s="295"/>
+      <c r="AN8" s="295"/>
       <c r="AO8" s="19"/>
     </row>
     <row r="9" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -23508,9 +23630,9 @@
       <c r="C9" s="98" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="287"/>
-      <c r="E9" s="274"/>
-      <c r="F9" s="274"/>
+      <c r="D9" s="280"/>
+      <c r="E9" s="281"/>
+      <c r="F9" s="281"/>
       <c r="G9" s="79"/>
       <c r="H9" s="94" t="s">
         <v>110</v>
@@ -23531,7 +23653,7 @@
         <v>100</v>
       </c>
       <c r="S9" s="19"/>
-      <c r="T9" s="272"/>
+      <c r="T9" s="299"/>
       <c r="U9" s="122"/>
       <c r="V9" s="105" t="s">
         <v>104</v>
@@ -23541,7 +23663,7 @@
         <v>106</v>
       </c>
       <c r="Y9" s="124"/>
-      <c r="Z9" s="273"/>
+      <c r="Z9" s="300"/>
       <c r="AA9" s="140"/>
       <c r="AB9" s="173" t="s">
         <v>103</v>
@@ -23549,7 +23671,7 @@
       <c r="AC9" s="165" t="s">
         <v>77</v>
       </c>
-      <c r="AD9" s="337" t="s">
+      <c r="AD9" s="265" t="s">
         <v>76</v>
       </c>
       <c r="AE9" s="176" t="s">
@@ -23559,7 +23681,7 @@
       <c r="AG9" s="173" t="s">
         <v>103</v>
       </c>
-      <c r="AH9" s="337" t="s">
+      <c r="AH9" s="265" t="s">
         <v>77</v>
       </c>
       <c r="AI9" s="168" t="s">
@@ -23568,9 +23690,9 @@
       <c r="AJ9" s="176" t="s">
         <v>103</v>
       </c>
-      <c r="AL9" s="275"/>
-      <c r="AM9" s="275"/>
-      <c r="AN9" s="275"/>
+      <c r="AL9" s="295"/>
+      <c r="AM9" s="295"/>
+      <c r="AN9" s="295"/>
       <c r="AO9" s="166"/>
     </row>
     <row r="10" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -23580,9 +23702,9 @@
       <c r="C10" s="95" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="287"/>
-      <c r="E10" s="274"/>
-      <c r="F10" s="274"/>
+      <c r="D10" s="280"/>
+      <c r="E10" s="281"/>
+      <c r="F10" s="281"/>
       <c r="G10" s="79"/>
       <c r="H10" s="99" t="s">
         <v>114</v>
@@ -23590,11 +23712,11 @@
       <c r="I10" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="J10" s="287" t="s">
+      <c r="J10" s="280" t="s">
         <v>116</v>
       </c>
-      <c r="K10" s="274"/>
-      <c r="L10" s="274"/>
+      <c r="K10" s="281"/>
+      <c r="L10" s="281"/>
       <c r="N10" s="105" t="s">
         <v>104</v>
       </c>
@@ -23608,7 +23730,7 @@
         <v>109</v>
       </c>
       <c r="S10" s="19"/>
-      <c r="T10" s="272"/>
+      <c r="T10" s="299"/>
       <c r="U10" s="122"/>
       <c r="V10" s="80" t="s">
         <v>113</v>
@@ -23618,7 +23740,7 @@
         <v>120</v>
       </c>
       <c r="Y10" s="124"/>
-      <c r="Z10" s="273"/>
+      <c r="Z10" s="300"/>
       <c r="AA10" s="140"/>
       <c r="AB10" s="248"/>
       <c r="AC10" s="248"/>
@@ -23629,9 +23751,9 @@
       <c r="AH10" s="248"/>
       <c r="AI10" s="248"/>
       <c r="AJ10" s="248"/>
-      <c r="AL10" s="275"/>
-      <c r="AM10" s="275"/>
-      <c r="AN10" s="275"/>
+      <c r="AL10" s="295"/>
+      <c r="AM10" s="295"/>
+      <c r="AN10" s="295"/>
       <c r="AO10" s="19"/>
     </row>
     <row r="11" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -23641,9 +23763,9 @@
       <c r="C11" s="98" t="s">
         <v>118</v>
       </c>
-      <c r="D11" s="287"/>
-      <c r="E11" s="274"/>
-      <c r="F11" s="274"/>
+      <c r="D11" s="280"/>
+      <c r="E11" s="281"/>
+      <c r="F11" s="281"/>
       <c r="G11" s="79"/>
       <c r="H11" s="94" t="s">
         <v>119</v>
@@ -23651,9 +23773,9 @@
       <c r="I11" s="98" t="s">
         <v>115</v>
       </c>
-      <c r="J11" s="287"/>
-      <c r="K11" s="274"/>
-      <c r="L11" s="274"/>
+      <c r="J11" s="280"/>
+      <c r="K11" s="281"/>
+      <c r="L11" s="281"/>
       <c r="N11" s="80" t="s">
         <v>113</v>
       </c>
@@ -23667,7 +23789,7 @@
         <v>111</v>
       </c>
       <c r="S11" s="19"/>
-      <c r="T11" s="272"/>
+      <c r="T11" s="299"/>
       <c r="U11" s="122"/>
       <c r="V11" s="105" t="s">
         <v>114</v>
@@ -23677,12 +23799,12 @@
         <v>83</v>
       </c>
       <c r="Y11" s="124"/>
-      <c r="Z11" s="273"/>
+      <c r="Z11" s="300"/>
       <c r="AA11" s="140"/>
       <c r="AB11" s="172" t="s">
         <v>86</v>
       </c>
-      <c r="AC11" s="334" t="s">
+      <c r="AC11" s="262" t="s">
         <v>77</v>
       </c>
       <c r="AD11" s="162" t="s">
@@ -23698,15 +23820,15 @@
       <c r="AH11" s="167" t="s">
         <v>77</v>
       </c>
-      <c r="AI11" s="334" t="s">
+      <c r="AI11" s="262" t="s">
         <v>76</v>
       </c>
       <c r="AJ11" s="175" t="s">
         <v>86</v>
       </c>
-      <c r="AL11" s="275"/>
-      <c r="AM11" s="275"/>
-      <c r="AN11" s="275"/>
+      <c r="AL11" s="295"/>
+      <c r="AM11" s="295"/>
+      <c r="AN11" s="295"/>
       <c r="AO11" s="19"/>
     </row>
     <row r="12" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -23716,9 +23838,9 @@
       <c r="C12" s="95" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="287"/>
-      <c r="E12" s="274"/>
-      <c r="F12" s="274"/>
+      <c r="D12" s="280"/>
+      <c r="E12" s="281"/>
+      <c r="F12" s="281"/>
       <c r="G12" s="79"/>
       <c r="H12" s="99" t="s">
         <v>122</v>
@@ -23726,9 +23848,9 @@
       <c r="I12" s="95" t="s">
         <v>105</v>
       </c>
-      <c r="J12" s="287"/>
-      <c r="K12" s="274"/>
-      <c r="L12" s="274"/>
+      <c r="J12" s="280"/>
+      <c r="K12" s="281"/>
+      <c r="L12" s="281"/>
       <c r="N12" s="105" t="s">
         <v>114</v>
       </c>
@@ -23742,7 +23864,7 @@
         <v>118</v>
       </c>
       <c r="S12" s="19"/>
-      <c r="T12" s="272"/>
+      <c r="T12" s="299"/>
       <c r="U12" s="122"/>
       <c r="V12" s="80" t="s">
         <v>121</v>
@@ -23752,12 +23874,12 @@
         <v>94</v>
       </c>
       <c r="Y12" s="124"/>
-      <c r="Z12" s="273"/>
+      <c r="Z12" s="300"/>
       <c r="AA12" s="140"/>
-      <c r="AB12" s="336" t="s">
+      <c r="AB12" s="264" t="s">
         <v>92</v>
       </c>
-      <c r="AC12" s="332" t="s">
+      <c r="AC12" s="260" t="s">
         <v>92</v>
       </c>
       <c r="AD12" s="163"/>
@@ -23769,11 +23891,11 @@
       <c r="AH12" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="AI12" s="332"/>
-      <c r="AJ12" s="331"/>
-      <c r="AL12" s="275"/>
-      <c r="AM12" s="275"/>
-      <c r="AN12" s="275"/>
+      <c r="AI12" s="260"/>
+      <c r="AJ12" s="259"/>
+      <c r="AL12" s="295"/>
+      <c r="AM12" s="295"/>
+      <c r="AN12" s="295"/>
       <c r="AO12" s="19"/>
     </row>
     <row r="13" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -23783,9 +23905,9 @@
       <c r="C13" s="98" t="s">
         <v>100</v>
       </c>
-      <c r="D13" s="287"/>
-      <c r="E13" s="274"/>
-      <c r="F13" s="274"/>
+      <c r="D13" s="280"/>
+      <c r="E13" s="281"/>
+      <c r="F13" s="281"/>
       <c r="G13" s="79"/>
       <c r="H13" s="94" t="s">
         <v>125</v>
@@ -23793,9 +23915,9 @@
       <c r="I13" s="98" t="s">
         <v>88</v>
       </c>
-      <c r="J13" s="287"/>
-      <c r="K13" s="274"/>
-      <c r="L13" s="274"/>
+      <c r="J13" s="280"/>
+      <c r="K13" s="281"/>
+      <c r="L13" s="281"/>
       <c r="N13" s="80" t="s">
         <v>121</v>
       </c>
@@ -23809,7 +23931,7 @@
         <v>115</v>
       </c>
       <c r="S13" s="19"/>
-      <c r="T13" s="272"/>
+      <c r="T13" s="299"/>
       <c r="U13" s="122"/>
       <c r="V13" s="105" t="s">
         <v>122</v>
@@ -23819,7 +23941,7 @@
         <v>105</v>
       </c>
       <c r="Y13" s="124"/>
-      <c r="Z13" s="273"/>
+      <c r="Z13" s="300"/>
       <c r="AA13" s="140"/>
       <c r="AB13" s="177" t="s">
         <v>92</v>
@@ -23827,13 +23949,13 @@
       <c r="AC13" s="167" t="s">
         <v>92</v>
       </c>
-      <c r="AD13" s="332"/>
-      <c r="AE13" s="335"/>
+      <c r="AD13" s="260"/>
+      <c r="AE13" s="263"/>
       <c r="AF13" s="19"/>
-      <c r="AG13" s="330" t="s">
+      <c r="AG13" s="258" t="s">
         <v>92</v>
       </c>
-      <c r="AH13" s="332" t="s">
+      <c r="AH13" s="260" t="s">
         <v>92</v>
       </c>
       <c r="AI13" s="162"/>
@@ -23850,9 +23972,9 @@
       <c r="C14" s="95" t="s">
         <v>124</v>
       </c>
-      <c r="D14" s="287"/>
-      <c r="E14" s="274"/>
-      <c r="F14" s="274"/>
+      <c r="D14" s="280"/>
+      <c r="E14" s="281"/>
+      <c r="F14" s="281"/>
       <c r="G14" s="79"/>
       <c r="H14" s="99" t="s">
         <v>96</v>
@@ -23860,9 +23982,9 @@
       <c r="I14" s="95" t="s">
         <v>85</v>
       </c>
-      <c r="J14" s="287"/>
-      <c r="K14" s="274"/>
-      <c r="L14" s="274"/>
+      <c r="J14" s="280"/>
+      <c r="K14" s="281"/>
+      <c r="L14" s="281"/>
       <c r="N14" s="105" t="s">
         <v>122</v>
       </c>
@@ -23876,7 +23998,7 @@
         <v>124</v>
       </c>
       <c r="S14" s="19"/>
-      <c r="T14" s="272"/>
+      <c r="T14" s="299"/>
       <c r="U14" s="122"/>
       <c r="V14" s="84" t="s">
         <v>126</v>
@@ -23886,7 +24008,7 @@
         <v>128</v>
       </c>
       <c r="Y14" s="124"/>
-      <c r="Z14" s="273"/>
+      <c r="Z14" s="300"/>
       <c r="AA14" s="140"/>
       <c r="AB14" s="178" t="s">
         <v>103</v>
@@ -23894,7 +24016,7 @@
       <c r="AC14" s="170" t="s">
         <v>77</v>
       </c>
-      <c r="AD14" s="329" t="s">
+      <c r="AD14" s="257" t="s">
         <v>76</v>
       </c>
       <c r="AE14" s="174" t="s">
@@ -23904,7 +24026,7 @@
       <c r="AG14" s="178" t="s">
         <v>103</v>
       </c>
-      <c r="AH14" s="329" t="s">
+      <c r="AH14" s="257" t="s">
         <v>77</v>
       </c>
       <c r="AI14" s="163" t="s">
@@ -23913,11 +24035,11 @@
       <c r="AJ14" s="174" t="s">
         <v>103</v>
       </c>
-      <c r="AL14" s="274" t="s">
+      <c r="AL14" s="281" t="s">
         <v>158</v>
       </c>
-      <c r="AM14" s="274"/>
-      <c r="AN14" s="274"/>
+      <c r="AM14" s="281"/>
+      <c r="AN14" s="281"/>
     </row>
     <row r="15" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="94" t="s">
@@ -23926,9 +24048,9 @@
       <c r="C15" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="287"/>
-      <c r="E15" s="274"/>
-      <c r="F15" s="274"/>
+      <c r="D15" s="280"/>
+      <c r="E15" s="281"/>
+      <c r="F15" s="281"/>
       <c r="G15" s="79"/>
       <c r="H15" s="94" t="s">
         <v>91</v>
@@ -23936,9 +24058,9 @@
       <c r="I15" s="98" t="s">
         <v>101</v>
       </c>
-      <c r="J15" s="287"/>
-      <c r="K15" s="274"/>
-      <c r="L15" s="274"/>
+      <c r="J15" s="280"/>
+      <c r="K15" s="281"/>
+      <c r="L15" s="281"/>
       <c r="N15" s="84" t="s">
         <v>126</v>
       </c>
@@ -23952,16 +24074,16 @@
         <v>88</v>
       </c>
       <c r="S15" s="19"/>
-      <c r="T15" s="272"/>
+      <c r="T15" s="299"/>
       <c r="U15" s="125"/>
       <c r="V15" s="126"/>
       <c r="W15" s="127"/>
       <c r="X15" s="128"/>
       <c r="Y15" s="129"/>
-      <c r="Z15" s="273"/>
-      <c r="AL15" s="274"/>
-      <c r="AM15" s="274"/>
-      <c r="AN15" s="274"/>
+      <c r="Z15" s="300"/>
+      <c r="AL15" s="281"/>
+      <c r="AM15" s="281"/>
+      <c r="AN15" s="281"/>
       <c r="AO15" s="19"/>
     </row>
     <row r="16" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -23971,9 +24093,9 @@
       <c r="C16" s="95" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="287"/>
-      <c r="E16" s="274"/>
-      <c r="F16" s="274"/>
+      <c r="D16" s="280"/>
+      <c r="E16" s="281"/>
+      <c r="F16" s="281"/>
       <c r="G16" s="79"/>
       <c r="H16" s="99" t="s">
         <v>108</v>
@@ -23981,19 +24103,19 @@
       <c r="I16" s="95" t="s">
         <v>97</v>
       </c>
-      <c r="J16" s="287"/>
-      <c r="K16" s="274"/>
-      <c r="L16" s="274"/>
-      <c r="T16" s="272"/>
+      <c r="J16" s="280"/>
+      <c r="K16" s="281"/>
+      <c r="L16" s="281"/>
+      <c r="T16" s="299"/>
       <c r="U16" s="122"/>
       <c r="V16" s="130"/>
       <c r="W16" s="131"/>
       <c r="X16" s="132"/>
       <c r="Y16" s="124"/>
-      <c r="Z16" s="273"/>
-      <c r="AL16" s="274"/>
-      <c r="AM16" s="274"/>
-      <c r="AN16" s="274"/>
+      <c r="Z16" s="300"/>
+      <c r="AL16" s="281"/>
+      <c r="AM16" s="281"/>
+      <c r="AN16" s="281"/>
       <c r="AO16" s="19"/>
     </row>
     <row r="17" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -24003,9 +24125,9 @@
       <c r="C17" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="287"/>
-      <c r="E17" s="274"/>
-      <c r="F17" s="274"/>
+      <c r="D17" s="280"/>
+      <c r="E17" s="281"/>
+      <c r="F17" s="281"/>
       <c r="G17" s="79"/>
       <c r="H17" s="94" t="s">
         <v>102</v>
@@ -24013,11 +24135,11 @@
       <c r="I17" s="98" t="s">
         <v>112</v>
       </c>
-      <c r="J17" s="287"/>
-      <c r="K17" s="274"/>
-      <c r="L17" s="274"/>
+      <c r="J17" s="280"/>
+      <c r="K17" s="281"/>
+      <c r="L17" s="281"/>
       <c r="S17" s="142"/>
-      <c r="T17" s="272"/>
+      <c r="T17" s="299"/>
       <c r="U17" s="122"/>
       <c r="V17" s="87" t="s">
         <v>85</v>
@@ -24027,22 +24149,22 @@
         <v>96</v>
       </c>
       <c r="Y17" s="124"/>
-      <c r="Z17" s="273"/>
+      <c r="Z17" s="300"/>
       <c r="AA17" s="140"/>
-      <c r="AB17" s="267" t="s">
+      <c r="AB17" s="279" t="s">
         <v>190</v>
       </c>
-      <c r="AC17" s="267"/>
-      <c r="AD17" s="267"/>
-      <c r="AE17" s="267"/>
-      <c r="AF17" s="267"/>
-      <c r="AG17" s="267"/>
-      <c r="AH17" s="267"/>
-      <c r="AI17" s="267"/>
-      <c r="AJ17" s="267"/>
-      <c r="AL17" s="274"/>
-      <c r="AM17" s="274"/>
-      <c r="AN17" s="274"/>
+      <c r="AC17" s="279"/>
+      <c r="AD17" s="279"/>
+      <c r="AE17" s="279"/>
+      <c r="AF17" s="279"/>
+      <c r="AG17" s="279"/>
+      <c r="AH17" s="279"/>
+      <c r="AI17" s="279"/>
+      <c r="AJ17" s="279"/>
+      <c r="AL17" s="281"/>
+      <c r="AM17" s="281"/>
+      <c r="AN17" s="281"/>
       <c r="AO17" s="19"/>
     </row>
     <row r="18" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -24052,9 +24174,9 @@
       <c r="C18" s="95" t="s">
         <v>130</v>
       </c>
-      <c r="D18" s="287"/>
-      <c r="E18" s="274"/>
-      <c r="F18" s="274"/>
+      <c r="D18" s="280"/>
+      <c r="E18" s="281"/>
+      <c r="F18" s="281"/>
       <c r="G18" s="79"/>
       <c r="H18" s="99" t="s">
         <v>117</v>
@@ -24062,21 +24184,21 @@
       <c r="I18" s="95" t="s">
         <v>109</v>
       </c>
-      <c r="J18" s="287"/>
-      <c r="K18" s="274"/>
-      <c r="L18" s="274"/>
+      <c r="J18" s="280"/>
+      <c r="K18" s="281"/>
+      <c r="L18" s="281"/>
       <c r="M18" s="89"/>
-      <c r="N18" s="267" t="s">
+      <c r="N18" s="279" t="s">
         <v>149</v>
       </c>
-      <c r="O18" s="267"/>
+      <c r="O18" s="279"/>
       <c r="P18" s="89"/>
-      <c r="Q18" s="268" t="s">
+      <c r="Q18" s="284" t="s">
         <v>150</v>
       </c>
-      <c r="R18" s="268"/>
+      <c r="R18" s="284"/>
       <c r="S18" s="142"/>
-      <c r="T18" s="272"/>
+      <c r="T18" s="299"/>
       <c r="U18" s="122"/>
       <c r="V18" s="105" t="s">
         <v>90</v>
@@ -24086,7 +24208,7 @@
         <v>87</v>
       </c>
       <c r="Y18" s="124"/>
-      <c r="Z18" s="273"/>
+      <c r="Z18" s="300"/>
       <c r="AA18" s="140"/>
       <c r="AB18" s="177" t="s">
         <v>86</v>
@@ -24094,7 +24216,7 @@
       <c r="AC18" s="167" t="s">
         <v>77</v>
       </c>
-      <c r="AD18" s="334" t="s">
+      <c r="AD18" s="262" t="s">
         <v>76</v>
       </c>
       <c r="AE18" s="171" t="s">
@@ -24107,15 +24229,15 @@
       <c r="AH18" s="164" t="s">
         <v>77</v>
       </c>
-      <c r="AI18" s="328" t="s">
+      <c r="AI18" s="256" t="s">
         <v>76</v>
       </c>
       <c r="AJ18" s="171" t="s">
         <v>86</v>
       </c>
-      <c r="AL18" s="274"/>
-      <c r="AM18" s="274"/>
-      <c r="AN18" s="274"/>
+      <c r="AL18" s="281"/>
+      <c r="AM18" s="281"/>
+      <c r="AN18" s="281"/>
       <c r="AO18" s="19"/>
     </row>
     <row r="19" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -24125,9 +24247,9 @@
       <c r="C19" s="98" t="s">
         <v>111</v>
       </c>
-      <c r="D19" s="287"/>
-      <c r="E19" s="274"/>
-      <c r="F19" s="274"/>
+      <c r="D19" s="280"/>
+      <c r="E19" s="281"/>
+      <c r="F19" s="281"/>
       <c r="G19" s="79"/>
       <c r="H19" s="94" t="s">
         <v>113</v>
@@ -24135,9 +24257,9 @@
       <c r="I19" s="98" t="s">
         <v>120</v>
       </c>
-      <c r="J19" s="287"/>
-      <c r="K19" s="274"/>
-      <c r="L19" s="274"/>
+      <c r="J19" s="280"/>
+      <c r="K19" s="281"/>
+      <c r="L19" s="281"/>
       <c r="M19" s="32"/>
       <c r="N19" s="183" t="s">
         <v>76</v>
@@ -24153,7 +24275,7 @@
         <v>77</v>
       </c>
       <c r="S19" s="142"/>
-      <c r="T19" s="272"/>
+      <c r="T19" s="299"/>
       <c r="U19" s="122"/>
       <c r="V19" s="80" t="s">
         <v>97</v>
@@ -24163,23 +24285,23 @@
         <v>108</v>
       </c>
       <c r="Y19" s="124"/>
-      <c r="Z19" s="273"/>
+      <c r="Z19" s="300"/>
       <c r="AA19" s="140"/>
       <c r="AB19" s="178"/>
       <c r="AC19" s="170"/>
-      <c r="AD19" s="332" t="s">
+      <c r="AD19" s="260" t="s">
         <v>92</v>
       </c>
-      <c r="AE19" s="335" t="s">
+      <c r="AE19" s="263" t="s">
         <v>92</v>
       </c>
       <c r="AF19" s="19"/>
       <c r="AG19" s="178"/>
       <c r="AH19" s="165"/>
-      <c r="AI19" s="333" t="s">
+      <c r="AI19" s="261" t="s">
         <v>92</v>
       </c>
-      <c r="AJ19" s="335" t="s">
+      <c r="AJ19" s="263" t="s">
         <v>92</v>
       </c>
       <c r="AO19" s="166"/>
@@ -24191,9 +24313,9 @@
       <c r="C20" s="95" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="287"/>
-      <c r="E20" s="274"/>
-      <c r="F20" s="274"/>
+      <c r="D20" s="280"/>
+      <c r="E20" s="281"/>
+      <c r="F20" s="281"/>
       <c r="G20" s="79"/>
       <c r="H20" s="99" t="s">
         <v>123</v>
@@ -24201,9 +24323,9 @@
       <c r="I20" s="95" t="s">
         <v>118</v>
       </c>
-      <c r="J20" s="287"/>
-      <c r="K20" s="274"/>
-      <c r="L20" s="274"/>
+      <c r="J20" s="280"/>
+      <c r="K20" s="281"/>
+      <c r="L20" s="281"/>
       <c r="M20" s="32"/>
       <c r="N20" s="112" t="s">
         <v>82</v>
@@ -24219,7 +24341,7 @@
         <v>84</v>
       </c>
       <c r="S20" s="142"/>
-      <c r="T20" s="272"/>
+      <c r="T20" s="299"/>
       <c r="U20" s="122"/>
       <c r="V20" s="105" t="s">
         <v>100</v>
@@ -24229,10 +24351,10 @@
         <v>98</v>
       </c>
       <c r="Y20" s="124"/>
-      <c r="Z20" s="273"/>
+      <c r="Z20" s="300"/>
       <c r="AA20" s="140"/>
-      <c r="AB20" s="336"/>
-      <c r="AC20" s="332"/>
+      <c r="AB20" s="264"/>
+      <c r="AC20" s="260"/>
       <c r="AD20" s="162" t="s">
         <v>92</v>
       </c>
@@ -24240,19 +24362,19 @@
         <v>92</v>
       </c>
       <c r="AF20" s="19"/>
-      <c r="AG20" s="336"/>
-      <c r="AH20" s="333"/>
+      <c r="AG20" s="264"/>
+      <c r="AH20" s="261"/>
       <c r="AI20" s="169" t="s">
         <v>92</v>
       </c>
       <c r="AJ20" s="175" t="s">
         <v>92</v>
       </c>
-      <c r="AL20" s="274" t="s">
+      <c r="AL20" s="281" t="s">
         <v>131</v>
       </c>
-      <c r="AM20" s="274"/>
-      <c r="AN20" s="274"/>
+      <c r="AM20" s="281"/>
+      <c r="AN20" s="281"/>
       <c r="AO20" s="19"/>
     </row>
     <row r="21" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -24262,9 +24384,9 @@
       <c r="C21" s="98" t="s">
         <v>109</v>
       </c>
-      <c r="D21" s="287"/>
-      <c r="E21" s="274"/>
-      <c r="F21" s="274"/>
+      <c r="D21" s="280"/>
+      <c r="E21" s="281"/>
+      <c r="F21" s="281"/>
       <c r="G21" s="79"/>
       <c r="H21" s="94" t="s">
         <v>121</v>
@@ -24272,9 +24394,9 @@
       <c r="I21" s="98" t="s">
         <v>94</v>
       </c>
-      <c r="J21" s="287"/>
-      <c r="K21" s="274"/>
-      <c r="L21" s="274"/>
+      <c r="J21" s="280"/>
+      <c r="K21" s="281"/>
+      <c r="L21" s="281"/>
       <c r="N21" s="83" t="s">
         <v>91</v>
       </c>
@@ -24288,7 +24410,7 @@
         <v>101</v>
       </c>
       <c r="S21" s="142"/>
-      <c r="T21" s="272"/>
+      <c r="T21" s="299"/>
       <c r="U21" s="122"/>
       <c r="V21" s="80" t="s">
         <v>109</v>
@@ -24298,12 +24420,12 @@
         <v>117</v>
       </c>
       <c r="Y21" s="124"/>
-      <c r="Z21" s="273"/>
+      <c r="Z21" s="300"/>
       <c r="AA21" s="140"/>
       <c r="AB21" s="173" t="s">
         <v>103</v>
       </c>
-      <c r="AC21" s="329" t="s">
+      <c r="AC21" s="257" t="s">
         <v>77</v>
       </c>
       <c r="AD21" s="163" t="s">
@@ -24316,7 +24438,7 @@
       <c r="AG21" s="173" t="s">
         <v>103</v>
       </c>
-      <c r="AH21" s="337" t="s">
+      <c r="AH21" s="265" t="s">
         <v>77</v>
       </c>
       <c r="AI21" s="168" t="s">
@@ -24337,9 +24459,9 @@
       <c r="C22" s="95" t="s">
         <v>132</v>
       </c>
-      <c r="D22" s="287"/>
-      <c r="E22" s="274"/>
-      <c r="F22" s="274"/>
+      <c r="D22" s="280"/>
+      <c r="E22" s="281"/>
+      <c r="F22" s="281"/>
       <c r="G22" s="79"/>
       <c r="H22" s="99" t="s">
         <v>127</v>
@@ -24347,9 +24469,9 @@
       <c r="I22" s="95" t="s">
         <v>124</v>
       </c>
-      <c r="J22" s="287"/>
-      <c r="K22" s="274"/>
-      <c r="L22" s="274"/>
+      <c r="J22" s="280"/>
+      <c r="K22" s="281"/>
+      <c r="L22" s="281"/>
       <c r="N22" s="106" t="s">
         <v>93</v>
       </c>
@@ -24363,7 +24485,7 @@
         <v>95</v>
       </c>
       <c r="S22" s="143"/>
-      <c r="T22" s="272"/>
+      <c r="T22" s="299"/>
       <c r="U22" s="122"/>
       <c r="V22" s="105" t="s">
         <v>111</v>
@@ -24373,7 +24495,7 @@
         <v>110</v>
       </c>
       <c r="Y22" s="124"/>
-      <c r="Z22" s="273"/>
+      <c r="Z22" s="300"/>
       <c r="AA22" s="140"/>
       <c r="AB22" s="248"/>
       <c r="AC22" s="248"/>
@@ -24384,10 +24506,10 @@
       <c r="AH22" s="248"/>
       <c r="AI22" s="248"/>
       <c r="AJ22" s="248"/>
-      <c r="AL22" s="274" t="s">
+      <c r="AL22" s="281" t="s">
         <v>133</v>
       </c>
-      <c r="AM22" s="274"/>
+      <c r="AM22" s="281"/>
       <c r="AN22" s="88" t="s">
         <v>134</v>
       </c>
@@ -24400,9 +24522,9 @@
       <c r="C23" s="100" t="s">
         <v>112</v>
       </c>
-      <c r="D23" s="287"/>
-      <c r="E23" s="274"/>
-      <c r="F23" s="274"/>
+      <c r="D23" s="280"/>
+      <c r="E23" s="281"/>
+      <c r="F23" s="281"/>
       <c r="G23" s="79"/>
       <c r="H23" s="96" t="s">
         <v>126</v>
@@ -24410,9 +24532,9 @@
       <c r="I23" s="100" t="s">
         <v>128</v>
       </c>
-      <c r="J23" s="287"/>
-      <c r="K23" s="274"/>
-      <c r="L23" s="274"/>
+      <c r="J23" s="280"/>
+      <c r="K23" s="281"/>
+      <c r="L23" s="281"/>
       <c r="N23" s="83" t="s">
         <v>102</v>
       </c>
@@ -24425,7 +24547,7 @@
       <c r="R23" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="T23" s="272"/>
+      <c r="T23" s="299"/>
       <c r="U23" s="122"/>
       <c r="V23" s="80" t="s">
         <v>118</v>
@@ -24435,7 +24557,7 @@
         <v>123</v>
       </c>
       <c r="Y23" s="124"/>
-      <c r="Z23" s="273"/>
+      <c r="Z23" s="300"/>
       <c r="AA23" s="140"/>
       <c r="AB23" s="172" t="s">
         <v>86</v>
@@ -24443,7 +24565,7 @@
       <c r="AC23" s="164" t="s">
         <v>77</v>
       </c>
-      <c r="AD23" s="328" t="s">
+      <c r="AD23" s="256" t="s">
         <v>76</v>
       </c>
       <c r="AE23" s="175" t="s">
@@ -24456,16 +24578,16 @@
       <c r="AH23" s="167" t="s">
         <v>77</v>
       </c>
-      <c r="AI23" s="334" t="s">
+      <c r="AI23" s="262" t="s">
         <v>76</v>
       </c>
       <c r="AJ23" s="175" t="s">
         <v>86</v>
       </c>
-      <c r="AL23" s="274" t="s">
+      <c r="AL23" s="281" t="s">
         <v>135</v>
       </c>
-      <c r="AM23" s="274"/>
+      <c r="AM23" s="281"/>
       <c r="AN23" s="88" t="s">
         <v>134</v>
       </c>
@@ -24488,7 +24610,7 @@
         <v>106</v>
       </c>
       <c r="S24" s="19"/>
-      <c r="T24" s="272"/>
+      <c r="T24" s="299"/>
       <c r="U24" s="122"/>
       <c r="V24" s="105" t="s">
         <v>115</v>
@@ -24498,29 +24620,29 @@
         <v>119</v>
       </c>
       <c r="Y24" s="124"/>
-      <c r="Z24" s="273"/>
+      <c r="Z24" s="300"/>
       <c r="AA24" s="140"/>
       <c r="AB24" s="173"/>
       <c r="AC24" s="165"/>
-      <c r="AD24" s="333" t="s">
+      <c r="AD24" s="261" t="s">
         <v>92</v>
       </c>
-      <c r="AE24" s="331" t="s">
+      <c r="AE24" s="259" t="s">
         <v>92</v>
       </c>
       <c r="AF24" s="19"/>
       <c r="AG24" s="173"/>
       <c r="AH24" s="170"/>
-      <c r="AI24" s="332" t="s">
+      <c r="AI24" s="260" t="s">
         <v>92</v>
       </c>
-      <c r="AJ24" s="331" t="s">
+      <c r="AJ24" s="259" t="s">
         <v>92</v>
       </c>
-      <c r="AL24" s="274" t="s">
+      <c r="AL24" s="281" t="s">
         <v>139</v>
       </c>
-      <c r="AM24" s="274"/>
+      <c r="AM24" s="281"/>
       <c r="AN24" s="88" t="s">
         <v>134</v>
       </c>
@@ -24531,13 +24653,13 @@
       <c r="D25" s="32"/>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
-      <c r="H25" s="275" t="s">
+      <c r="H25" s="295" t="s">
         <v>159</v>
       </c>
-      <c r="I25" s="275"/>
-      <c r="J25" s="275"/>
-      <c r="K25" s="275"/>
-      <c r="L25" s="275"/>
+      <c r="I25" s="295"/>
+      <c r="J25" s="295"/>
+      <c r="K25" s="295"/>
+      <c r="L25" s="295"/>
       <c r="N25" s="83" t="s">
         <v>113</v>
       </c>
@@ -24551,7 +24673,7 @@
         <v>120</v>
       </c>
       <c r="S25" s="19"/>
-      <c r="T25" s="272"/>
+      <c r="T25" s="299"/>
       <c r="U25" s="122"/>
       <c r="V25" s="80" t="s">
         <v>124</v>
@@ -24561,10 +24683,10 @@
         <v>127</v>
       </c>
       <c r="Y25" s="124"/>
-      <c r="Z25" s="273"/>
+      <c r="Z25" s="300"/>
       <c r="AA25" s="140"/>
-      <c r="AB25" s="330"/>
-      <c r="AC25" s="333"/>
+      <c r="AB25" s="258"/>
+      <c r="AC25" s="261"/>
       <c r="AD25" s="169" t="s">
         <v>92</v>
       </c>
@@ -24572,8 +24694,8 @@
         <v>92</v>
       </c>
       <c r="AF25" s="19"/>
-      <c r="AG25" s="330"/>
-      <c r="AH25" s="332"/>
+      <c r="AG25" s="258"/>
+      <c r="AH25" s="260"/>
       <c r="AI25" s="162" t="s">
         <v>92</v>
       </c>
@@ -24588,19 +24710,19 @@
       <c r="B26" s="90" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="278" t="s">
+      <c r="C26" s="285" t="s">
         <v>137</v>
       </c>
-      <c r="D26" s="279"/>
-      <c r="E26" s="278" t="s">
+      <c r="D26" s="286"/>
+      <c r="E26" s="285" t="s">
         <v>138</v>
       </c>
-      <c r="F26" s="280"/>
-      <c r="H26" s="275"/>
-      <c r="I26" s="275"/>
-      <c r="J26" s="275"/>
-      <c r="K26" s="275"/>
-      <c r="L26" s="275"/>
+      <c r="F26" s="287"/>
+      <c r="H26" s="295"/>
+      <c r="I26" s="295"/>
+      <c r="J26" s="295"/>
+      <c r="K26" s="295"/>
+      <c r="L26" s="295"/>
       <c r="N26" s="106" t="s">
         <v>114</v>
       </c>
@@ -24614,7 +24736,7 @@
         <v>83</v>
       </c>
       <c r="S26" s="19"/>
-      <c r="T26" s="272"/>
+      <c r="T26" s="299"/>
       <c r="U26" s="135"/>
       <c r="V26" s="111" t="s">
         <v>88</v>
@@ -24624,12 +24746,12 @@
         <v>125</v>
       </c>
       <c r="Y26" s="129"/>
-      <c r="Z26" s="273"/>
+      <c r="Z26" s="300"/>
       <c r="AA26" s="140"/>
       <c r="AB26" s="178" t="s">
         <v>103</v>
       </c>
-      <c r="AC26" s="337" t="s">
+      <c r="AC26" s="265" t="s">
         <v>77</v>
       </c>
       <c r="AD26" s="168" t="s">
@@ -24642,7 +24764,7 @@
       <c r="AG26" s="178" t="s">
         <v>103</v>
       </c>
-      <c r="AH26" s="329" t="s">
+      <c r="AH26" s="257" t="s">
         <v>77</v>
       </c>
       <c r="AI26" s="163" t="s">
@@ -24659,19 +24781,19 @@
       <c r="B27" s="91" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="281">
+      <c r="C27" s="288">
         <v>0.8</v>
       </c>
-      <c r="D27" s="282"/>
-      <c r="E27" s="281">
+      <c r="D27" s="289"/>
+      <c r="E27" s="288">
         <v>100</v>
       </c>
-      <c r="F27" s="283"/>
-      <c r="H27" s="275"/>
-      <c r="I27" s="275"/>
-      <c r="J27" s="275"/>
-      <c r="K27" s="275"/>
-      <c r="L27" s="275"/>
+      <c r="F27" s="290"/>
+      <c r="H27" s="295"/>
+      <c r="I27" s="295"/>
+      <c r="J27" s="295"/>
+      <c r="K27" s="295"/>
+      <c r="L27" s="295"/>
       <c r="N27" s="83" t="s">
         <v>121</v>
       </c>
@@ -24700,19 +24822,19 @@
       <c r="B28" s="92" t="s">
         <v>141</v>
       </c>
-      <c r="C28" s="284">
+      <c r="C28" s="291">
         <v>1</v>
       </c>
-      <c r="D28" s="285"/>
-      <c r="E28" s="284">
+      <c r="D28" s="292"/>
+      <c r="E28" s="291">
         <v>180</v>
       </c>
-      <c r="F28" s="286"/>
-      <c r="H28" s="275"/>
-      <c r="I28" s="275"/>
-      <c r="J28" s="275"/>
-      <c r="K28" s="275"/>
-      <c r="L28" s="275"/>
+      <c r="F28" s="293"/>
+      <c r="H28" s="295"/>
+      <c r="I28" s="295"/>
+      <c r="J28" s="295"/>
+      <c r="K28" s="295"/>
+      <c r="L28" s="295"/>
       <c r="N28" s="106" t="s">
         <v>122</v>
       </c>
@@ -24726,25 +24848,25 @@
         <v>105</v>
       </c>
       <c r="U28" s="101"/>
-      <c r="V28" s="270" t="s">
+      <c r="V28" s="297" t="s">
         <v>81</v>
       </c>
-      <c r="W28" s="270"/>
-      <c r="X28" s="270"/>
+      <c r="W28" s="297"/>
+      <c r="X28" s="297"/>
     </row>
     <row r="29" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="277" t="s">
+      <c r="B29" s="283" t="s">
         <v>142</v>
       </c>
-      <c r="C29" s="277"/>
-      <c r="D29" s="277"/>
-      <c r="E29" s="277"/>
-      <c r="F29" s="277"/>
-      <c r="H29" s="275"/>
-      <c r="I29" s="275"/>
-      <c r="J29" s="275"/>
-      <c r="K29" s="275"/>
-      <c r="L29" s="275"/>
+      <c r="C29" s="283"/>
+      <c r="D29" s="283"/>
+      <c r="E29" s="283"/>
+      <c r="F29" s="283"/>
+      <c r="H29" s="295"/>
+      <c r="I29" s="295"/>
+      <c r="J29" s="295"/>
+      <c r="K29" s="295"/>
+      <c r="L29" s="295"/>
       <c r="N29" s="85" t="s">
         <v>126</v>
       </c>
@@ -24800,13 +24922,18 @@
     <row r="41" spans="19:19" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="AB17:AJ17"/>
-    <mergeCell ref="AB5:AJ5"/>
-    <mergeCell ref="D3:F4"/>
-    <mergeCell ref="J3:L7"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="AL3:AN3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="V28:X28"/>
+    <mergeCell ref="T5:T26"/>
+    <mergeCell ref="Z5:Z26"/>
+    <mergeCell ref="AL24:AM24"/>
+    <mergeCell ref="AL14:AN18"/>
+    <mergeCell ref="AL20:AN20"/>
+    <mergeCell ref="AL22:AM22"/>
+    <mergeCell ref="AL23:AM23"/>
+    <mergeCell ref="AL4:AN12"/>
+    <mergeCell ref="AB3:AJ3"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="N18:O18"/>
     <mergeCell ref="Q18:R18"/>
@@ -24820,18 +24947,13 @@
     <mergeCell ref="J8:L8"/>
     <mergeCell ref="J10:L23"/>
     <mergeCell ref="H25:L29"/>
-    <mergeCell ref="AL3:AN3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="V28:X28"/>
-    <mergeCell ref="T5:T26"/>
-    <mergeCell ref="Z5:Z26"/>
-    <mergeCell ref="AL24:AM24"/>
-    <mergeCell ref="AL14:AN18"/>
-    <mergeCell ref="AL20:AN20"/>
-    <mergeCell ref="AL22:AM22"/>
-    <mergeCell ref="AL23:AM23"/>
-    <mergeCell ref="AL4:AN12"/>
-    <mergeCell ref="AB3:AJ3"/>
+    <mergeCell ref="AB17:AJ17"/>
+    <mergeCell ref="AB5:AJ5"/>
+    <mergeCell ref="D3:F4"/>
+    <mergeCell ref="J3:L7"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="D5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -24843,10 +24965,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AC30"/>
+  <dimension ref="A2:AC43"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="50" workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11:AB13"/>
+    <sheetView zoomScale="84" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -24862,27 +24984,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:29" ht="16" x14ac:dyDescent="0.35">
-      <c r="B2" s="303" t="s">
+      <c r="B2" s="307" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="303"/>
-      <c r="D2" s="303"/>
-      <c r="E2" s="303"/>
-      <c r="F2" s="303"/>
-      <c r="N2" s="326" t="s">
+      <c r="C2" s="307"/>
+      <c r="D2" s="307"/>
+      <c r="E2" s="307"/>
+      <c r="F2" s="307"/>
+      <c r="N2" s="308" t="s">
         <v>182</v>
       </c>
-      <c r="O2" s="326"/>
-      <c r="P2" s="326"/>
-      <c r="Q2" s="326"/>
-      <c r="R2" s="326"/>
-      <c r="T2" s="326" t="s">
+      <c r="O2" s="308"/>
+      <c r="P2" s="308"/>
+      <c r="Q2" s="308"/>
+      <c r="R2" s="308"/>
+      <c r="T2" s="308" t="s">
         <v>181</v>
       </c>
-      <c r="U2" s="326"/>
-      <c r="V2" s="326"/>
-      <c r="W2" s="326"/>
-      <c r="X2" s="326"/>
+      <c r="U2" s="308"/>
+      <c r="V2" s="308"/>
+      <c r="W2" s="308"/>
+      <c r="X2" s="308"/>
     </row>
     <row r="3" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H3" s="38" t="s">
@@ -24891,34 +25013,34 @@
       <c r="I3" s="1">
         <v>20</v>
       </c>
-      <c r="N3" s="296" t="s">
+      <c r="N3" s="310" t="s">
         <v>185</v>
       </c>
-      <c r="O3" s="296"/>
-      <c r="P3" s="296"/>
-      <c r="Q3" s="296"/>
-      <c r="R3" s="296"/>
-      <c r="T3" s="296" t="s">
+      <c r="O3" s="310"/>
+      <c r="P3" s="310"/>
+      <c r="Q3" s="310"/>
+      <c r="R3" s="310"/>
+      <c r="T3" s="310" t="s">
         <v>186</v>
       </c>
-      <c r="U3" s="296"/>
-      <c r="V3" s="296"/>
-      <c r="W3" s="296"/>
-      <c r="X3" s="296"/>
-      <c r="Z3" s="274" t="s">
+      <c r="U3" s="310"/>
+      <c r="V3" s="310"/>
+      <c r="W3" s="310"/>
+      <c r="X3" s="310"/>
+      <c r="Z3" s="281" t="s">
         <v>34</v>
       </c>
-      <c r="AA3" s="274"/>
-      <c r="AB3" s="274"/>
+      <c r="AA3" s="281"/>
+      <c r="AB3" s="281"/>
     </row>
     <row r="4" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="40"/>
-      <c r="C4" s="304" t="s">
+      <c r="C4" s="309" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="294"/>
-      <c r="E4" s="294"/>
-      <c r="F4" s="294"/>
+      <c r="D4" s="302"/>
+      <c r="E4" s="302"/>
+      <c r="F4" s="302"/>
       <c r="H4" s="1" t="s">
         <v>4</v>
       </c>
@@ -24935,9 +25057,9 @@
       <c r="V4" s="31"/>
       <c r="W4" s="31"/>
       <c r="X4" s="37"/>
-      <c r="Z4" s="274"/>
-      <c r="AA4" s="274"/>
-      <c r="AB4" s="274"/>
+      <c r="Z4" s="281"/>
+      <c r="AA4" s="281"/>
+      <c r="AB4" s="281"/>
     </row>
     <row r="5" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H5" s="1" t="s">
@@ -24956,46 +25078,46 @@
       <c r="V5" s="249"/>
       <c r="W5" s="249"/>
       <c r="X5" s="249"/>
-      <c r="Z5" s="274"/>
-      <c r="AA5" s="274"/>
-      <c r="AB5" s="274"/>
+      <c r="Z5" s="281"/>
+      <c r="AA5" s="281"/>
+      <c r="AB5" s="281"/>
       <c r="AC5" s="32"/>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="294" t="s">
+      <c r="C6" s="302" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="294"/>
-      <c r="E6" s="294"/>
-      <c r="F6" s="294"/>
+      <c r="D6" s="302"/>
+      <c r="E6" s="302"/>
+      <c r="F6" s="302"/>
       <c r="H6" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I6" s="1">
         <v>20</v>
       </c>
-      <c r="N6" s="297" t="s">
+      <c r="N6" s="303" t="s">
         <v>36</v>
       </c>
-      <c r="O6" s="298"/>
+      <c r="O6" s="304"/>
       <c r="P6" s="249"/>
-      <c r="Q6" s="297" t="s">
+      <c r="Q6" s="303" t="s">
         <v>36</v>
       </c>
-      <c r="R6" s="298"/>
+      <c r="R6" s="304"/>
       <c r="S6" s="249"/>
-      <c r="T6" s="297" t="s">
+      <c r="T6" s="303" t="s">
         <v>37</v>
       </c>
-      <c r="U6" s="298"/>
+      <c r="U6" s="304"/>
       <c r="V6" s="249"/>
-      <c r="W6" s="297" t="s">
+      <c r="W6" s="303" t="s">
         <v>37</v>
       </c>
-      <c r="X6" s="298"/>
+      <c r="X6" s="304"/>
       <c r="Z6" s="32"/>
       <c r="AA6" s="32"/>
       <c r="AB6" s="32"/>
@@ -25014,22 +25136,22 @@
       <c r="V7" s="249"/>
       <c r="W7" s="249"/>
       <c r="X7" s="249"/>
-      <c r="Z7" s="274" t="s">
+      <c r="Z7" s="281" t="s">
         <v>44</v>
       </c>
-      <c r="AA7" s="274"/>
-      <c r="AB7" s="274"/>
+      <c r="AA7" s="281"/>
+      <c r="AB7" s="281"/>
     </row>
     <row r="8" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="294" t="s">
+      <c r="C8" s="302" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="294"/>
-      <c r="E8" s="294"/>
-      <c r="F8" s="294"/>
+      <c r="D8" s="302"/>
+      <c r="E8" s="302"/>
+      <c r="F8" s="302"/>
       <c r="N8" s="44" t="s">
         <v>43</v>
       </c>
@@ -25057,9 +25179,9 @@
       <c r="X8" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="Z8" s="274"/>
-      <c r="AA8" s="274"/>
-      <c r="AB8" s="274"/>
+      <c r="Z8" s="281"/>
+      <c r="AA8" s="281"/>
+      <c r="AB8" s="281"/>
     </row>
     <row r="9" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="N9" s="249"/>
@@ -25073,20 +25195,20 @@
       <c r="V9" s="249"/>
       <c r="W9" s="249"/>
       <c r="X9" s="249"/>
-      <c r="Z9" s="274"/>
-      <c r="AA9" s="274"/>
-      <c r="AB9" s="274"/>
+      <c r="Z9" s="281"/>
+      <c r="AA9" s="281"/>
+      <c r="AB9" s="281"/>
     </row>
     <row r="10" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="294" t="s">
+      <c r="C10" s="302" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="294"/>
-      <c r="E10" s="294"/>
-      <c r="F10" s="294"/>
+      <c r="D10" s="302"/>
+      <c r="E10" s="302"/>
+      <c r="F10" s="302"/>
       <c r="N10" s="48" t="s">
         <v>46</v>
       </c>
@@ -25119,39 +25241,39 @@
       <c r="AB10" s="52"/>
     </row>
     <row r="11" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N11" s="289" t="s">
+      <c r="N11" s="282" t="s">
         <v>62</v>
       </c>
-      <c r="O11" s="289"/>
+      <c r="O11" s="282"/>
       <c r="P11" s="249"/>
-      <c r="Q11" s="289" t="s">
+      <c r="Q11" s="282" t="s">
         <v>62</v>
       </c>
-      <c r="R11" s="289"/>
+      <c r="R11" s="282"/>
       <c r="S11" s="249"/>
-      <c r="T11" s="294" t="s">
+      <c r="T11" s="302" t="s">
         <v>50</v>
       </c>
-      <c r="U11" s="294"/>
+      <c r="U11" s="302"/>
       <c r="V11" s="249"/>
-      <c r="W11" s="294" t="s">
+      <c r="W11" s="302" t="s">
         <v>50</v>
       </c>
-      <c r="X11" s="294"/>
-      <c r="Z11" s="274" t="s">
+      <c r="X11" s="302"/>
+      <c r="Z11" s="281" t="s">
         <v>51</v>
       </c>
-      <c r="AA11" s="274"/>
-      <c r="AB11" s="274"/>
+      <c r="AA11" s="281"/>
+      <c r="AB11" s="281"/>
     </row>
     <row r="12" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="299" t="s">
+      <c r="B12" s="311" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="299"/>
-      <c r="D12" s="299"/>
-      <c r="E12" s="299"/>
-      <c r="F12" s="299"/>
+      <c r="C12" s="311"/>
+      <c r="D12" s="311"/>
+      <c r="E12" s="311"/>
+      <c r="F12" s="311"/>
       <c r="N12" s="54" t="s">
         <v>47</v>
       </c>
@@ -25179,49 +25301,49 @@
       <c r="X12" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="Z12" s="274"/>
-      <c r="AA12" s="274"/>
-      <c r="AB12" s="274"/>
+      <c r="Z12" s="281"/>
+      <c r="AA12" s="281"/>
+      <c r="AB12" s="281"/>
     </row>
     <row r="13" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N13" s="289" t="s">
+      <c r="N13" s="282" t="s">
         <v>65</v>
       </c>
-      <c r="O13" s="289"/>
+      <c r="O13" s="282"/>
       <c r="P13" s="249"/>
-      <c r="Q13" s="289" t="s">
+      <c r="Q13" s="282" t="s">
         <v>65</v>
       </c>
-      <c r="R13" s="289"/>
+      <c r="R13" s="282"/>
       <c r="S13" s="249"/>
-      <c r="T13" s="289" t="s">
+      <c r="T13" s="282" t="s">
         <v>54</v>
       </c>
-      <c r="U13" s="289"/>
+      <c r="U13" s="282"/>
       <c r="V13" s="249"/>
-      <c r="W13" s="289" t="s">
+      <c r="W13" s="282" t="s">
         <v>54</v>
       </c>
-      <c r="X13" s="289"/>
-      <c r="Z13" s="274"/>
-      <c r="AA13" s="274"/>
-      <c r="AB13" s="274"/>
+      <c r="X13" s="282"/>
+      <c r="Z13" s="281"/>
+      <c r="AA13" s="281"/>
+      <c r="AB13" s="281"/>
     </row>
     <row r="14" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="300" t="s">
+      <c r="B14" s="312" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="300"/>
-      <c r="D14" s="300"/>
-      <c r="E14" s="300"/>
-      <c r="F14" s="300"/>
-      <c r="H14" s="301" t="s">
+      <c r="C14" s="312"/>
+      <c r="D14" s="312"/>
+      <c r="E14" s="312"/>
+      <c r="F14" s="312"/>
+      <c r="H14" s="313" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="301"/>
-      <c r="J14" s="301"/>
-      <c r="K14" s="301"/>
-      <c r="L14" s="301"/>
+      <c r="I14" s="313"/>
+      <c r="J14" s="313"/>
+      <c r="K14" s="313"/>
+      <c r="L14" s="313"/>
       <c r="N14" s="58" t="s">
         <v>184</v>
       </c>
@@ -25251,33 +25373,33 @@
       </c>
     </row>
     <row r="15" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N15" s="294" t="s">
+      <c r="N15" s="302" t="s">
         <v>69</v>
       </c>
-      <c r="O15" s="294"/>
+      <c r="O15" s="302"/>
       <c r="P15" s="249"/>
-      <c r="Q15" s="294" t="s">
+      <c r="Q15" s="302" t="s">
         <v>69</v>
       </c>
-      <c r="R15" s="294"/>
+      <c r="R15" s="302"/>
       <c r="S15" s="249"/>
-      <c r="T15" s="289" t="s">
+      <c r="T15" s="282" t="s">
         <v>55</v>
       </c>
-      <c r="U15" s="289"/>
+      <c r="U15" s="282"/>
       <c r="V15" s="249"/>
-      <c r="W15" s="289" t="s">
+      <c r="W15" s="282" t="s">
         <v>55</v>
       </c>
-      <c r="X15" s="289"/>
-      <c r="Z15" s="274" t="s">
+      <c r="X15" s="282"/>
+      <c r="Z15" s="281" t="s">
         <v>57</v>
       </c>
-      <c r="AA15" s="274"/>
-      <c r="AB15" s="274"/>
+      <c r="AA15" s="281"/>
+      <c r="AB15" s="281"/>
     </row>
     <row r="16" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="290">
+      <c r="A16" s="314">
         <v>1</v>
       </c>
       <c r="B16" s="59" t="s">
@@ -25286,7 +25408,7 @@
       <c r="C16" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="291">
+      <c r="D16" s="315">
         <v>3</v>
       </c>
       <c r="E16" s="59" t="s">
@@ -25295,7 +25417,7 @@
       <c r="F16" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="290">
+      <c r="G16" s="314">
         <v>1</v>
       </c>
       <c r="H16" s="61" t="s">
@@ -25304,7 +25426,7 @@
       <c r="I16" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="291">
+      <c r="J16" s="315">
         <v>3</v>
       </c>
       <c r="K16" s="61" t="s">
@@ -25324,61 +25446,61 @@
       <c r="V16" s="249"/>
       <c r="W16" s="249"/>
       <c r="X16" s="249"/>
-      <c r="Z16" s="274"/>
-      <c r="AA16" s="274"/>
-      <c r="AB16" s="274"/>
+      <c r="Z16" s="281"/>
+      <c r="AA16" s="281"/>
+      <c r="AB16" s="281"/>
     </row>
     <row r="17" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="290"/>
+      <c r="A17" s="314"/>
       <c r="B17" s="63" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="291"/>
+      <c r="D17" s="315"/>
       <c r="E17" s="63" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="290"/>
+      <c r="G17" s="314"/>
       <c r="H17" s="65" t="s">
         <v>16</v>
       </c>
       <c r="I17" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="291"/>
+      <c r="J17" s="315"/>
       <c r="K17" s="65" t="s">
         <v>15</v>
       </c>
       <c r="L17" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="N17" s="297" t="s">
+      <c r="N17" s="303" t="s">
         <v>58</v>
       </c>
-      <c r="O17" s="298"/>
+      <c r="O17" s="304"/>
       <c r="P17" s="41"/>
-      <c r="Q17" s="297" t="s">
+      <c r="Q17" s="303" t="s">
         <v>58</v>
       </c>
-      <c r="R17" s="298"/>
+      <c r="R17" s="304"/>
       <c r="S17" s="249"/>
-      <c r="T17" s="297" t="s">
+      <c r="T17" s="303" t="s">
         <v>59</v>
       </c>
-      <c r="U17" s="298"/>
+      <c r="U17" s="304"/>
       <c r="V17" s="41"/>
-      <c r="W17" s="297" t="s">
+      <c r="W17" s="303" t="s">
         <v>59</v>
       </c>
-      <c r="X17" s="298"/>
-      <c r="Z17" s="274"/>
-      <c r="AA17" s="274"/>
-      <c r="AB17" s="274"/>
+      <c r="X17" s="304"/>
+      <c r="Z17" s="281"/>
+      <c r="AA17" s="281"/>
+      <c r="AB17" s="281"/>
     </row>
     <row r="18" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="N18" s="249"/>
@@ -25394,7 +25516,7 @@
       <c r="X18" s="249"/>
     </row>
     <row r="19" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="290">
+      <c r="A19" s="314">
         <v>2</v>
       </c>
       <c r="B19" s="59" t="s">
@@ -25403,7 +25525,7 @@
       <c r="C19" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="291">
+      <c r="D19" s="315">
         <v>4</v>
       </c>
       <c r="E19" s="59" t="s">
@@ -25412,7 +25534,7 @@
       <c r="F19" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="290">
+      <c r="G19" s="314">
         <v>2</v>
       </c>
       <c r="H19" s="61" t="s">
@@ -25421,7 +25543,7 @@
       <c r="I19" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="J19" s="291">
+      <c r="J19" s="315">
         <v>4</v>
       </c>
       <c r="K19" s="61" t="s">
@@ -25457,35 +25579,35 @@
       <c r="X19" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="Z19" s="274" t="s">
+      <c r="Z19" s="281" t="s">
         <v>61</v>
       </c>
-      <c r="AA19" s="274"/>
-      <c r="AB19" s="274"/>
+      <c r="AA19" s="281"/>
+      <c r="AB19" s="281"/>
     </row>
     <row r="20" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="290"/>
+      <c r="A20" s="314"/>
       <c r="B20" s="63" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="291"/>
+      <c r="D20" s="315"/>
       <c r="E20" s="63" t="s">
         <v>15</v>
       </c>
       <c r="F20" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="290"/>
+      <c r="G20" s="314"/>
       <c r="H20" s="65" t="s">
         <v>16</v>
       </c>
       <c r="I20" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="291"/>
+      <c r="J20" s="315"/>
       <c r="K20" s="65" t="s">
         <v>15</v>
       </c>
@@ -25503,9 +25625,9 @@
       <c r="V20" s="249"/>
       <c r="W20" s="249"/>
       <c r="X20" s="249"/>
-      <c r="Z20" s="274"/>
-      <c r="AA20" s="274"/>
-      <c r="AB20" s="274"/>
+      <c r="Z20" s="281"/>
+      <c r="AA20" s="281"/>
+      <c r="AB20" s="281"/>
     </row>
     <row r="21" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="N21" s="49" t="s">
@@ -25535,46 +25657,46 @@
       <c r="X21" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="Z21" s="274"/>
-      <c r="AA21" s="274"/>
-      <c r="AB21" s="274"/>
+      <c r="Z21" s="281"/>
+      <c r="AA21" s="281"/>
+      <c r="AB21" s="281"/>
     </row>
     <row r="22" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N22" s="302" t="s">
+      <c r="N22" s="301" t="s">
         <v>49</v>
       </c>
-      <c r="O22" s="302"/>
+      <c r="O22" s="301"/>
       <c r="P22" s="249"/>
-      <c r="Q22" s="302" t="s">
+      <c r="Q22" s="301" t="s">
         <v>49</v>
       </c>
-      <c r="R22" s="302"/>
+      <c r="R22" s="301"/>
       <c r="S22" s="249"/>
-      <c r="T22" s="302" t="s">
+      <c r="T22" s="301" t="s">
         <v>63</v>
       </c>
-      <c r="U22" s="302"/>
+      <c r="U22" s="301"/>
       <c r="V22" s="249"/>
-      <c r="W22" s="302" t="s">
+      <c r="W22" s="301" t="s">
         <v>63</v>
       </c>
-      <c r="X22" s="302"/>
+      <c r="X22" s="301"/>
     </row>
     <row r="23" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="295" t="s">
+      <c r="B23" s="317" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="295"/>
-      <c r="D23" s="295"/>
-      <c r="E23" s="295"/>
-      <c r="F23" s="295"/>
-      <c r="H23" s="274" t="s">
+      <c r="C23" s="317"/>
+      <c r="D23" s="317"/>
+      <c r="E23" s="317"/>
+      <c r="F23" s="317"/>
+      <c r="H23" s="281" t="s">
         <v>64</v>
       </c>
-      <c r="I23" s="274"/>
-      <c r="J23" s="274"/>
-      <c r="K23" s="274"/>
-      <c r="L23" s="274"/>
+      <c r="I23" s="281"/>
+      <c r="J23" s="281"/>
+      <c r="K23" s="281"/>
+      <c r="L23" s="281"/>
       <c r="N23" s="53" t="s">
         <v>48</v>
       </c>
@@ -25602,43 +25724,43 @@
       <c r="X23" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="Z23" s="274" t="s">
+      <c r="Z23" s="281" t="s">
         <v>67</v>
       </c>
-      <c r="AA23" s="274"/>
-      <c r="AB23" s="274"/>
+      <c r="AA23" s="281"/>
+      <c r="AB23" s="281"/>
     </row>
     <row r="24" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H24" s="274"/>
-      <c r="I24" s="274"/>
-      <c r="J24" s="274"/>
-      <c r="K24" s="274"/>
-      <c r="L24" s="274"/>
-      <c r="N24" s="294" t="s">
+      <c r="H24" s="281"/>
+      <c r="I24" s="281"/>
+      <c r="J24" s="281"/>
+      <c r="K24" s="281"/>
+      <c r="L24" s="281"/>
+      <c r="N24" s="302" t="s">
         <v>53</v>
       </c>
-      <c r="O24" s="294"/>
+      <c r="O24" s="302"/>
       <c r="P24" s="249"/>
-      <c r="Q24" s="294" t="s">
+      <c r="Q24" s="302" t="s">
         <v>53</v>
       </c>
-      <c r="R24" s="294"/>
+      <c r="R24" s="302"/>
       <c r="S24" s="249"/>
-      <c r="T24" s="294" t="s">
+      <c r="T24" s="302" t="s">
         <v>66</v>
       </c>
-      <c r="U24" s="294"/>
+      <c r="U24" s="302"/>
       <c r="V24" s="249"/>
-      <c r="W24" s="294" t="s">
+      <c r="W24" s="302" t="s">
         <v>66</v>
       </c>
-      <c r="X24" s="294"/>
-      <c r="Z24" s="274"/>
-      <c r="AA24" s="274"/>
-      <c r="AB24" s="274"/>
+      <c r="X24" s="302"/>
+      <c r="Z24" s="281"/>
+      <c r="AA24" s="281"/>
+      <c r="AB24" s="281"/>
     </row>
     <row r="25" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="290">
+      <c r="A25" s="314">
         <v>1</v>
       </c>
       <c r="B25" s="67" t="s">
@@ -25647,7 +25769,7 @@
       <c r="C25" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="291">
+      <c r="D25" s="315">
         <v>3</v>
       </c>
       <c r="E25" s="67" t="s">
@@ -25656,11 +25778,11 @@
       <c r="F25" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="274"/>
-      <c r="I25" s="274"/>
-      <c r="J25" s="274"/>
-      <c r="K25" s="274"/>
-      <c r="L25" s="274"/>
+      <c r="H25" s="281"/>
+      <c r="I25" s="281"/>
+      <c r="J25" s="281"/>
+      <c r="K25" s="281"/>
+      <c r="L25" s="281"/>
       <c r="N25" s="56" t="s">
         <v>47</v>
       </c>
@@ -25688,56 +25810,56 @@
       <c r="X25" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="Z25" s="274"/>
-      <c r="AA25" s="274"/>
-      <c r="AB25" s="274"/>
+      <c r="Z25" s="281"/>
+      <c r="AA25" s="281"/>
+      <c r="AB25" s="281"/>
     </row>
     <row r="26" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="290"/>
+      <c r="A26" s="314"/>
       <c r="B26" s="69" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="291"/>
+      <c r="D26" s="315"/>
       <c r="E26" s="69" t="s">
         <v>15</v>
       </c>
       <c r="F26" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="274"/>
-      <c r="I26" s="274"/>
-      <c r="J26" s="274"/>
-      <c r="K26" s="274"/>
-      <c r="L26" s="274"/>
-      <c r="N26" s="294" t="s">
+      <c r="H26" s="281"/>
+      <c r="I26" s="281"/>
+      <c r="J26" s="281"/>
+      <c r="K26" s="281"/>
+      <c r="L26" s="281"/>
+      <c r="N26" s="302" t="s">
         <v>56</v>
       </c>
-      <c r="O26" s="294"/>
+      <c r="O26" s="302"/>
       <c r="P26" s="249"/>
-      <c r="Q26" s="294" t="s">
+      <c r="Q26" s="302" t="s">
         <v>56</v>
       </c>
-      <c r="R26" s="294"/>
+      <c r="R26" s="302"/>
       <c r="S26" s="249"/>
-      <c r="T26" s="294" t="s">
+      <c r="T26" s="302" t="s">
         <v>68</v>
       </c>
-      <c r="U26" s="294"/>
+      <c r="U26" s="302"/>
       <c r="V26" s="249"/>
-      <c r="W26" s="294" t="s">
+      <c r="W26" s="302" t="s">
         <v>68</v>
       </c>
-      <c r="X26" s="294"/>
+      <c r="X26" s="302"/>
     </row>
     <row r="27" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H27" s="274"/>
-      <c r="I27" s="274"/>
-      <c r="J27" s="274"/>
-      <c r="K27" s="274"/>
-      <c r="L27" s="274"/>
+      <c r="H27" s="281"/>
+      <c r="I27" s="281"/>
+      <c r="J27" s="281"/>
+      <c r="K27" s="281"/>
+      <c r="L27" s="281"/>
       <c r="N27" s="71"/>
       <c r="O27" s="250"/>
       <c r="P27" s="250"/>
@@ -25750,7 +25872,7 @@
       <c r="X27" s="36"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A28" s="290">
+      <c r="A28" s="314">
         <v>2</v>
       </c>
       <c r="B28" s="67" t="s">
@@ -25759,7 +25881,7 @@
       <c r="C28" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="291">
+      <c r="D28" s="315">
         <v>4</v>
       </c>
       <c r="E28" s="67" t="s">
@@ -25768,49 +25890,49 @@
       <c r="F28" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="274"/>
-      <c r="I28" s="274"/>
-      <c r="J28" s="274"/>
-      <c r="K28" s="274"/>
-      <c r="L28" s="274"/>
-      <c r="N28" s="327" t="s">
+      <c r="H28" s="281"/>
+      <c r="I28" s="281"/>
+      <c r="J28" s="281"/>
+      <c r="K28" s="281"/>
+      <c r="L28" s="281"/>
+      <c r="N28" s="305" t="s">
         <v>188</v>
       </c>
-      <c r="O28" s="327"/>
-      <c r="P28" s="327"/>
-      <c r="Q28" s="327"/>
-      <c r="R28" s="327"/>
+      <c r="O28" s="305"/>
+      <c r="P28" s="305"/>
+      <c r="Q28" s="305"/>
+      <c r="R28" s="305"/>
       <c r="S28" s="72"/>
-      <c r="T28" s="293" t="s">
+      <c r="T28" s="306" t="s">
         <v>187</v>
       </c>
-      <c r="U28" s="293"/>
-      <c r="V28" s="293"/>
-      <c r="W28" s="293"/>
-      <c r="X28" s="293"/>
+      <c r="U28" s="306"/>
+      <c r="V28" s="306"/>
+      <c r="W28" s="306"/>
+      <c r="X28" s="306"/>
     </row>
     <row r="29" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="290"/>
+      <c r="A29" s="314"/>
       <c r="B29" s="69" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="291"/>
+      <c r="D29" s="315"/>
       <c r="E29" s="69" t="s">
         <v>15</v>
       </c>
       <c r="F29" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="292" t="s">
+      <c r="H29" s="316" t="s">
         <v>70</v>
       </c>
-      <c r="I29" s="292"/>
-      <c r="J29" s="292"/>
-      <c r="K29" s="292"/>
-      <c r="L29" s="292"/>
+      <c r="I29" s="316"/>
+      <c r="J29" s="316"/>
+      <c r="K29" s="316"/>
+      <c r="L29" s="316"/>
       <c r="N29" s="73"/>
       <c r="O29" s="73"/>
       <c r="P29" s="72"/>
@@ -25831,22 +25953,246 @@
       <c r="U30" s="74"/>
       <c r="V30" s="74"/>
     </row>
+    <row r="31" spans="1:28" s="255" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N31" s="73"/>
+      <c r="O31" s="73"/>
+      <c r="P31" s="72"/>
+      <c r="R31" s="73"/>
+      <c r="T31" s="74"/>
+      <c r="U31" s="74"/>
+      <c r="V31" s="74"/>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B32" s="351"/>
+      <c r="C32" s="349" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="349" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="350" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="352"/>
+      <c r="H32" s="349" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" s="350" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B33" s="353" t="s">
+        <v>192</v>
+      </c>
+      <c r="C33" s="254" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="254" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="341" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="353" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="254" t="s">
+        <v>199</v>
+      </c>
+      <c r="I33" s="341" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B34" s="344"/>
+      <c r="C34" s="254" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="254" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="341" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="346"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="347"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B35" s="346"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="347"/>
+      <c r="G35" s="348" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="254" t="s">
+        <v>198</v>
+      </c>
+      <c r="I35" s="341" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B36" s="348" t="s">
+        <v>193</v>
+      </c>
+      <c r="C36" s="254" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="254" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="341" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="346"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="347"/>
+    </row>
+    <row r="37" spans="2:9" ht="14" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="344"/>
+      <c r="C37" s="254" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="254" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="341" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="354" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="342" t="s">
+        <v>198</v>
+      </c>
+      <c r="I37" s="343" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B38" s="346"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="347"/>
+    </row>
+    <row r="39" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="348" t="s">
+        <v>194</v>
+      </c>
+      <c r="C39" s="254" t="s">
+        <v>196</v>
+      </c>
+      <c r="D39" s="254" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="341" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="281" t="s">
+        <v>200</v>
+      </c>
+      <c r="H39" s="281"/>
+      <c r="I39" s="281"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B40" s="344"/>
+      <c r="C40" s="254" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="254" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="341" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="281"/>
+      <c r="H40" s="281"/>
+      <c r="I40" s="281"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B41" s="346"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="347"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B42" s="348" t="s">
+        <v>195</v>
+      </c>
+      <c r="C42" s="254" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="254" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="341" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
+    </row>
+    <row r="43" spans="2:9" ht="14" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="345"/>
+      <c r="C43" s="342" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="342" t="s">
+        <v>197</v>
+      </c>
+      <c r="E43" s="343" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+    </row>
   </sheetData>
-  <mergeCells count="67">
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="T26:U26"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="Q17:R17"/>
+  <mergeCells count="68">
+    <mergeCell ref="G39:I40"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="Z23:AB25"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="H23:L28"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="Z19:AB21"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="Z15:AB17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="W17:X17"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="Z7:AB9"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="Z11:AB13"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="Z3:AB5"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="T3:X3"/>
     <mergeCell ref="N28:R28"/>
     <mergeCell ref="T28:X28"/>
     <mergeCell ref="N6:O6"/>
@@ -25863,43 +26209,20 @@
     <mergeCell ref="T13:U13"/>
     <mergeCell ref="T15:U15"/>
     <mergeCell ref="W11:X11"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="T2:X2"/>
-    <mergeCell ref="Z3:AB5"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="T3:X3"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="Z7:AB9"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="Z11:AB13"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="H14:L14"/>
-    <mergeCell ref="W13:X13"/>
-    <mergeCell ref="Z15:AB17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="W15:X15"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="W17:X17"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="Z19:AB21"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="Z23:AB25"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="H23:L28"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="W26:X26"/>
   </mergeCells>
   <pageMargins left="2.56" right="2.15" top="0.75" bottom="0.75" header="0.61" footer="0.3"/>
   <pageSetup scale="32" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -25928,10 +26251,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B2" s="306" t="s">
+      <c r="B2" s="320" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="306"/>
+      <c r="C2" s="320"/>
       <c r="D2" s="75"/>
       <c r="E2" s="75"/>
       <c r="F2" s="75"/>
@@ -25945,28 +26268,28 @@
       <c r="N2" s="75"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B3" s="267" t="s">
+      <c r="B3" s="279" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="267"/>
-      <c r="D3" s="267"/>
-      <c r="E3" s="267"/>
-      <c r="F3" s="267"/>
-      <c r="G3" s="267"/>
-      <c r="H3" s="267"/>
-      <c r="I3" s="267"/>
-      <c r="J3" s="267"/>
-      <c r="K3" s="267"/>
-      <c r="L3" s="267"/>
-      <c r="M3" s="267"/>
+      <c r="C3" s="279"/>
+      <c r="D3" s="279"/>
+      <c r="E3" s="279"/>
+      <c r="F3" s="279"/>
+      <c r="G3" s="279"/>
+      <c r="H3" s="279"/>
+      <c r="I3" s="279"/>
+      <c r="J3" s="279"/>
+      <c r="K3" s="279"/>
+      <c r="L3" s="279"/>
+      <c r="M3" s="279"/>
       <c r="N3" s="75"/>
-      <c r="O3" s="276" t="s">
+      <c r="O3" s="318" t="s">
         <v>153</v>
       </c>
-      <c r="P3" s="276"/>
-      <c r="Q3" s="276"/>
-      <c r="R3" s="276"/>
-      <c r="S3" s="267"/>
+      <c r="P3" s="318"/>
+      <c r="Q3" s="318"/>
+      <c r="R3" s="318"/>
+      <c r="S3" s="279"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" s="77">
@@ -26006,164 +26329,164 @@
         <v>12</v>
       </c>
       <c r="N4" s="145"/>
-      <c r="O4" s="276"/>
-      <c r="P4" s="276"/>
-      <c r="Q4" s="276"/>
-      <c r="R4" s="276"/>
-      <c r="S4" s="267"/>
+      <c r="O4" s="318"/>
+      <c r="P4" s="318"/>
+      <c r="Q4" s="318"/>
+      <c r="R4" s="318"/>
+      <c r="S4" s="279"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B5" s="307" t="s">
+      <c r="B5" s="321" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="270"/>
-      <c r="D5" s="307" t="s">
+      <c r="C5" s="297"/>
+      <c r="D5" s="321" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="270"/>
-      <c r="F5" s="307" t="s">
+      <c r="E5" s="297"/>
+      <c r="F5" s="321" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="270"/>
-      <c r="H5" s="307" t="s">
+      <c r="G5" s="297"/>
+      <c r="H5" s="321" t="s">
         <v>74</v>
       </c>
-      <c r="I5" s="270"/>
-      <c r="J5" s="307" t="s">
+      <c r="I5" s="297"/>
+      <c r="J5" s="321" t="s">
         <v>73</v>
       </c>
-      <c r="K5" s="308"/>
-      <c r="L5" s="307" t="s">
+      <c r="K5" s="322"/>
+      <c r="L5" s="321" t="s">
         <v>74</v>
       </c>
-      <c r="M5" s="308"/>
+      <c r="M5" s="322"/>
       <c r="N5" s="161"/>
-      <c r="S5" s="267"/>
+      <c r="S5" s="279"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6" s="78"/>
-      <c r="O6" s="274" t="s">
+      <c r="O6" s="281" t="s">
         <v>155</v>
       </c>
-      <c r="P6" s="274"/>
-      <c r="Q6" s="274"/>
-      <c r="R6" s="274"/>
-      <c r="S6" s="267"/>
+      <c r="P6" s="281"/>
+      <c r="Q6" s="281"/>
+      <c r="R6" s="281"/>
+      <c r="S6" s="279"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B7" s="276" t="s">
+      <c r="B7" s="318" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="276"/>
-      <c r="D7" s="276"/>
-      <c r="E7" s="276"/>
-      <c r="F7" s="276"/>
-      <c r="G7" s="276"/>
-      <c r="H7" s="276"/>
-      <c r="I7" s="276"/>
-      <c r="J7" s="276"/>
-      <c r="K7" s="276"/>
-      <c r="L7" s="276"/>
-      <c r="M7" s="276"/>
+      <c r="C7" s="318"/>
+      <c r="D7" s="318"/>
+      <c r="E7" s="318"/>
+      <c r="F7" s="318"/>
+      <c r="G7" s="318"/>
+      <c r="H7" s="318"/>
+      <c r="I7" s="318"/>
+      <c r="J7" s="318"/>
+      <c r="K7" s="318"/>
+      <c r="L7" s="318"/>
+      <c r="M7" s="318"/>
       <c r="N7" s="160"/>
-      <c r="O7" s="274"/>
-      <c r="P7" s="274"/>
-      <c r="Q7" s="274"/>
-      <c r="R7" s="274"/>
-      <c r="S7" s="267"/>
+      <c r="O7" s="281"/>
+      <c r="P7" s="281"/>
+      <c r="Q7" s="281"/>
+      <c r="R7" s="281"/>
+      <c r="S7" s="279"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B8" s="276"/>
-      <c r="C8" s="276"/>
-      <c r="D8" s="276"/>
-      <c r="E8" s="276"/>
-      <c r="F8" s="276"/>
-      <c r="G8" s="276"/>
-      <c r="H8" s="276"/>
-      <c r="I8" s="276"/>
-      <c r="J8" s="276"/>
-      <c r="K8" s="276"/>
-      <c r="L8" s="276"/>
-      <c r="M8" s="276"/>
+      <c r="B8" s="318"/>
+      <c r="C8" s="318"/>
+      <c r="D8" s="318"/>
+      <c r="E8" s="318"/>
+      <c r="F8" s="318"/>
+      <c r="G8" s="318"/>
+      <c r="H8" s="318"/>
+      <c r="I8" s="318"/>
+      <c r="J8" s="318"/>
+      <c r="K8" s="318"/>
+      <c r="L8" s="318"/>
+      <c r="M8" s="318"/>
       <c r="N8" s="160"/>
-      <c r="O8" s="274"/>
-      <c r="P8" s="274"/>
-      <c r="Q8" s="274"/>
-      <c r="R8" s="274"/>
-      <c r="S8" s="267"/>
+      <c r="O8" s="281"/>
+      <c r="P8" s="281"/>
+      <c r="Q8" s="281"/>
+      <c r="R8" s="281"/>
+      <c r="S8" s="279"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B9" s="276"/>
-      <c r="C9" s="276"/>
-      <c r="D9" s="276"/>
-      <c r="E9" s="276"/>
-      <c r="F9" s="276"/>
-      <c r="G9" s="276"/>
-      <c r="H9" s="276"/>
-      <c r="I9" s="276"/>
-      <c r="J9" s="276"/>
-      <c r="K9" s="276"/>
-      <c r="L9" s="276"/>
-      <c r="M9" s="276"/>
+      <c r="B9" s="318"/>
+      <c r="C9" s="318"/>
+      <c r="D9" s="318"/>
+      <c r="E9" s="318"/>
+      <c r="F9" s="318"/>
+      <c r="G9" s="318"/>
+      <c r="H9" s="318"/>
+      <c r="I9" s="318"/>
+      <c r="J9" s="318"/>
+      <c r="K9" s="318"/>
+      <c r="L9" s="318"/>
+      <c r="M9" s="318"/>
       <c r="N9" s="160"/>
-      <c r="O9" s="274"/>
-      <c r="P9" s="274"/>
-      <c r="Q9" s="274"/>
-      <c r="R9" s="274"/>
-      <c r="S9" s="267"/>
+      <c r="O9" s="281"/>
+      <c r="P9" s="281"/>
+      <c r="Q9" s="281"/>
+      <c r="R9" s="281"/>
+      <c r="S9" s="279"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B10" s="276"/>
-      <c r="C10" s="276"/>
-      <c r="D10" s="276"/>
-      <c r="E10" s="276"/>
-      <c r="F10" s="276"/>
-      <c r="G10" s="276"/>
-      <c r="H10" s="276"/>
-      <c r="I10" s="276"/>
-      <c r="J10" s="276"/>
-      <c r="K10" s="276"/>
-      <c r="L10" s="276"/>
-      <c r="M10" s="276"/>
+      <c r="B10" s="318"/>
+      <c r="C10" s="318"/>
+      <c r="D10" s="318"/>
+      <c r="E10" s="318"/>
+      <c r="F10" s="318"/>
+      <c r="G10" s="318"/>
+      <c r="H10" s="318"/>
+      <c r="I10" s="318"/>
+      <c r="J10" s="318"/>
+      <c r="K10" s="318"/>
+      <c r="L10" s="318"/>
+      <c r="M10" s="318"/>
       <c r="N10" s="160"/>
-      <c r="O10" s="274"/>
-      <c r="P10" s="274"/>
-      <c r="Q10" s="274"/>
-      <c r="R10" s="274"/>
-      <c r="S10" s="267"/>
+      <c r="O10" s="281"/>
+      <c r="P10" s="281"/>
+      <c r="Q10" s="281"/>
+      <c r="R10" s="281"/>
+      <c r="S10" s="279"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B11" s="276"/>
-      <c r="C11" s="276"/>
-      <c r="D11" s="276"/>
-      <c r="E11" s="276"/>
-      <c r="F11" s="276"/>
-      <c r="G11" s="276"/>
-      <c r="H11" s="276"/>
-      <c r="I11" s="276"/>
-      <c r="J11" s="276"/>
-      <c r="K11" s="276"/>
-      <c r="L11" s="276"/>
-      <c r="M11" s="276"/>
+      <c r="B11" s="318"/>
+      <c r="C11" s="318"/>
+      <c r="D11" s="318"/>
+      <c r="E11" s="318"/>
+      <c r="F11" s="318"/>
+      <c r="G11" s="318"/>
+      <c r="H11" s="318"/>
+      <c r="I11" s="318"/>
+      <c r="J11" s="318"/>
+      <c r="K11" s="318"/>
+      <c r="L11" s="318"/>
+      <c r="M11" s="318"/>
       <c r="N11" s="160"/>
-      <c r="O11" s="274"/>
-      <c r="P11" s="274"/>
-      <c r="Q11" s="274"/>
-      <c r="R11" s="274"/>
-      <c r="S11" s="267"/>
+      <c r="O11" s="281"/>
+      <c r="P11" s="281"/>
+      <c r="Q11" s="281"/>
+      <c r="R11" s="281"/>
+      <c r="S11" s="279"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="O12" s="274"/>
-      <c r="P12" s="274"/>
-      <c r="Q12" s="274"/>
-      <c r="R12" s="274"/>
-      <c r="S12" s="267"/>
+      <c r="O12" s="281"/>
+      <c r="P12" s="281"/>
+      <c r="Q12" s="281"/>
+      <c r="R12" s="281"/>
+      <c r="S12" s="279"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B13" s="305" t="s">
+      <c r="B13" s="319" t="s">
         <v>161</v>
       </c>
-      <c r="C13" s="305"/>
+      <c r="C13" s="319"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B14" s="75">
@@ -26180,12 +26503,12 @@
       <c r="C15" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="O15" s="274" t="s">
+      <c r="O15" s="281" t="s">
         <v>154</v>
       </c>
-      <c r="P15" s="274"/>
-      <c r="Q15" s="274"/>
-      <c r="R15" s="274"/>
+      <c r="P15" s="281"/>
+      <c r="Q15" s="281"/>
+      <c r="R15" s="281"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B16" s="75">
@@ -26194,10 +26517,10 @@
       <c r="C16" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="O16" s="274"/>
-      <c r="P16" s="274"/>
-      <c r="Q16" s="274"/>
-      <c r="R16" s="274"/>
+      <c r="O16" s="281"/>
+      <c r="P16" s="281"/>
+      <c r="Q16" s="281"/>
+      <c r="R16" s="281"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B17" s="75">
@@ -26214,12 +26537,12 @@
       <c r="C18" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="O18" s="274" t="s">
+      <c r="O18" s="281" t="s">
         <v>156</v>
       </c>
-      <c r="P18" s="274"/>
-      <c r="Q18" s="274"/>
-      <c r="R18" s="274"/>
+      <c r="P18" s="281"/>
+      <c r="Q18" s="281"/>
+      <c r="R18" s="281"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B19" s="75">
@@ -26228,97 +26551,97 @@
       <c r="C19" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="O19" s="274"/>
-      <c r="P19" s="274"/>
-      <c r="Q19" s="274"/>
-      <c r="R19" s="274"/>
+      <c r="O19" s="281"/>
+      <c r="P19" s="281"/>
+      <c r="Q19" s="281"/>
+      <c r="R19" s="281"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O20" s="274"/>
-      <c r="P20" s="274"/>
-      <c r="Q20" s="274"/>
-      <c r="R20" s="274"/>
+      <c r="O20" s="281"/>
+      <c r="P20" s="281"/>
+      <c r="Q20" s="281"/>
+      <c r="R20" s="281"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O21" s="274"/>
-      <c r="P21" s="274"/>
-      <c r="Q21" s="274"/>
-      <c r="R21" s="274"/>
+      <c r="O21" s="281"/>
+      <c r="P21" s="281"/>
+      <c r="Q21" s="281"/>
+      <c r="R21" s="281"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O22" s="274"/>
-      <c r="P22" s="274"/>
-      <c r="Q22" s="274"/>
-      <c r="R22" s="274"/>
+      <c r="O22" s="281"/>
+      <c r="P22" s="281"/>
+      <c r="Q22" s="281"/>
+      <c r="R22" s="281"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O23" s="274"/>
-      <c r="P23" s="274"/>
-      <c r="Q23" s="274"/>
-      <c r="R23" s="274"/>
+      <c r="O23" s="281"/>
+      <c r="P23" s="281"/>
+      <c r="Q23" s="281"/>
+      <c r="R23" s="281"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O27" s="276" t="s">
+      <c r="O27" s="318" t="s">
         <v>152</v>
       </c>
-      <c r="P27" s="276"/>
-      <c r="Q27" s="276"/>
-      <c r="R27" s="276"/>
+      <c r="P27" s="318"/>
+      <c r="Q27" s="318"/>
+      <c r="R27" s="318"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O28" s="276"/>
-      <c r="P28" s="276"/>
-      <c r="Q28" s="276"/>
-      <c r="R28" s="276"/>
+      <c r="O28" s="318"/>
+      <c r="P28" s="318"/>
+      <c r="Q28" s="318"/>
+      <c r="R28" s="318"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O30" s="274" t="s">
+      <c r="O30" s="281" t="s">
         <v>151</v>
       </c>
-      <c r="P30" s="274"/>
-      <c r="Q30" s="274"/>
-      <c r="R30" s="274"/>
+      <c r="P30" s="281"/>
+      <c r="Q30" s="281"/>
+      <c r="R30" s="281"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O31" s="274"/>
-      <c r="P31" s="274"/>
-      <c r="Q31" s="274"/>
-      <c r="R31" s="274"/>
+      <c r="O31" s="281"/>
+      <c r="P31" s="281"/>
+      <c r="Q31" s="281"/>
+      <c r="R31" s="281"/>
     </row>
     <row r="32" spans="2:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M32" s="89"/>
       <c r="N32" s="89"/>
-      <c r="O32" s="274"/>
-      <c r="P32" s="274"/>
-      <c r="Q32" s="274"/>
-      <c r="R32" s="274"/>
+      <c r="O32" s="281"/>
+      <c r="P32" s="281"/>
+      <c r="Q32" s="281"/>
+      <c r="R32" s="281"/>
     </row>
     <row r="33" spans="12:18" x14ac:dyDescent="0.35">
       <c r="L33" s="89"/>
       <c r="M33" s="89"/>
       <c r="N33" s="89"/>
-      <c r="O33" s="274"/>
-      <c r="P33" s="274"/>
-      <c r="Q33" s="274"/>
-      <c r="R33" s="274"/>
+      <c r="O33" s="281"/>
+      <c r="P33" s="281"/>
+      <c r="Q33" s="281"/>
+      <c r="R33" s="281"/>
     </row>
     <row r="34" spans="12:18" x14ac:dyDescent="0.35">
       <c r="L34" s="89"/>
       <c r="M34" s="89"/>
       <c r="N34" s="89"/>
-      <c r="O34" s="274"/>
-      <c r="P34" s="274"/>
-      <c r="Q34" s="274"/>
-      <c r="R34" s="274"/>
+      <c r="O34" s="281"/>
+      <c r="P34" s="281"/>
+      <c r="Q34" s="281"/>
+      <c r="R34" s="281"/>
     </row>
     <row r="35" spans="12:18" x14ac:dyDescent="0.35">
       <c r="L35" s="89"/>
       <c r="M35" s="89"/>
       <c r="N35" s="89"/>
-      <c r="O35" s="274"/>
-      <c r="P35" s="274"/>
-      <c r="Q35" s="274"/>
-      <c r="R35" s="274"/>
+      <c r="O35" s="281"/>
+      <c r="P35" s="281"/>
+      <c r="Q35" s="281"/>
+      <c r="R35" s="281"/>
     </row>
     <row r="36" spans="12:18" x14ac:dyDescent="0.35">
       <c r="L36" s="89"/>
@@ -26346,6 +26669,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="O30:R35"/>
+    <mergeCell ref="O15:R16"/>
+    <mergeCell ref="O3:R4"/>
+    <mergeCell ref="O18:R23"/>
+    <mergeCell ref="O6:R12"/>
     <mergeCell ref="B7:M11"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="S3:S12"/>
@@ -26358,11 +26686,6 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
-    <mergeCell ref="O30:R35"/>
-    <mergeCell ref="O15:R16"/>
-    <mergeCell ref="O3:R4"/>
-    <mergeCell ref="O18:R23"/>
-    <mergeCell ref="O6:R12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="55" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -26375,10 +26698,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:R19"/>
+  <dimension ref="B3:R23"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="81" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -26390,57 +26713,57 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="311" t="s">
+      <c r="B3" s="329" t="s">
         <v>162</v>
       </c>
-      <c r="C3" s="315"/>
-      <c r="D3" s="315"/>
-      <c r="E3" s="315"/>
-      <c r="F3" s="311" t="s">
+      <c r="C3" s="333"/>
+      <c r="D3" s="333"/>
+      <c r="E3" s="333"/>
+      <c r="F3" s="329" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="311"/>
-      <c r="H3" s="311"/>
-      <c r="I3" s="311"/>
-      <c r="J3" s="311"/>
-      <c r="K3" s="311"/>
-      <c r="L3" s="311"/>
-      <c r="M3" s="311"/>
-      <c r="N3" s="311"/>
-      <c r="O3" s="311"/>
-      <c r="P3" s="311"/>
-      <c r="Q3" s="311"/>
+      <c r="G3" s="329"/>
+      <c r="H3" s="329"/>
+      <c r="I3" s="329"/>
+      <c r="J3" s="329"/>
+      <c r="K3" s="329"/>
+      <c r="L3" s="329"/>
+      <c r="M3" s="329"/>
+      <c r="N3" s="329"/>
+      <c r="O3" s="329"/>
+      <c r="P3" s="329"/>
+      <c r="Q3" s="329"/>
     </row>
     <row r="4" spans="2:18" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="319" t="s">
+      <c r="B4" s="337" t="s">
         <v>170</v>
       </c>
-      <c r="C4" s="319"/>
-      <c r="D4" s="319"/>
-      <c r="E4" s="319"/>
-      <c r="F4" s="320" t="s">
+      <c r="C4" s="337"/>
+      <c r="D4" s="337"/>
+      <c r="E4" s="337"/>
+      <c r="F4" s="338" t="s">
         <v>171</v>
       </c>
-      <c r="G4" s="320"/>
-      <c r="H4" s="320"/>
-      <c r="I4" s="320"/>
-      <c r="J4" s="320"/>
-      <c r="K4" s="320"/>
-      <c r="L4" s="320"/>
-      <c r="M4" s="320"/>
-      <c r="N4" s="320"/>
-      <c r="O4" s="320"/>
-      <c r="P4" s="320"/>
-      <c r="Q4" s="320"/>
+      <c r="G4" s="338"/>
+      <c r="H4" s="338"/>
+      <c r="I4" s="338"/>
+      <c r="J4" s="338"/>
+      <c r="K4" s="338"/>
+      <c r="L4" s="338"/>
+      <c r="M4" s="338"/>
+      <c r="N4" s="338"/>
+      <c r="O4" s="338"/>
+      <c r="P4" s="338"/>
+      <c r="Q4" s="338"/>
       <c r="R4" s="206"/>
     </row>
     <row r="5" spans="2:18" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="316">
+      <c r="B5" s="334">
         <v>80</v>
       </c>
-      <c r="C5" s="317"/>
-      <c r="D5" s="317"/>
-      <c r="E5" s="318"/>
+      <c r="C5" s="335"/>
+      <c r="D5" s="335"/>
+      <c r="E5" s="336"/>
       <c r="F5" s="205">
         <v>6</v>
       </c>
@@ -26519,29 +26842,29 @@
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B8" s="207"/>
-      <c r="C8" s="314" t="s">
+      <c r="C8" s="332" t="s">
         <v>165</v>
       </c>
-      <c r="D8" s="314"/>
+      <c r="D8" s="332"/>
       <c r="E8" s="197"/>
       <c r="F8" s="212"/>
       <c r="G8" s="213"/>
-      <c r="H8" s="309" t="s">
+      <c r="H8" s="327" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="310"/>
+      <c r="I8" s="328"/>
       <c r="J8" s="212"/>
       <c r="K8" s="213"/>
-      <c r="L8" s="309" t="s">
+      <c r="L8" s="327" t="s">
         <v>74</v>
       </c>
-      <c r="M8" s="310"/>
+      <c r="M8" s="328"/>
       <c r="N8" s="212"/>
       <c r="O8" s="213"/>
-      <c r="P8" s="312" t="s">
+      <c r="P8" s="330" t="s">
         <v>74</v>
       </c>
-      <c r="Q8" s="313"/>
+      <c r="Q8" s="331"/>
       <c r="R8" s="196"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.35">
@@ -26553,22 +26876,22 @@
         <v>20</v>
       </c>
       <c r="E9" s="199"/>
-      <c r="F9" s="325" t="s">
+      <c r="F9" s="326" t="s">
         <v>73</v>
       </c>
-      <c r="G9" s="325"/>
+      <c r="G9" s="326"/>
       <c r="H9" s="216"/>
       <c r="I9" s="217"/>
-      <c r="J9" s="325" t="s">
+      <c r="J9" s="326" t="s">
         <v>73</v>
       </c>
-      <c r="K9" s="325"/>
+      <c r="K9" s="326"/>
       <c r="L9" s="218"/>
       <c r="M9" s="218"/>
-      <c r="N9" s="325" t="s">
+      <c r="N9" s="326" t="s">
         <v>73</v>
       </c>
-      <c r="O9" s="325"/>
+      <c r="O9" s="326"/>
       <c r="P9" s="218"/>
       <c r="Q9" s="218"/>
       <c r="R9" s="196"/>
@@ -26601,28 +26924,28 @@
       <c r="C11" s="201"/>
       <c r="D11" s="201"/>
       <c r="E11" s="201"/>
-      <c r="F11" s="321" t="s">
+      <c r="F11" s="339" t="s">
         <v>174</v>
       </c>
-      <c r="G11" s="321"/>
-      <c r="H11" s="321"/>
-      <c r="I11" s="321"/>
-      <c r="J11" s="321"/>
-      <c r="K11" s="321"/>
-      <c r="L11" s="321"/>
-      <c r="M11" s="321"/>
-      <c r="N11" s="321"/>
-      <c r="O11" s="321"/>
-      <c r="P11" s="321"/>
-      <c r="Q11" s="321"/>
+      <c r="G11" s="339"/>
+      <c r="H11" s="339"/>
+      <c r="I11" s="339"/>
+      <c r="J11" s="339"/>
+      <c r="K11" s="339"/>
+      <c r="L11" s="339"/>
+      <c r="M11" s="339"/>
+      <c r="N11" s="339"/>
+      <c r="O11" s="339"/>
+      <c r="P11" s="339"/>
+      <c r="Q11" s="339"/>
       <c r="R11" s="196"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B12" s="202"/>
-      <c r="C12" s="314" t="s">
+      <c r="C12" s="332" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="314"/>
+      <c r="D12" s="332"/>
       <c r="E12" s="202"/>
       <c r="F12" s="226"/>
       <c r="G12" s="226"/>
@@ -26650,15 +26973,15 @@
       <c r="F13" s="227"/>
       <c r="G13" s="228"/>
       <c r="H13" s="227"/>
-      <c r="I13" s="324" t="s">
+      <c r="I13" s="325" t="s">
         <v>176</v>
       </c>
-      <c r="J13" s="324"/>
-      <c r="K13" s="324"/>
-      <c r="L13" s="324"/>
-      <c r="M13" s="324"/>
-      <c r="N13" s="324"/>
-      <c r="O13" s="324"/>
+      <c r="J13" s="325"/>
+      <c r="K13" s="325"/>
+      <c r="L13" s="325"/>
+      <c r="M13" s="325"/>
+      <c r="N13" s="325"/>
+      <c r="O13" s="325"/>
       <c r="P13" s="229"/>
       <c r="Q13" s="229"/>
       <c r="R13" s="196"/>
@@ -26679,9 +27002,9 @@
       <c r="J14" s="244" t="s">
         <v>177</v>
       </c>
-      <c r="K14" s="323"/>
-      <c r="L14" s="323"/>
-      <c r="M14" s="323"/>
+      <c r="K14" s="324"/>
+      <c r="L14" s="324"/>
+      <c r="M14" s="324"/>
       <c r="N14" s="244" t="s">
         <v>178</v>
       </c>
@@ -26761,13 +27084,13 @@
       <c r="G17" s="227"/>
       <c r="H17" s="227"/>
       <c r="I17" s="237"/>
-      <c r="J17" s="322" t="s">
+      <c r="J17" s="323" t="s">
         <v>175</v>
       </c>
-      <c r="K17" s="322"/>
-      <c r="L17" s="322"/>
-      <c r="M17" s="322"/>
-      <c r="N17" s="322"/>
+      <c r="K17" s="323"/>
+      <c r="L17" s="323"/>
+      <c r="M17" s="323"/>
+      <c r="N17" s="323"/>
       <c r="O17" s="238"/>
       <c r="P17" s="227"/>
       <c r="Q17" s="227"/>
@@ -26808,14 +27131,65 @@
       <c r="P19" s="227"/>
       <c r="Q19" s="227"/>
     </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B21" s="340" t="s">
+        <v>191</v>
+      </c>
+      <c r="C21" s="340"/>
+      <c r="D21" s="340"/>
+      <c r="E21" s="340"/>
+      <c r="F21" s="340"/>
+      <c r="G21" s="340"/>
+      <c r="H21" s="340"/>
+      <c r="I21" s="340"/>
+      <c r="J21" s="340"/>
+      <c r="K21" s="340"/>
+      <c r="L21" s="340"/>
+      <c r="M21" s="340"/>
+      <c r="N21" s="340"/>
+      <c r="O21" s="340"/>
+      <c r="P21" s="340"/>
+      <c r="Q21" s="340"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B22" s="340"/>
+      <c r="C22" s="340"/>
+      <c r="D22" s="340"/>
+      <c r="E22" s="340"/>
+      <c r="F22" s="340"/>
+      <c r="G22" s="340"/>
+      <c r="H22" s="340"/>
+      <c r="I22" s="340"/>
+      <c r="J22" s="340"/>
+      <c r="K22" s="340"/>
+      <c r="L22" s="340"/>
+      <c r="M22" s="340"/>
+      <c r="N22" s="340"/>
+      <c r="O22" s="340"/>
+      <c r="P22" s="340"/>
+      <c r="Q22" s="340"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B23" s="340"/>
+      <c r="C23" s="340"/>
+      <c r="D23" s="340"/>
+      <c r="E23" s="340"/>
+      <c r="F23" s="340"/>
+      <c r="G23" s="340"/>
+      <c r="H23" s="340"/>
+      <c r="I23" s="340"/>
+      <c r="J23" s="340"/>
+      <c r="K23" s="340"/>
+      <c r="L23" s="340"/>
+      <c r="M23" s="340"/>
+      <c r="N23" s="340"/>
+      <c r="O23" s="340"/>
+      <c r="P23" s="340"/>
+      <c r="Q23" s="340"/>
+    </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="J17:N17"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="I13:O13"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="N9:O9"/>
+  <mergeCells count="18">
+    <mergeCell ref="B21:Q23"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="F3:Q3"/>
     <mergeCell ref="H8:I8"/>
@@ -26827,6 +27201,12 @@
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="F4:Q4"/>
     <mergeCell ref="F11:Q11"/>
+    <mergeCell ref="J17:N17"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="I13:O13"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="N9:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed File Naming Structure
- In each file name:
- if the critical word is an s or sh
- if the critical word is shifted or not shifted
- the full written out stimuli
</commit_message>
<xml_diff>
--- a/Writeups/Exp.1_Master.xlsx
+++ b/Writeups/Exp.1_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\Social.Influence_Speech.Perception\SI.SP\Writeups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40260C03-AA70-408E-8AAB-F397728AE770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA4A4A8-B532-480B-9246-32D82B4EBED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6F4FE53E-24C5-4985-9E6F-6A265A63BA90}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{6F4FE53E-24C5-4985-9E6F-6A265A63BA90}"/>
   </bookViews>
   <sheets>
     <sheet name="Exposure Phase" sheetId="1" r:id="rId1"/>
@@ -2948,6 +2948,48 @@
     <xf numFmtId="0" fontId="1" fillId="18" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2990,121 +3032,121 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="180"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3119,6 +3161,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="44" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3130,90 +3214,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="37" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3223,16 +3223,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFECFFCD"/>
+      <color rgb="FFEDF2F9"/>
+      <color rgb="FFE9EEF7"/>
+      <color rgb="FFE3E9F5"/>
       <color rgb="FFD1DFA9"/>
       <color rgb="FFB5CC76"/>
       <color rgb="FFFFDAA3"/>
       <color rgb="FF77CEF9"/>
       <color rgb="FFB2E3FC"/>
       <color rgb="FFFFBE5F"/>
-      <color rgb="FFDEF3FE"/>
-      <color rgb="FFFFE8C5"/>
-      <color rgb="FFE0EED6"/>
-      <color rgb="FFFFF3CD"/>
     </mruColors>
   </colors>
   <extLst>
@@ -4880,7 +4880,7 @@
   </sheetPr>
   <dimension ref="A1:AH718"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="65" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AL19" sqref="AL19"/>
     </sheetView>
   </sheetViews>
@@ -4925,14 +4925,14 @@
       <c r="AB1" s="5"/>
     </row>
     <row r="2" spans="1:34" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="268" t="s">
+      <c r="B2" s="282" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="268"/>
-      <c r="D2" s="268"/>
-      <c r="E2" s="268"/>
-      <c r="F2" s="268"/>
-      <c r="G2" s="268"/>
+      <c r="C2" s="282"/>
+      <c r="D2" s="282"/>
+      <c r="E2" s="282"/>
+      <c r="F2" s="282"/>
+      <c r="G2" s="282"/>
       <c r="H2" s="20"/>
       <c r="I2" s="13" t="s">
         <v>179</v>
@@ -4942,40 +4942,40 @@
         <v>17</v>
       </c>
       <c r="L2" s="20"/>
-      <c r="M2" s="268" t="s">
+      <c r="M2" s="282" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="268"/>
-      <c r="O2" s="268"/>
-      <c r="P2" s="268"/>
-      <c r="Q2" s="268"/>
-      <c r="R2" s="268"/>
-      <c r="S2" s="268"/>
-      <c r="T2" s="268"/>
-      <c r="U2" s="268"/>
-      <c r="V2" s="268"/>
-      <c r="W2" s="268"/>
-      <c r="X2" s="268"/>
-      <c r="Y2" s="268"/>
-      <c r="Z2" s="268"/>
-      <c r="AA2" s="268"/>
-      <c r="AB2" s="268"/>
+      <c r="N2" s="282"/>
+      <c r="O2" s="282"/>
+      <c r="P2" s="282"/>
+      <c r="Q2" s="282"/>
+      <c r="R2" s="282"/>
+      <c r="S2" s="282"/>
+      <c r="T2" s="282"/>
+      <c r="U2" s="282"/>
+      <c r="V2" s="282"/>
+      <c r="W2" s="282"/>
+      <c r="X2" s="282"/>
+      <c r="Y2" s="282"/>
+      <c r="Z2" s="282"/>
+      <c r="AA2" s="282"/>
+      <c r="AB2" s="282"/>
     </row>
     <row r="3" spans="1:34" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="269" t="s">
+      <c r="B3" s="283" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="270"/>
-      <c r="D3" s="270"/>
-      <c r="E3" s="270"/>
-      <c r="F3" s="270"/>
-      <c r="G3" s="271"/>
+      <c r="C3" s="284"/>
+      <c r="D3" s="284"/>
+      <c r="E3" s="284"/>
+      <c r="F3" s="284"/>
+      <c r="G3" s="285"/>
       <c r="H3" s="28"/>
-      <c r="I3" s="272" t="s">
+      <c r="I3" s="286" t="s">
         <v>25</v>
       </c>
       <c r="J3" s="28"/>
-      <c r="K3" s="272" t="s">
+      <c r="K3" s="286" t="s">
         <v>27</v>
       </c>
       <c r="L3" s="3"/>
@@ -4983,26 +4983,26 @@
         <v>21</v>
       </c>
       <c r="N3" s="251"/>
-      <c r="O3" s="276" t="s">
+      <c r="O3" s="290" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="276"/>
-      <c r="Q3" s="276"/>
-      <c r="R3" s="276"/>
+      <c r="P3" s="290"/>
+      <c r="Q3" s="290"/>
+      <c r="R3" s="290"/>
       <c r="S3" s="191"/>
-      <c r="T3" s="276" t="s">
+      <c r="T3" s="290" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="276"/>
-      <c r="V3" s="276"/>
-      <c r="W3" s="276"/>
+      <c r="U3" s="290"/>
+      <c r="V3" s="290"/>
+      <c r="W3" s="290"/>
       <c r="X3" s="190"/>
-      <c r="Y3" s="276" t="s">
+      <c r="Y3" s="290" t="s">
         <v>14</v>
       </c>
-      <c r="Z3" s="276"/>
-      <c r="AA3" s="276"/>
-      <c r="AB3" s="277"/>
+      <c r="Z3" s="290"/>
+      <c r="AA3" s="290"/>
+      <c r="AB3" s="291"/>
     </row>
     <row r="4" spans="1:34" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D4" s="4"/>
@@ -5010,34 +5010,34 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="274"/>
+      <c r="I4" s="288"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="273"/>
+      <c r="K4" s="287"/>
       <c r="L4" s="5"/>
-      <c r="M4" s="273" t="s">
+      <c r="M4" s="287" t="s">
         <v>180</v>
       </c>
       <c r="N4" s="193"/>
-      <c r="O4" s="275" t="s">
+      <c r="O4" s="289" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="275"/>
-      <c r="Q4" s="275"/>
-      <c r="R4" s="275"/>
+      <c r="P4" s="289"/>
+      <c r="Q4" s="289"/>
+      <c r="R4" s="289"/>
       <c r="S4" s="192"/>
-      <c r="T4" s="275" t="s">
+      <c r="T4" s="289" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="275"/>
-      <c r="V4" s="275"/>
-      <c r="W4" s="275"/>
+      <c r="U4" s="289"/>
+      <c r="V4" s="289"/>
+      <c r="W4" s="289"/>
       <c r="X4" s="193"/>
-      <c r="Y4" s="275" t="s">
+      <c r="Y4" s="289" t="s">
         <v>30</v>
       </c>
-      <c r="Z4" s="275"/>
-      <c r="AA4" s="275"/>
-      <c r="AB4" s="275"/>
+      <c r="Z4" s="289"/>
+      <c r="AA4" s="289"/>
+      <c r="AB4" s="289"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="C5" s="4" t="s">
@@ -5056,10 +5056,10 @@
         <v>3</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="274"/>
+      <c r="I5" s="288"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="273"/>
-      <c r="M5" s="273"/>
+      <c r="K5" s="287"/>
+      <c r="M5" s="287"/>
       <c r="N5" s="194"/>
       <c r="O5" s="7" t="s">
         <v>18</v>
@@ -5129,10 +5129,10 @@
       <c r="AA6" s="10"/>
       <c r="AB6" s="9"/>
       <c r="AE6" s="33"/>
-      <c r="AF6" s="266" t="s">
+      <c r="AF6" s="280" t="s">
         <v>28</v>
       </c>
-      <c r="AG6" s="278"/>
+      <c r="AG6" s="292"/>
       <c r="AH6" s="32"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.35">
@@ -5204,8 +5204,8 @@
         <v>9</v>
       </c>
       <c r="AE7" s="34"/>
-      <c r="AF7" s="266"/>
-      <c r="AG7" s="278"/>
+      <c r="AF7" s="280"/>
+      <c r="AG7" s="292"/>
       <c r="AH7" s="32"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.35">
@@ -5258,8 +5258,8 @@
         <v>8</v>
       </c>
       <c r="AE8" s="34"/>
-      <c r="AF8" s="266"/>
-      <c r="AG8" s="278"/>
+      <c r="AF8" s="280"/>
+      <c r="AG8" s="292"/>
       <c r="AH8" s="32"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.35">
@@ -5290,8 +5290,8 @@
       <c r="AA9" s="12"/>
       <c r="AB9" s="14"/>
       <c r="AE9" s="34"/>
-      <c r="AF9" s="266"/>
-      <c r="AG9" s="278"/>
+      <c r="AF9" s="280"/>
+      <c r="AG9" s="292"/>
       <c r="AH9" s="32"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.35">
@@ -5350,8 +5350,8 @@
         <v>9</v>
       </c>
       <c r="AE10" s="34"/>
-      <c r="AF10" s="266"/>
-      <c r="AG10" s="278"/>
+      <c r="AF10" s="280"/>
+      <c r="AG10" s="292"/>
       <c r="AH10" s="32"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.35">
@@ -5394,8 +5394,8 @@
         <v>8</v>
       </c>
       <c r="AE11" s="35"/>
-      <c r="AF11" s="266"/>
-      <c r="AG11" s="278"/>
+      <c r="AF11" s="280"/>
+      <c r="AG11" s="292"/>
       <c r="AH11" s="32"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.35">
@@ -5702,10 +5702,10 @@
       <c r="AA18" s="9"/>
       <c r="AB18" s="9"/>
       <c r="AE18" s="37"/>
-      <c r="AF18" s="266" t="s">
+      <c r="AF18" s="280" t="s">
         <v>28</v>
       </c>
-      <c r="AG18" s="267"/>
+      <c r="AG18" s="281"/>
     </row>
     <row r="19" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B19" s="11">
@@ -5776,8 +5776,8 @@
         <v>9</v>
       </c>
       <c r="AE19" s="2"/>
-      <c r="AF19" s="266"/>
-      <c r="AG19" s="267"/>
+      <c r="AF19" s="280"/>
+      <c r="AG19" s="281"/>
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B20" s="20"/>
@@ -5829,8 +5829,8 @@
         <v>8</v>
       </c>
       <c r="AE20" s="2"/>
-      <c r="AF20" s="266"/>
-      <c r="AG20" s="267"/>
+      <c r="AF20" s="280"/>
+      <c r="AG20" s="281"/>
     </row>
     <row r="21" spans="2:33" x14ac:dyDescent="0.35">
       <c r="C21" s="23"/>
@@ -5860,8 +5860,8 @@
       <c r="AA21" s="12"/>
       <c r="AB21" s="14"/>
       <c r="AE21" s="2"/>
-      <c r="AF21" s="266"/>
-      <c r="AG21" s="267"/>
+      <c r="AF21" s="280"/>
+      <c r="AG21" s="281"/>
     </row>
     <row r="22" spans="2:33" x14ac:dyDescent="0.35">
       <c r="C22" s="23"/>
@@ -5919,8 +5919,8 @@
         <v>9</v>
       </c>
       <c r="AE22" s="2"/>
-      <c r="AF22" s="266"/>
-      <c r="AG22" s="267"/>
+      <c r="AF22" s="280"/>
+      <c r="AG22" s="281"/>
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.35">
       <c r="C23" s="23"/>
@@ -5961,8 +5961,8 @@
         <v>8</v>
       </c>
       <c r="AE23" s="36"/>
-      <c r="AF23" s="266"/>
-      <c r="AG23" s="267"/>
+      <c r="AF23" s="280"/>
+      <c r="AG23" s="281"/>
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B24" s="11"/>
@@ -23244,11 +23244,11 @@
       <c r="C3" s="189" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="280" t="s">
+      <c r="D3" s="312" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="281"/>
-      <c r="F3" s="281"/>
+      <c r="E3" s="299"/>
+      <c r="F3" s="299"/>
       <c r="G3" s="79"/>
       <c r="H3" s="188" t="s">
         <v>76</v>
@@ -23256,46 +23256,46 @@
       <c r="I3" s="189" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="280" t="s">
+      <c r="J3" s="312" t="s">
         <v>79</v>
       </c>
-      <c r="K3" s="281"/>
-      <c r="L3" s="281"/>
-      <c r="N3" s="282" t="s">
+      <c r="K3" s="299"/>
+      <c r="L3" s="299"/>
+      <c r="N3" s="314" t="s">
         <v>80</v>
       </c>
-      <c r="O3" s="282"/>
+      <c r="O3" s="314"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="282" t="s">
+      <c r="Q3" s="314" t="s">
         <v>81</v>
       </c>
-      <c r="R3" s="282"/>
+      <c r="R3" s="314"/>
       <c r="S3" s="19"/>
       <c r="T3" s="179"/>
       <c r="U3" s="179"/>
-      <c r="V3" s="296" t="s">
+      <c r="V3" s="294" t="s">
         <v>80</v>
       </c>
-      <c r="W3" s="296"/>
-      <c r="X3" s="296"/>
+      <c r="W3" s="294"/>
+      <c r="X3" s="294"/>
       <c r="Y3" s="179"/>
       <c r="Z3" s="179"/>
-      <c r="AB3" s="279" t="s">
+      <c r="AB3" s="293" t="s">
         <v>157</v>
       </c>
-      <c r="AC3" s="279"/>
-      <c r="AD3" s="279"/>
-      <c r="AE3" s="279"/>
-      <c r="AF3" s="279"/>
-      <c r="AG3" s="279"/>
-      <c r="AH3" s="279"/>
-      <c r="AI3" s="279"/>
-      <c r="AJ3" s="279"/>
-      <c r="AL3" s="279" t="s">
+      <c r="AC3" s="293"/>
+      <c r="AD3" s="293"/>
+      <c r="AE3" s="293"/>
+      <c r="AF3" s="293"/>
+      <c r="AG3" s="293"/>
+      <c r="AH3" s="293"/>
+      <c r="AI3" s="293"/>
+      <c r="AJ3" s="293"/>
+      <c r="AL3" s="293" t="s">
         <v>32</v>
       </c>
-      <c r="AM3" s="279"/>
-      <c r="AN3" s="279"/>
+      <c r="AM3" s="293"/>
+      <c r="AN3" s="293"/>
     </row>
     <row r="4" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="97" t="s">
@@ -23304,9 +23304,9 @@
       <c r="C4" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="280"/>
-      <c r="E4" s="281"/>
-      <c r="F4" s="281"/>
+      <c r="D4" s="312"/>
+      <c r="E4" s="299"/>
+      <c r="F4" s="299"/>
       <c r="G4" s="79"/>
       <c r="H4" s="97" t="s">
         <v>82</v>
@@ -23314,9 +23314,9 @@
       <c r="I4" s="93" t="s">
         <v>84</v>
       </c>
-      <c r="J4" s="280"/>
-      <c r="K4" s="281"/>
-      <c r="L4" s="281"/>
+      <c r="J4" s="312"/>
+      <c r="K4" s="299"/>
+      <c r="L4" s="299"/>
       <c r="N4" s="86" t="s">
         <v>76</v>
       </c>
@@ -23336,11 +23336,11 @@
       <c r="W4" s="116"/>
       <c r="X4" s="117"/>
       <c r="Z4" s="179"/>
-      <c r="AL4" s="295" t="s">
+      <c r="AL4" s="300" t="s">
         <v>160</v>
       </c>
-      <c r="AM4" s="295"/>
-      <c r="AN4" s="295"/>
+      <c r="AM4" s="300"/>
+      <c r="AN4" s="300"/>
     </row>
     <row r="5" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="94" t="s">
@@ -23349,11 +23349,11 @@
       <c r="C5" s="98" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="280" t="s">
+      <c r="D5" s="312" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="281"/>
-      <c r="F5" s="281"/>
+      <c r="E5" s="299"/>
+      <c r="F5" s="299"/>
       <c r="G5" s="79"/>
       <c r="H5" s="94" t="s">
         <v>87</v>
@@ -23361,9 +23361,9 @@
       <c r="I5" s="98" t="s">
         <v>90</v>
       </c>
-      <c r="J5" s="280"/>
-      <c r="K5" s="281"/>
-      <c r="L5" s="281"/>
+      <c r="J5" s="312"/>
+      <c r="K5" s="299"/>
+      <c r="L5" s="299"/>
       <c r="N5" s="154" t="s">
         <v>149</v>
       </c>
@@ -23378,7 +23378,7 @@
         <v>149</v>
       </c>
       <c r="S5" s="19"/>
-      <c r="T5" s="298" t="s">
+      <c r="T5" s="296" t="s">
         <v>149</v>
       </c>
       <c r="U5" s="118"/>
@@ -23390,24 +23390,24 @@
         <v>84</v>
       </c>
       <c r="Y5" s="121"/>
-      <c r="Z5" s="300" t="s">
+      <c r="Z5" s="298" t="s">
         <v>150</v>
       </c>
       <c r="AA5" s="179"/>
-      <c r="AB5" s="279" t="s">
+      <c r="AB5" s="293" t="s">
         <v>189</v>
       </c>
-      <c r="AC5" s="279"/>
-      <c r="AD5" s="279"/>
-      <c r="AE5" s="279"/>
-      <c r="AF5" s="279"/>
-      <c r="AG5" s="279"/>
-      <c r="AH5" s="279"/>
-      <c r="AI5" s="279"/>
-      <c r="AJ5" s="279"/>
-      <c r="AL5" s="295"/>
-      <c r="AM5" s="295"/>
-      <c r="AN5" s="295"/>
+      <c r="AC5" s="293"/>
+      <c r="AD5" s="293"/>
+      <c r="AE5" s="293"/>
+      <c r="AF5" s="293"/>
+      <c r="AG5" s="293"/>
+      <c r="AH5" s="293"/>
+      <c r="AI5" s="293"/>
+      <c r="AJ5" s="293"/>
+      <c r="AL5" s="300"/>
+      <c r="AM5" s="300"/>
+      <c r="AN5" s="300"/>
       <c r="AO5" s="19"/>
     </row>
     <row r="6" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -23427,9 +23427,9 @@
       <c r="I6" s="95" t="s">
         <v>95</v>
       </c>
-      <c r="J6" s="280"/>
-      <c r="K6" s="281"/>
-      <c r="L6" s="281"/>
+      <c r="J6" s="312"/>
+      <c r="K6" s="299"/>
+      <c r="L6" s="299"/>
       <c r="N6" s="119" t="s">
         <v>82</v>
       </c>
@@ -23443,7 +23443,7 @@
         <v>85</v>
       </c>
       <c r="S6" s="19"/>
-      <c r="T6" s="299"/>
+      <c r="T6" s="297"/>
       <c r="U6" s="122"/>
       <c r="V6" s="80" t="s">
         <v>91</v>
@@ -23453,7 +23453,7 @@
         <v>101</v>
       </c>
       <c r="Y6" s="124"/>
-      <c r="Z6" s="300"/>
+      <c r="Z6" s="298"/>
       <c r="AA6" s="179"/>
       <c r="AB6" s="177" t="s">
         <v>86</v>
@@ -23480,9 +23480,9 @@
       <c r="AJ6" s="171" t="s">
         <v>86</v>
       </c>
-      <c r="AL6" s="295"/>
-      <c r="AM6" s="295"/>
-      <c r="AN6" s="295"/>
+      <c r="AL6" s="300"/>
+      <c r="AM6" s="300"/>
+      <c r="AN6" s="300"/>
       <c r="AO6" s="19"/>
     </row>
     <row r="7" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -23492,11 +23492,11 @@
       <c r="C7" s="98" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="280" t="s">
+      <c r="D7" s="312" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="281"/>
-      <c r="F7" s="281"/>
+      <c r="E7" s="299"/>
+      <c r="F7" s="299"/>
       <c r="G7" s="79"/>
       <c r="H7" s="94" t="s">
         <v>98</v>
@@ -23504,9 +23504,9 @@
       <c r="I7" s="98" t="s">
         <v>100</v>
       </c>
-      <c r="J7" s="280"/>
-      <c r="K7" s="281"/>
-      <c r="L7" s="281"/>
+      <c r="J7" s="312"/>
+      <c r="K7" s="299"/>
+      <c r="L7" s="299"/>
       <c r="N7" s="80" t="s">
         <v>91</v>
       </c>
@@ -23520,7 +23520,7 @@
         <v>90</v>
       </c>
       <c r="S7" s="19"/>
-      <c r="T7" s="299"/>
+      <c r="T7" s="297"/>
       <c r="U7" s="122"/>
       <c r="V7" s="105" t="s">
         <v>93</v>
@@ -23530,7 +23530,7 @@
         <v>95</v>
       </c>
       <c r="Y7" s="124"/>
-      <c r="Z7" s="300"/>
+      <c r="Z7" s="298"/>
       <c r="AA7" s="140"/>
       <c r="AB7" s="258" t="s">
         <v>92</v>
@@ -23549,9 +23549,9 @@
       </c>
       <c r="AI7" s="261"/>
       <c r="AJ7" s="263"/>
-      <c r="AL7" s="295"/>
-      <c r="AM7" s="295"/>
-      <c r="AN7" s="295"/>
+      <c r="AL7" s="300"/>
+      <c r="AM7" s="300"/>
+      <c r="AN7" s="300"/>
       <c r="AO7" s="19"/>
     </row>
     <row r="8" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -23561,9 +23561,9 @@
       <c r="C8" s="95" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="280"/>
-      <c r="E8" s="281"/>
-      <c r="F8" s="281"/>
+      <c r="D8" s="312"/>
+      <c r="E8" s="299"/>
+      <c r="F8" s="299"/>
       <c r="G8" s="41"/>
       <c r="H8" s="99" t="s">
         <v>104</v>
@@ -23571,11 +23571,11 @@
       <c r="I8" s="95" t="s">
         <v>106</v>
       </c>
-      <c r="J8" s="294" t="s">
+      <c r="J8" s="313" t="s">
         <v>107</v>
       </c>
-      <c r="K8" s="279"/>
-      <c r="L8" s="279"/>
+      <c r="K8" s="293"/>
+      <c r="L8" s="293"/>
       <c r="N8" s="105" t="s">
         <v>93</v>
       </c>
@@ -23589,7 +23589,7 @@
         <v>97</v>
       </c>
       <c r="S8" s="19"/>
-      <c r="T8" s="299"/>
+      <c r="T8" s="297"/>
       <c r="U8" s="122"/>
       <c r="V8" s="80" t="s">
         <v>102</v>
@@ -23599,7 +23599,7 @@
         <v>112</v>
       </c>
       <c r="Y8" s="124"/>
-      <c r="Z8" s="300"/>
+      <c r="Z8" s="298"/>
       <c r="AA8" s="140"/>
       <c r="AB8" s="172" t="s">
         <v>92</v>
@@ -23618,9 +23618,9 @@
       </c>
       <c r="AI8" s="169"/>
       <c r="AJ8" s="175"/>
-      <c r="AL8" s="295"/>
-      <c r="AM8" s="295"/>
-      <c r="AN8" s="295"/>
+      <c r="AL8" s="300"/>
+      <c r="AM8" s="300"/>
+      <c r="AN8" s="300"/>
       <c r="AO8" s="19"/>
     </row>
     <row r="9" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -23630,9 +23630,9 @@
       <c r="C9" s="98" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="280"/>
-      <c r="E9" s="281"/>
-      <c r="F9" s="281"/>
+      <c r="D9" s="312"/>
+      <c r="E9" s="299"/>
+      <c r="F9" s="299"/>
       <c r="G9" s="79"/>
       <c r="H9" s="94" t="s">
         <v>110</v>
@@ -23653,7 +23653,7 @@
         <v>100</v>
       </c>
       <c r="S9" s="19"/>
-      <c r="T9" s="299"/>
+      <c r="T9" s="297"/>
       <c r="U9" s="122"/>
       <c r="V9" s="105" t="s">
         <v>104</v>
@@ -23663,7 +23663,7 @@
         <v>106</v>
       </c>
       <c r="Y9" s="124"/>
-      <c r="Z9" s="300"/>
+      <c r="Z9" s="298"/>
       <c r="AA9" s="140"/>
       <c r="AB9" s="173" t="s">
         <v>103</v>
@@ -23690,9 +23690,9 @@
       <c r="AJ9" s="176" t="s">
         <v>103</v>
       </c>
-      <c r="AL9" s="295"/>
-      <c r="AM9" s="295"/>
-      <c r="AN9" s="295"/>
+      <c r="AL9" s="300"/>
+      <c r="AM9" s="300"/>
+      <c r="AN9" s="300"/>
       <c r="AO9" s="166"/>
     </row>
     <row r="10" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -23702,9 +23702,9 @@
       <c r="C10" s="95" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="280"/>
-      <c r="E10" s="281"/>
-      <c r="F10" s="281"/>
+      <c r="D10" s="312"/>
+      <c r="E10" s="299"/>
+      <c r="F10" s="299"/>
       <c r="G10" s="79"/>
       <c r="H10" s="99" t="s">
         <v>114</v>
@@ -23712,11 +23712,11 @@
       <c r="I10" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="J10" s="280" t="s">
+      <c r="J10" s="312" t="s">
         <v>116</v>
       </c>
-      <c r="K10" s="281"/>
-      <c r="L10" s="281"/>
+      <c r="K10" s="299"/>
+      <c r="L10" s="299"/>
       <c r="N10" s="105" t="s">
         <v>104</v>
       </c>
@@ -23730,7 +23730,7 @@
         <v>109</v>
       </c>
       <c r="S10" s="19"/>
-      <c r="T10" s="299"/>
+      <c r="T10" s="297"/>
       <c r="U10" s="122"/>
       <c r="V10" s="80" t="s">
         <v>113</v>
@@ -23740,7 +23740,7 @@
         <v>120</v>
       </c>
       <c r="Y10" s="124"/>
-      <c r="Z10" s="300"/>
+      <c r="Z10" s="298"/>
       <c r="AA10" s="140"/>
       <c r="AB10" s="248"/>
       <c r="AC10" s="248"/>
@@ -23751,9 +23751,9 @@
       <c r="AH10" s="248"/>
       <c r="AI10" s="248"/>
       <c r="AJ10" s="248"/>
-      <c r="AL10" s="295"/>
-      <c r="AM10" s="295"/>
-      <c r="AN10" s="295"/>
+      <c r="AL10" s="300"/>
+      <c r="AM10" s="300"/>
+      <c r="AN10" s="300"/>
       <c r="AO10" s="19"/>
     </row>
     <row r="11" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -23763,9 +23763,9 @@
       <c r="C11" s="98" t="s">
         <v>118</v>
       </c>
-      <c r="D11" s="280"/>
-      <c r="E11" s="281"/>
-      <c r="F11" s="281"/>
+      <c r="D11" s="312"/>
+      <c r="E11" s="299"/>
+      <c r="F11" s="299"/>
       <c r="G11" s="79"/>
       <c r="H11" s="94" t="s">
         <v>119</v>
@@ -23773,9 +23773,9 @@
       <c r="I11" s="98" t="s">
         <v>115</v>
       </c>
-      <c r="J11" s="280"/>
-      <c r="K11" s="281"/>
-      <c r="L11" s="281"/>
+      <c r="J11" s="312"/>
+      <c r="K11" s="299"/>
+      <c r="L11" s="299"/>
       <c r="N11" s="80" t="s">
         <v>113</v>
       </c>
@@ -23789,7 +23789,7 @@
         <v>111</v>
       </c>
       <c r="S11" s="19"/>
-      <c r="T11" s="299"/>
+      <c r="T11" s="297"/>
       <c r="U11" s="122"/>
       <c r="V11" s="105" t="s">
         <v>114</v>
@@ -23799,7 +23799,7 @@
         <v>83</v>
       </c>
       <c r="Y11" s="124"/>
-      <c r="Z11" s="300"/>
+      <c r="Z11" s="298"/>
       <c r="AA11" s="140"/>
       <c r="AB11" s="172" t="s">
         <v>86</v>
@@ -23826,9 +23826,9 @@
       <c r="AJ11" s="175" t="s">
         <v>86</v>
       </c>
-      <c r="AL11" s="295"/>
-      <c r="AM11" s="295"/>
-      <c r="AN11" s="295"/>
+      <c r="AL11" s="300"/>
+      <c r="AM11" s="300"/>
+      <c r="AN11" s="300"/>
       <c r="AO11" s="19"/>
     </row>
     <row r="12" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -23838,9 +23838,9 @@
       <c r="C12" s="95" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="280"/>
-      <c r="E12" s="281"/>
-      <c r="F12" s="281"/>
+      <c r="D12" s="312"/>
+      <c r="E12" s="299"/>
+      <c r="F12" s="299"/>
       <c r="G12" s="79"/>
       <c r="H12" s="99" t="s">
         <v>122</v>
@@ -23848,9 +23848,9 @@
       <c r="I12" s="95" t="s">
         <v>105</v>
       </c>
-      <c r="J12" s="280"/>
-      <c r="K12" s="281"/>
-      <c r="L12" s="281"/>
+      <c r="J12" s="312"/>
+      <c r="K12" s="299"/>
+      <c r="L12" s="299"/>
       <c r="N12" s="105" t="s">
         <v>114</v>
       </c>
@@ -23864,7 +23864,7 @@
         <v>118</v>
       </c>
       <c r="S12" s="19"/>
-      <c r="T12" s="299"/>
+      <c r="T12" s="297"/>
       <c r="U12" s="122"/>
       <c r="V12" s="80" t="s">
         <v>121</v>
@@ -23874,7 +23874,7 @@
         <v>94</v>
       </c>
       <c r="Y12" s="124"/>
-      <c r="Z12" s="300"/>
+      <c r="Z12" s="298"/>
       <c r="AA12" s="140"/>
       <c r="AB12" s="264" t="s">
         <v>92</v>
@@ -23893,9 +23893,9 @@
       </c>
       <c r="AI12" s="260"/>
       <c r="AJ12" s="259"/>
-      <c r="AL12" s="295"/>
-      <c r="AM12" s="295"/>
-      <c r="AN12" s="295"/>
+      <c r="AL12" s="300"/>
+      <c r="AM12" s="300"/>
+      <c r="AN12" s="300"/>
       <c r="AO12" s="19"/>
     </row>
     <row r="13" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -23905,9 +23905,9 @@
       <c r="C13" s="98" t="s">
         <v>100</v>
       </c>
-      <c r="D13" s="280"/>
-      <c r="E13" s="281"/>
-      <c r="F13" s="281"/>
+      <c r="D13" s="312"/>
+      <c r="E13" s="299"/>
+      <c r="F13" s="299"/>
       <c r="G13" s="79"/>
       <c r="H13" s="94" t="s">
         <v>125</v>
@@ -23915,9 +23915,9 @@
       <c r="I13" s="98" t="s">
         <v>88</v>
       </c>
-      <c r="J13" s="280"/>
-      <c r="K13" s="281"/>
-      <c r="L13" s="281"/>
+      <c r="J13" s="312"/>
+      <c r="K13" s="299"/>
+      <c r="L13" s="299"/>
       <c r="N13" s="80" t="s">
         <v>121</v>
       </c>
@@ -23931,7 +23931,7 @@
         <v>115</v>
       </c>
       <c r="S13" s="19"/>
-      <c r="T13" s="299"/>
+      <c r="T13" s="297"/>
       <c r="U13" s="122"/>
       <c r="V13" s="105" t="s">
         <v>122</v>
@@ -23941,7 +23941,7 @@
         <v>105</v>
       </c>
       <c r="Y13" s="124"/>
-      <c r="Z13" s="300"/>
+      <c r="Z13" s="298"/>
       <c r="AA13" s="140"/>
       <c r="AB13" s="177" t="s">
         <v>92</v>
@@ -23972,9 +23972,9 @@
       <c r="C14" s="95" t="s">
         <v>124</v>
       </c>
-      <c r="D14" s="280"/>
-      <c r="E14" s="281"/>
-      <c r="F14" s="281"/>
+      <c r="D14" s="312"/>
+      <c r="E14" s="299"/>
+      <c r="F14" s="299"/>
       <c r="G14" s="79"/>
       <c r="H14" s="99" t="s">
         <v>96</v>
@@ -23982,9 +23982,9 @@
       <c r="I14" s="95" t="s">
         <v>85</v>
       </c>
-      <c r="J14" s="280"/>
-      <c r="K14" s="281"/>
-      <c r="L14" s="281"/>
+      <c r="J14" s="312"/>
+      <c r="K14" s="299"/>
+      <c r="L14" s="299"/>
       <c r="N14" s="105" t="s">
         <v>122</v>
       </c>
@@ -23998,7 +23998,7 @@
         <v>124</v>
       </c>
       <c r="S14" s="19"/>
-      <c r="T14" s="299"/>
+      <c r="T14" s="297"/>
       <c r="U14" s="122"/>
       <c r="V14" s="84" t="s">
         <v>126</v>
@@ -24008,7 +24008,7 @@
         <v>128</v>
       </c>
       <c r="Y14" s="124"/>
-      <c r="Z14" s="300"/>
+      <c r="Z14" s="298"/>
       <c r="AA14" s="140"/>
       <c r="AB14" s="178" t="s">
         <v>103</v>
@@ -24035,11 +24035,11 @@
       <c r="AJ14" s="174" t="s">
         <v>103</v>
       </c>
-      <c r="AL14" s="281" t="s">
+      <c r="AL14" s="299" t="s">
         <v>158</v>
       </c>
-      <c r="AM14" s="281"/>
-      <c r="AN14" s="281"/>
+      <c r="AM14" s="299"/>
+      <c r="AN14" s="299"/>
     </row>
     <row r="15" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="94" t="s">
@@ -24048,9 +24048,9 @@
       <c r="C15" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="280"/>
-      <c r="E15" s="281"/>
-      <c r="F15" s="281"/>
+      <c r="D15" s="312"/>
+      <c r="E15" s="299"/>
+      <c r="F15" s="299"/>
       <c r="G15" s="79"/>
       <c r="H15" s="94" t="s">
         <v>91</v>
@@ -24058,9 +24058,9 @@
       <c r="I15" s="98" t="s">
         <v>101</v>
       </c>
-      <c r="J15" s="280"/>
-      <c r="K15" s="281"/>
-      <c r="L15" s="281"/>
+      <c r="J15" s="312"/>
+      <c r="K15" s="299"/>
+      <c r="L15" s="299"/>
       <c r="N15" s="84" t="s">
         <v>126</v>
       </c>
@@ -24074,16 +24074,16 @@
         <v>88</v>
       </c>
       <c r="S15" s="19"/>
-      <c r="T15" s="299"/>
+      <c r="T15" s="297"/>
       <c r="U15" s="125"/>
       <c r="V15" s="126"/>
       <c r="W15" s="127"/>
       <c r="X15" s="128"/>
       <c r="Y15" s="129"/>
-      <c r="Z15" s="300"/>
-      <c r="AL15" s="281"/>
-      <c r="AM15" s="281"/>
-      <c r="AN15" s="281"/>
+      <c r="Z15" s="298"/>
+      <c r="AL15" s="299"/>
+      <c r="AM15" s="299"/>
+      <c r="AN15" s="299"/>
       <c r="AO15" s="19"/>
     </row>
     <row r="16" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -24093,9 +24093,9 @@
       <c r="C16" s="95" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="280"/>
-      <c r="E16" s="281"/>
-      <c r="F16" s="281"/>
+      <c r="D16" s="312"/>
+      <c r="E16" s="299"/>
+      <c r="F16" s="299"/>
       <c r="G16" s="79"/>
       <c r="H16" s="99" t="s">
         <v>108</v>
@@ -24103,19 +24103,19 @@
       <c r="I16" s="95" t="s">
         <v>97</v>
       </c>
-      <c r="J16" s="280"/>
-      <c r="K16" s="281"/>
-      <c r="L16" s="281"/>
-      <c r="T16" s="299"/>
+      <c r="J16" s="312"/>
+      <c r="K16" s="299"/>
+      <c r="L16" s="299"/>
+      <c r="T16" s="297"/>
       <c r="U16" s="122"/>
       <c r="V16" s="130"/>
       <c r="W16" s="131"/>
       <c r="X16" s="132"/>
       <c r="Y16" s="124"/>
-      <c r="Z16" s="300"/>
-      <c r="AL16" s="281"/>
-      <c r="AM16" s="281"/>
-      <c r="AN16" s="281"/>
+      <c r="Z16" s="298"/>
+      <c r="AL16" s="299"/>
+      <c r="AM16" s="299"/>
+      <c r="AN16" s="299"/>
       <c r="AO16" s="19"/>
     </row>
     <row r="17" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -24125,9 +24125,9 @@
       <c r="C17" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="280"/>
-      <c r="E17" s="281"/>
-      <c r="F17" s="281"/>
+      <c r="D17" s="312"/>
+      <c r="E17" s="299"/>
+      <c r="F17" s="299"/>
       <c r="G17" s="79"/>
       <c r="H17" s="94" t="s">
         <v>102</v>
@@ -24135,11 +24135,11 @@
       <c r="I17" s="98" t="s">
         <v>112</v>
       </c>
-      <c r="J17" s="280"/>
-      <c r="K17" s="281"/>
-      <c r="L17" s="281"/>
+      <c r="J17" s="312"/>
+      <c r="K17" s="299"/>
+      <c r="L17" s="299"/>
       <c r="S17" s="142"/>
-      <c r="T17" s="299"/>
+      <c r="T17" s="297"/>
       <c r="U17" s="122"/>
       <c r="V17" s="87" t="s">
         <v>85</v>
@@ -24149,22 +24149,22 @@
         <v>96</v>
       </c>
       <c r="Y17" s="124"/>
-      <c r="Z17" s="300"/>
+      <c r="Z17" s="298"/>
       <c r="AA17" s="140"/>
-      <c r="AB17" s="279" t="s">
+      <c r="AB17" s="293" t="s">
         <v>190</v>
       </c>
-      <c r="AC17" s="279"/>
-      <c r="AD17" s="279"/>
-      <c r="AE17" s="279"/>
-      <c r="AF17" s="279"/>
-      <c r="AG17" s="279"/>
-      <c r="AH17" s="279"/>
-      <c r="AI17" s="279"/>
-      <c r="AJ17" s="279"/>
-      <c r="AL17" s="281"/>
-      <c r="AM17" s="281"/>
-      <c r="AN17" s="281"/>
+      <c r="AC17" s="293"/>
+      <c r="AD17" s="293"/>
+      <c r="AE17" s="293"/>
+      <c r="AF17" s="293"/>
+      <c r="AG17" s="293"/>
+      <c r="AH17" s="293"/>
+      <c r="AI17" s="293"/>
+      <c r="AJ17" s="293"/>
+      <c r="AL17" s="299"/>
+      <c r="AM17" s="299"/>
+      <c r="AN17" s="299"/>
       <c r="AO17" s="19"/>
     </row>
     <row r="18" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -24174,9 +24174,9 @@
       <c r="C18" s="95" t="s">
         <v>130</v>
       </c>
-      <c r="D18" s="280"/>
-      <c r="E18" s="281"/>
-      <c r="F18" s="281"/>
+      <c r="D18" s="312"/>
+      <c r="E18" s="299"/>
+      <c r="F18" s="299"/>
       <c r="G18" s="79"/>
       <c r="H18" s="99" t="s">
         <v>117</v>
@@ -24184,21 +24184,21 @@
       <c r="I18" s="95" t="s">
         <v>109</v>
       </c>
-      <c r="J18" s="280"/>
-      <c r="K18" s="281"/>
-      <c r="L18" s="281"/>
+      <c r="J18" s="312"/>
+      <c r="K18" s="299"/>
+      <c r="L18" s="299"/>
       <c r="M18" s="89"/>
-      <c r="N18" s="279" t="s">
+      <c r="N18" s="293" t="s">
         <v>149</v>
       </c>
-      <c r="O18" s="279"/>
+      <c r="O18" s="293"/>
       <c r="P18" s="89"/>
-      <c r="Q18" s="284" t="s">
+      <c r="Q18" s="302" t="s">
         <v>150</v>
       </c>
-      <c r="R18" s="284"/>
+      <c r="R18" s="302"/>
       <c r="S18" s="142"/>
-      <c r="T18" s="299"/>
+      <c r="T18" s="297"/>
       <c r="U18" s="122"/>
       <c r="V18" s="105" t="s">
         <v>90</v>
@@ -24208,7 +24208,7 @@
         <v>87</v>
       </c>
       <c r="Y18" s="124"/>
-      <c r="Z18" s="300"/>
+      <c r="Z18" s="298"/>
       <c r="AA18" s="140"/>
       <c r="AB18" s="177" t="s">
         <v>86</v>
@@ -24235,9 +24235,9 @@
       <c r="AJ18" s="171" t="s">
         <v>86</v>
       </c>
-      <c r="AL18" s="281"/>
-      <c r="AM18" s="281"/>
-      <c r="AN18" s="281"/>
+      <c r="AL18" s="299"/>
+      <c r="AM18" s="299"/>
+      <c r="AN18" s="299"/>
       <c r="AO18" s="19"/>
     </row>
     <row r="19" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -24247,9 +24247,9 @@
       <c r="C19" s="98" t="s">
         <v>111</v>
       </c>
-      <c r="D19" s="280"/>
-      <c r="E19" s="281"/>
-      <c r="F19" s="281"/>
+      <c r="D19" s="312"/>
+      <c r="E19" s="299"/>
+      <c r="F19" s="299"/>
       <c r="G19" s="79"/>
       <c r="H19" s="94" t="s">
         <v>113</v>
@@ -24257,9 +24257,9 @@
       <c r="I19" s="98" t="s">
         <v>120</v>
       </c>
-      <c r="J19" s="280"/>
-      <c r="K19" s="281"/>
-      <c r="L19" s="281"/>
+      <c r="J19" s="312"/>
+      <c r="K19" s="299"/>
+      <c r="L19" s="299"/>
       <c r="M19" s="32"/>
       <c r="N19" s="183" t="s">
         <v>76</v>
@@ -24275,7 +24275,7 @@
         <v>77</v>
       </c>
       <c r="S19" s="142"/>
-      <c r="T19" s="299"/>
+      <c r="T19" s="297"/>
       <c r="U19" s="122"/>
       <c r="V19" s="80" t="s">
         <v>97</v>
@@ -24285,7 +24285,7 @@
         <v>108</v>
       </c>
       <c r="Y19" s="124"/>
-      <c r="Z19" s="300"/>
+      <c r="Z19" s="298"/>
       <c r="AA19" s="140"/>
       <c r="AB19" s="178"/>
       <c r="AC19" s="170"/>
@@ -24313,9 +24313,9 @@
       <c r="C20" s="95" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="280"/>
-      <c r="E20" s="281"/>
-      <c r="F20" s="281"/>
+      <c r="D20" s="312"/>
+      <c r="E20" s="299"/>
+      <c r="F20" s="299"/>
       <c r="G20" s="79"/>
       <c r="H20" s="99" t="s">
         <v>123</v>
@@ -24323,9 +24323,9 @@
       <c r="I20" s="95" t="s">
         <v>118</v>
       </c>
-      <c r="J20" s="280"/>
-      <c r="K20" s="281"/>
-      <c r="L20" s="281"/>
+      <c r="J20" s="312"/>
+      <c r="K20" s="299"/>
+      <c r="L20" s="299"/>
       <c r="M20" s="32"/>
       <c r="N20" s="112" t="s">
         <v>82</v>
@@ -24341,7 +24341,7 @@
         <v>84</v>
       </c>
       <c r="S20" s="142"/>
-      <c r="T20" s="299"/>
+      <c r="T20" s="297"/>
       <c r="U20" s="122"/>
       <c r="V20" s="105" t="s">
         <v>100</v>
@@ -24351,7 +24351,7 @@
         <v>98</v>
       </c>
       <c r="Y20" s="124"/>
-      <c r="Z20" s="300"/>
+      <c r="Z20" s="298"/>
       <c r="AA20" s="140"/>
       <c r="AB20" s="264"/>
       <c r="AC20" s="260"/>
@@ -24370,11 +24370,11 @@
       <c r="AJ20" s="175" t="s">
         <v>92</v>
       </c>
-      <c r="AL20" s="281" t="s">
+      <c r="AL20" s="299" t="s">
         <v>131</v>
       </c>
-      <c r="AM20" s="281"/>
-      <c r="AN20" s="281"/>
+      <c r="AM20" s="299"/>
+      <c r="AN20" s="299"/>
       <c r="AO20" s="19"/>
     </row>
     <row r="21" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -24384,9 +24384,9 @@
       <c r="C21" s="98" t="s">
         <v>109</v>
       </c>
-      <c r="D21" s="280"/>
-      <c r="E21" s="281"/>
-      <c r="F21" s="281"/>
+      <c r="D21" s="312"/>
+      <c r="E21" s="299"/>
+      <c r="F21" s="299"/>
       <c r="G21" s="79"/>
       <c r="H21" s="94" t="s">
         <v>121</v>
@@ -24394,9 +24394,9 @@
       <c r="I21" s="98" t="s">
         <v>94</v>
       </c>
-      <c r="J21" s="280"/>
-      <c r="K21" s="281"/>
-      <c r="L21" s="281"/>
+      <c r="J21" s="312"/>
+      <c r="K21" s="299"/>
+      <c r="L21" s="299"/>
       <c r="N21" s="83" t="s">
         <v>91</v>
       </c>
@@ -24410,7 +24410,7 @@
         <v>101</v>
       </c>
       <c r="S21" s="142"/>
-      <c r="T21" s="299"/>
+      <c r="T21" s="297"/>
       <c r="U21" s="122"/>
       <c r="V21" s="80" t="s">
         <v>109</v>
@@ -24420,7 +24420,7 @@
         <v>117</v>
       </c>
       <c r="Y21" s="124"/>
-      <c r="Z21" s="300"/>
+      <c r="Z21" s="298"/>
       <c r="AA21" s="140"/>
       <c r="AB21" s="173" t="s">
         <v>103</v>
@@ -24459,9 +24459,9 @@
       <c r="C22" s="95" t="s">
         <v>132</v>
       </c>
-      <c r="D22" s="280"/>
-      <c r="E22" s="281"/>
-      <c r="F22" s="281"/>
+      <c r="D22" s="312"/>
+      <c r="E22" s="299"/>
+      <c r="F22" s="299"/>
       <c r="G22" s="79"/>
       <c r="H22" s="99" t="s">
         <v>127</v>
@@ -24469,9 +24469,9 @@
       <c r="I22" s="95" t="s">
         <v>124</v>
       </c>
-      <c r="J22" s="280"/>
-      <c r="K22" s="281"/>
-      <c r="L22" s="281"/>
+      <c r="J22" s="312"/>
+      <c r="K22" s="299"/>
+      <c r="L22" s="299"/>
       <c r="N22" s="106" t="s">
         <v>93</v>
       </c>
@@ -24485,7 +24485,7 @@
         <v>95</v>
       </c>
       <c r="S22" s="143"/>
-      <c r="T22" s="299"/>
+      <c r="T22" s="297"/>
       <c r="U22" s="122"/>
       <c r="V22" s="105" t="s">
         <v>111</v>
@@ -24495,7 +24495,7 @@
         <v>110</v>
       </c>
       <c r="Y22" s="124"/>
-      <c r="Z22" s="300"/>
+      <c r="Z22" s="298"/>
       <c r="AA22" s="140"/>
       <c r="AB22" s="248"/>
       <c r="AC22" s="248"/>
@@ -24506,10 +24506,10 @@
       <c r="AH22" s="248"/>
       <c r="AI22" s="248"/>
       <c r="AJ22" s="248"/>
-      <c r="AL22" s="281" t="s">
+      <c r="AL22" s="299" t="s">
         <v>133</v>
       </c>
-      <c r="AM22" s="281"/>
+      <c r="AM22" s="299"/>
       <c r="AN22" s="88" t="s">
         <v>134</v>
       </c>
@@ -24522,9 +24522,9 @@
       <c r="C23" s="100" t="s">
         <v>112</v>
       </c>
-      <c r="D23" s="280"/>
-      <c r="E23" s="281"/>
-      <c r="F23" s="281"/>
+      <c r="D23" s="312"/>
+      <c r="E23" s="299"/>
+      <c r="F23" s="299"/>
       <c r="G23" s="79"/>
       <c r="H23" s="96" t="s">
         <v>126</v>
@@ -24532,9 +24532,9 @@
       <c r="I23" s="100" t="s">
         <v>128</v>
       </c>
-      <c r="J23" s="280"/>
-      <c r="K23" s="281"/>
-      <c r="L23" s="281"/>
+      <c r="J23" s="312"/>
+      <c r="K23" s="299"/>
+      <c r="L23" s="299"/>
       <c r="N23" s="83" t="s">
         <v>102</v>
       </c>
@@ -24547,7 +24547,7 @@
       <c r="R23" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="T23" s="299"/>
+      <c r="T23" s="297"/>
       <c r="U23" s="122"/>
       <c r="V23" s="80" t="s">
         <v>118</v>
@@ -24557,7 +24557,7 @@
         <v>123</v>
       </c>
       <c r="Y23" s="124"/>
-      <c r="Z23" s="300"/>
+      <c r="Z23" s="298"/>
       <c r="AA23" s="140"/>
       <c r="AB23" s="172" t="s">
         <v>86</v>
@@ -24584,10 +24584,10 @@
       <c r="AJ23" s="175" t="s">
         <v>86</v>
       </c>
-      <c r="AL23" s="281" t="s">
+      <c r="AL23" s="299" t="s">
         <v>135</v>
       </c>
-      <c r="AM23" s="281"/>
+      <c r="AM23" s="299"/>
       <c r="AN23" s="88" t="s">
         <v>134</v>
       </c>
@@ -24610,7 +24610,7 @@
         <v>106</v>
       </c>
       <c r="S24" s="19"/>
-      <c r="T24" s="299"/>
+      <c r="T24" s="297"/>
       <c r="U24" s="122"/>
       <c r="V24" s="105" t="s">
         <v>115</v>
@@ -24620,7 +24620,7 @@
         <v>119</v>
       </c>
       <c r="Y24" s="124"/>
-      <c r="Z24" s="300"/>
+      <c r="Z24" s="298"/>
       <c r="AA24" s="140"/>
       <c r="AB24" s="173"/>
       <c r="AC24" s="165"/>
@@ -24639,10 +24639,10 @@
       <c r="AJ24" s="259" t="s">
         <v>92</v>
       </c>
-      <c r="AL24" s="281" t="s">
+      <c r="AL24" s="299" t="s">
         <v>139</v>
       </c>
-      <c r="AM24" s="281"/>
+      <c r="AM24" s="299"/>
       <c r="AN24" s="88" t="s">
         <v>134</v>
       </c>
@@ -24653,13 +24653,13 @@
       <c r="D25" s="32"/>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
-      <c r="H25" s="295" t="s">
+      <c r="H25" s="300" t="s">
         <v>159</v>
       </c>
-      <c r="I25" s="295"/>
-      <c r="J25" s="295"/>
-      <c r="K25" s="295"/>
-      <c r="L25" s="295"/>
+      <c r="I25" s="300"/>
+      <c r="J25" s="300"/>
+      <c r="K25" s="300"/>
+      <c r="L25" s="300"/>
       <c r="N25" s="83" t="s">
         <v>113</v>
       </c>
@@ -24673,7 +24673,7 @@
         <v>120</v>
       </c>
       <c r="S25" s="19"/>
-      <c r="T25" s="299"/>
+      <c r="T25" s="297"/>
       <c r="U25" s="122"/>
       <c r="V25" s="80" t="s">
         <v>124</v>
@@ -24683,7 +24683,7 @@
         <v>127</v>
       </c>
       <c r="Y25" s="124"/>
-      <c r="Z25" s="300"/>
+      <c r="Z25" s="298"/>
       <c r="AA25" s="140"/>
       <c r="AB25" s="258"/>
       <c r="AC25" s="261"/>
@@ -24710,19 +24710,19 @@
       <c r="B26" s="90" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="285" t="s">
+      <c r="C26" s="303" t="s">
         <v>137</v>
       </c>
-      <c r="D26" s="286"/>
-      <c r="E26" s="285" t="s">
+      <c r="D26" s="304"/>
+      <c r="E26" s="303" t="s">
         <v>138</v>
       </c>
-      <c r="F26" s="287"/>
-      <c r="H26" s="295"/>
-      <c r="I26" s="295"/>
-      <c r="J26" s="295"/>
-      <c r="K26" s="295"/>
-      <c r="L26" s="295"/>
+      <c r="F26" s="305"/>
+      <c r="H26" s="300"/>
+      <c r="I26" s="300"/>
+      <c r="J26" s="300"/>
+      <c r="K26" s="300"/>
+      <c r="L26" s="300"/>
       <c r="N26" s="106" t="s">
         <v>114</v>
       </c>
@@ -24736,7 +24736,7 @@
         <v>83</v>
       </c>
       <c r="S26" s="19"/>
-      <c r="T26" s="299"/>
+      <c r="T26" s="297"/>
       <c r="U26" s="135"/>
       <c r="V26" s="111" t="s">
         <v>88</v>
@@ -24746,7 +24746,7 @@
         <v>125</v>
       </c>
       <c r="Y26" s="129"/>
-      <c r="Z26" s="300"/>
+      <c r="Z26" s="298"/>
       <c r="AA26" s="140"/>
       <c r="AB26" s="178" t="s">
         <v>103</v>
@@ -24781,19 +24781,19 @@
       <c r="B27" s="91" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="288">
+      <c r="C27" s="306">
         <v>0.8</v>
       </c>
-      <c r="D27" s="289"/>
-      <c r="E27" s="288">
+      <c r="D27" s="307"/>
+      <c r="E27" s="306">
         <v>100</v>
       </c>
-      <c r="F27" s="290"/>
-      <c r="H27" s="295"/>
-      <c r="I27" s="295"/>
-      <c r="J27" s="295"/>
-      <c r="K27" s="295"/>
-      <c r="L27" s="295"/>
+      <c r="F27" s="308"/>
+      <c r="H27" s="300"/>
+      <c r="I27" s="300"/>
+      <c r="J27" s="300"/>
+      <c r="K27" s="300"/>
+      <c r="L27" s="300"/>
       <c r="N27" s="83" t="s">
         <v>121</v>
       </c>
@@ -24822,19 +24822,19 @@
       <c r="B28" s="92" t="s">
         <v>141</v>
       </c>
-      <c r="C28" s="291">
+      <c r="C28" s="309">
         <v>1</v>
       </c>
-      <c r="D28" s="292"/>
-      <c r="E28" s="291">
+      <c r="D28" s="310"/>
+      <c r="E28" s="309">
         <v>180</v>
       </c>
-      <c r="F28" s="293"/>
-      <c r="H28" s="295"/>
-      <c r="I28" s="295"/>
-      <c r="J28" s="295"/>
-      <c r="K28" s="295"/>
-      <c r="L28" s="295"/>
+      <c r="F28" s="311"/>
+      <c r="H28" s="300"/>
+      <c r="I28" s="300"/>
+      <c r="J28" s="300"/>
+      <c r="K28" s="300"/>
+      <c r="L28" s="300"/>
       <c r="N28" s="106" t="s">
         <v>122</v>
       </c>
@@ -24848,25 +24848,25 @@
         <v>105</v>
       </c>
       <c r="U28" s="101"/>
-      <c r="V28" s="297" t="s">
+      <c r="V28" s="295" t="s">
         <v>81</v>
       </c>
-      <c r="W28" s="297"/>
-      <c r="X28" s="297"/>
+      <c r="W28" s="295"/>
+      <c r="X28" s="295"/>
     </row>
     <row r="29" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="283" t="s">
+      <c r="B29" s="301" t="s">
         <v>142</v>
       </c>
-      <c r="C29" s="283"/>
-      <c r="D29" s="283"/>
-      <c r="E29" s="283"/>
-      <c r="F29" s="283"/>
-      <c r="H29" s="295"/>
-      <c r="I29" s="295"/>
-      <c r="J29" s="295"/>
-      <c r="K29" s="295"/>
-      <c r="L29" s="295"/>
+      <c r="C29" s="301"/>
+      <c r="D29" s="301"/>
+      <c r="E29" s="301"/>
+      <c r="F29" s="301"/>
+      <c r="H29" s="300"/>
+      <c r="I29" s="300"/>
+      <c r="J29" s="300"/>
+      <c r="K29" s="300"/>
+      <c r="L29" s="300"/>
       <c r="N29" s="85" t="s">
         <v>126</v>
       </c>
@@ -24922,18 +24922,11 @@
     <row r="41" spans="19:19" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="AL3:AN3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="V28:X28"/>
-    <mergeCell ref="T5:T26"/>
-    <mergeCell ref="Z5:Z26"/>
-    <mergeCell ref="AL24:AM24"/>
-    <mergeCell ref="AL14:AN18"/>
-    <mergeCell ref="AL20:AN20"/>
-    <mergeCell ref="AL22:AM22"/>
-    <mergeCell ref="AL23:AM23"/>
-    <mergeCell ref="AL4:AN12"/>
-    <mergeCell ref="AB3:AJ3"/>
+    <mergeCell ref="D3:F4"/>
+    <mergeCell ref="J3:L7"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="D5:F5"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="N18:O18"/>
     <mergeCell ref="Q18:R18"/>
@@ -24947,13 +24940,20 @@
     <mergeCell ref="J8:L8"/>
     <mergeCell ref="J10:L23"/>
     <mergeCell ref="H25:L29"/>
+    <mergeCell ref="AL3:AN3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="V28:X28"/>
+    <mergeCell ref="T5:T26"/>
+    <mergeCell ref="Z5:Z26"/>
+    <mergeCell ref="AL24:AM24"/>
+    <mergeCell ref="AL14:AN18"/>
+    <mergeCell ref="AL20:AN20"/>
+    <mergeCell ref="AL22:AM22"/>
+    <mergeCell ref="AL23:AM23"/>
+    <mergeCell ref="AL4:AN12"/>
+    <mergeCell ref="AB3:AJ3"/>
     <mergeCell ref="AB17:AJ17"/>
     <mergeCell ref="AB5:AJ5"/>
-    <mergeCell ref="D3:F4"/>
-    <mergeCell ref="J3:L7"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="D5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -24984,27 +24984,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:29" ht="16" x14ac:dyDescent="0.35">
-      <c r="B2" s="307" t="s">
+      <c r="B2" s="325" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="307"/>
-      <c r="D2" s="307"/>
-      <c r="E2" s="307"/>
-      <c r="F2" s="307"/>
-      <c r="N2" s="308" t="s">
+      <c r="C2" s="325"/>
+      <c r="D2" s="325"/>
+      <c r="E2" s="325"/>
+      <c r="F2" s="325"/>
+      <c r="N2" s="326" t="s">
         <v>182</v>
       </c>
-      <c r="O2" s="308"/>
-      <c r="P2" s="308"/>
-      <c r="Q2" s="308"/>
-      <c r="R2" s="308"/>
-      <c r="T2" s="308" t="s">
+      <c r="O2" s="326"/>
+      <c r="P2" s="326"/>
+      <c r="Q2" s="326"/>
+      <c r="R2" s="326"/>
+      <c r="T2" s="326" t="s">
         <v>181</v>
       </c>
-      <c r="U2" s="308"/>
-      <c r="V2" s="308"/>
-      <c r="W2" s="308"/>
-      <c r="X2" s="308"/>
+      <c r="U2" s="326"/>
+      <c r="V2" s="326"/>
+      <c r="W2" s="326"/>
+      <c r="X2" s="326"/>
     </row>
     <row r="3" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H3" s="38" t="s">
@@ -25013,34 +25013,34 @@
       <c r="I3" s="1">
         <v>20</v>
       </c>
-      <c r="N3" s="310" t="s">
+      <c r="N3" s="328" t="s">
         <v>185</v>
       </c>
-      <c r="O3" s="310"/>
-      <c r="P3" s="310"/>
-      <c r="Q3" s="310"/>
-      <c r="R3" s="310"/>
-      <c r="T3" s="310" t="s">
+      <c r="O3" s="328"/>
+      <c r="P3" s="328"/>
+      <c r="Q3" s="328"/>
+      <c r="R3" s="328"/>
+      <c r="T3" s="328" t="s">
         <v>186</v>
       </c>
-      <c r="U3" s="310"/>
-      <c r="V3" s="310"/>
-      <c r="W3" s="310"/>
-      <c r="X3" s="310"/>
-      <c r="Z3" s="281" t="s">
+      <c r="U3" s="328"/>
+      <c r="V3" s="328"/>
+      <c r="W3" s="328"/>
+      <c r="X3" s="328"/>
+      <c r="Z3" s="299" t="s">
         <v>34</v>
       </c>
-      <c r="AA3" s="281"/>
-      <c r="AB3" s="281"/>
+      <c r="AA3" s="299"/>
+      <c r="AB3" s="299"/>
     </row>
     <row r="4" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="40"/>
-      <c r="C4" s="309" t="s">
+      <c r="C4" s="327" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="302"/>
-      <c r="E4" s="302"/>
-      <c r="F4" s="302"/>
+      <c r="D4" s="323"/>
+      <c r="E4" s="323"/>
+      <c r="F4" s="323"/>
       <c r="H4" s="1" t="s">
         <v>4</v>
       </c>
@@ -25057,9 +25057,9 @@
       <c r="V4" s="31"/>
       <c r="W4" s="31"/>
       <c r="X4" s="37"/>
-      <c r="Z4" s="281"/>
-      <c r="AA4" s="281"/>
-      <c r="AB4" s="281"/>
+      <c r="Z4" s="299"/>
+      <c r="AA4" s="299"/>
+      <c r="AB4" s="299"/>
     </row>
     <row r="5" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H5" s="1" t="s">
@@ -25078,46 +25078,46 @@
       <c r="V5" s="249"/>
       <c r="W5" s="249"/>
       <c r="X5" s="249"/>
-      <c r="Z5" s="281"/>
-      <c r="AA5" s="281"/>
-      <c r="AB5" s="281"/>
+      <c r="Z5" s="299"/>
+      <c r="AA5" s="299"/>
+      <c r="AB5" s="299"/>
       <c r="AC5" s="32"/>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="302" t="s">
+      <c r="C6" s="323" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="302"/>
-      <c r="E6" s="302"/>
-      <c r="F6" s="302"/>
+      <c r="D6" s="323"/>
+      <c r="E6" s="323"/>
+      <c r="F6" s="323"/>
       <c r="H6" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I6" s="1">
         <v>20</v>
       </c>
-      <c r="N6" s="303" t="s">
+      <c r="N6" s="321" t="s">
         <v>36</v>
       </c>
-      <c r="O6" s="304"/>
+      <c r="O6" s="322"/>
       <c r="P6" s="249"/>
-      <c r="Q6" s="303" t="s">
+      <c r="Q6" s="321" t="s">
         <v>36</v>
       </c>
-      <c r="R6" s="304"/>
+      <c r="R6" s="322"/>
       <c r="S6" s="249"/>
-      <c r="T6" s="303" t="s">
+      <c r="T6" s="321" t="s">
         <v>37</v>
       </c>
-      <c r="U6" s="304"/>
+      <c r="U6" s="322"/>
       <c r="V6" s="249"/>
-      <c r="W6" s="303" t="s">
+      <c r="W6" s="321" t="s">
         <v>37</v>
       </c>
-      <c r="X6" s="304"/>
+      <c r="X6" s="322"/>
       <c r="Z6" s="32"/>
       <c r="AA6" s="32"/>
       <c r="AB6" s="32"/>
@@ -25136,22 +25136,22 @@
       <c r="V7" s="249"/>
       <c r="W7" s="249"/>
       <c r="X7" s="249"/>
-      <c r="Z7" s="281" t="s">
+      <c r="Z7" s="299" t="s">
         <v>44</v>
       </c>
-      <c r="AA7" s="281"/>
-      <c r="AB7" s="281"/>
+      <c r="AA7" s="299"/>
+      <c r="AB7" s="299"/>
     </row>
     <row r="8" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="302" t="s">
+      <c r="C8" s="323" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="302"/>
-      <c r="E8" s="302"/>
-      <c r="F8" s="302"/>
+      <c r="D8" s="323"/>
+      <c r="E8" s="323"/>
+      <c r="F8" s="323"/>
       <c r="N8" s="44" t="s">
         <v>43</v>
       </c>
@@ -25179,9 +25179,9 @@
       <c r="X8" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="Z8" s="281"/>
-      <c r="AA8" s="281"/>
-      <c r="AB8" s="281"/>
+      <c r="Z8" s="299"/>
+      <c r="AA8" s="299"/>
+      <c r="AB8" s="299"/>
     </row>
     <row r="9" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="N9" s="249"/>
@@ -25195,20 +25195,20 @@
       <c r="V9" s="249"/>
       <c r="W9" s="249"/>
       <c r="X9" s="249"/>
-      <c r="Z9" s="281"/>
-      <c r="AA9" s="281"/>
-      <c r="AB9" s="281"/>
+      <c r="Z9" s="299"/>
+      <c r="AA9" s="299"/>
+      <c r="AB9" s="299"/>
     </row>
     <row r="10" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="302" t="s">
+      <c r="C10" s="323" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="302"/>
-      <c r="E10" s="302"/>
-      <c r="F10" s="302"/>
+      <c r="D10" s="323"/>
+      <c r="E10" s="323"/>
+      <c r="F10" s="323"/>
       <c r="N10" s="48" t="s">
         <v>46</v>
       </c>
@@ -25241,39 +25241,39 @@
       <c r="AB10" s="52"/>
     </row>
     <row r="11" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N11" s="282" t="s">
+      <c r="N11" s="314" t="s">
         <v>62</v>
       </c>
-      <c r="O11" s="282"/>
+      <c r="O11" s="314"/>
       <c r="P11" s="249"/>
-      <c r="Q11" s="282" t="s">
+      <c r="Q11" s="314" t="s">
         <v>62</v>
       </c>
-      <c r="R11" s="282"/>
+      <c r="R11" s="314"/>
       <c r="S11" s="249"/>
-      <c r="T11" s="302" t="s">
+      <c r="T11" s="323" t="s">
         <v>50</v>
       </c>
-      <c r="U11" s="302"/>
+      <c r="U11" s="323"/>
       <c r="V11" s="249"/>
-      <c r="W11" s="302" t="s">
+      <c r="W11" s="323" t="s">
         <v>50</v>
       </c>
-      <c r="X11" s="302"/>
-      <c r="Z11" s="281" t="s">
+      <c r="X11" s="323"/>
+      <c r="Z11" s="299" t="s">
         <v>51</v>
       </c>
-      <c r="AA11" s="281"/>
-      <c r="AB11" s="281"/>
+      <c r="AA11" s="299"/>
+      <c r="AB11" s="299"/>
     </row>
     <row r="12" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="311" t="s">
+      <c r="B12" s="324" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="311"/>
-      <c r="D12" s="311"/>
-      <c r="E12" s="311"/>
-      <c r="F12" s="311"/>
+      <c r="C12" s="324"/>
+      <c r="D12" s="324"/>
+      <c r="E12" s="324"/>
+      <c r="F12" s="324"/>
       <c r="N12" s="54" t="s">
         <v>47</v>
       </c>
@@ -25301,49 +25301,49 @@
       <c r="X12" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="Z12" s="281"/>
-      <c r="AA12" s="281"/>
-      <c r="AB12" s="281"/>
+      <c r="Z12" s="299"/>
+      <c r="AA12" s="299"/>
+      <c r="AB12" s="299"/>
     </row>
     <row r="13" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N13" s="282" t="s">
+      <c r="N13" s="314" t="s">
         <v>65</v>
       </c>
-      <c r="O13" s="282"/>
+      <c r="O13" s="314"/>
       <c r="P13" s="249"/>
-      <c r="Q13" s="282" t="s">
+      <c r="Q13" s="314" t="s">
         <v>65</v>
       </c>
-      <c r="R13" s="282"/>
+      <c r="R13" s="314"/>
       <c r="S13" s="249"/>
-      <c r="T13" s="282" t="s">
+      <c r="T13" s="314" t="s">
         <v>54</v>
       </c>
-      <c r="U13" s="282"/>
+      <c r="U13" s="314"/>
       <c r="V13" s="249"/>
-      <c r="W13" s="282" t="s">
+      <c r="W13" s="314" t="s">
         <v>54</v>
       </c>
-      <c r="X13" s="282"/>
-      <c r="Z13" s="281"/>
-      <c r="AA13" s="281"/>
-      <c r="AB13" s="281"/>
+      <c r="X13" s="314"/>
+      <c r="Z13" s="299"/>
+      <c r="AA13" s="299"/>
+      <c r="AB13" s="299"/>
     </row>
     <row r="14" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="312" t="s">
+      <c r="B14" s="319" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="312"/>
-      <c r="D14" s="312"/>
-      <c r="E14" s="312"/>
-      <c r="F14" s="312"/>
-      <c r="H14" s="313" t="s">
+      <c r="C14" s="319"/>
+      <c r="D14" s="319"/>
+      <c r="E14" s="319"/>
+      <c r="F14" s="319"/>
+      <c r="H14" s="320" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="313"/>
-      <c r="J14" s="313"/>
-      <c r="K14" s="313"/>
-      <c r="L14" s="313"/>
+      <c r="I14" s="320"/>
+      <c r="J14" s="320"/>
+      <c r="K14" s="320"/>
+      <c r="L14" s="320"/>
       <c r="N14" s="58" t="s">
         <v>184</v>
       </c>
@@ -25373,33 +25373,33 @@
       </c>
     </row>
     <row r="15" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N15" s="302" t="s">
+      <c r="N15" s="323" t="s">
         <v>69</v>
       </c>
-      <c r="O15" s="302"/>
+      <c r="O15" s="323"/>
       <c r="P15" s="249"/>
-      <c r="Q15" s="302" t="s">
+      <c r="Q15" s="323" t="s">
         <v>69</v>
       </c>
-      <c r="R15" s="302"/>
+      <c r="R15" s="323"/>
       <c r="S15" s="249"/>
-      <c r="T15" s="282" t="s">
+      <c r="T15" s="314" t="s">
         <v>55</v>
       </c>
-      <c r="U15" s="282"/>
+      <c r="U15" s="314"/>
       <c r="V15" s="249"/>
-      <c r="W15" s="282" t="s">
+      <c r="W15" s="314" t="s">
         <v>55</v>
       </c>
-      <c r="X15" s="282"/>
-      <c r="Z15" s="281" t="s">
+      <c r="X15" s="314"/>
+      <c r="Z15" s="299" t="s">
         <v>57</v>
       </c>
-      <c r="AA15" s="281"/>
-      <c r="AB15" s="281"/>
+      <c r="AA15" s="299"/>
+      <c r="AB15" s="299"/>
     </row>
     <row r="16" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="314">
+      <c r="A16" s="315">
         <v>1</v>
       </c>
       <c r="B16" s="59" t="s">
@@ -25408,7 +25408,7 @@
       <c r="C16" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="315">
+      <c r="D16" s="316">
         <v>3</v>
       </c>
       <c r="E16" s="59" t="s">
@@ -25417,7 +25417,7 @@
       <c r="F16" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="314">
+      <c r="G16" s="315">
         <v>1</v>
       </c>
       <c r="H16" s="61" t="s">
@@ -25426,7 +25426,7 @@
       <c r="I16" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="315">
+      <c r="J16" s="316">
         <v>3</v>
       </c>
       <c r="K16" s="61" t="s">
@@ -25446,61 +25446,61 @@
       <c r="V16" s="249"/>
       <c r="W16" s="249"/>
       <c r="X16" s="249"/>
-      <c r="Z16" s="281"/>
-      <c r="AA16" s="281"/>
-      <c r="AB16" s="281"/>
+      <c r="Z16" s="299"/>
+      <c r="AA16" s="299"/>
+      <c r="AB16" s="299"/>
     </row>
     <row r="17" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="314"/>
+      <c r="A17" s="315"/>
       <c r="B17" s="63" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="315"/>
+      <c r="D17" s="316"/>
       <c r="E17" s="63" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="314"/>
+      <c r="G17" s="315"/>
       <c r="H17" s="65" t="s">
         <v>16</v>
       </c>
       <c r="I17" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="315"/>
+      <c r="J17" s="316"/>
       <c r="K17" s="65" t="s">
         <v>15</v>
       </c>
       <c r="L17" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="N17" s="303" t="s">
+      <c r="N17" s="321" t="s">
         <v>58</v>
       </c>
-      <c r="O17" s="304"/>
+      <c r="O17" s="322"/>
       <c r="P17" s="41"/>
-      <c r="Q17" s="303" t="s">
+      <c r="Q17" s="321" t="s">
         <v>58</v>
       </c>
-      <c r="R17" s="304"/>
+      <c r="R17" s="322"/>
       <c r="S17" s="249"/>
-      <c r="T17" s="303" t="s">
+      <c r="T17" s="321" t="s">
         <v>59</v>
       </c>
-      <c r="U17" s="304"/>
+      <c r="U17" s="322"/>
       <c r="V17" s="41"/>
-      <c r="W17" s="303" t="s">
+      <c r="W17" s="321" t="s">
         <v>59</v>
       </c>
-      <c r="X17" s="304"/>
-      <c r="Z17" s="281"/>
-      <c r="AA17" s="281"/>
-      <c r="AB17" s="281"/>
+      <c r="X17" s="322"/>
+      <c r="Z17" s="299"/>
+      <c r="AA17" s="299"/>
+      <c r="AB17" s="299"/>
     </row>
     <row r="18" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="N18" s="249"/>
@@ -25516,7 +25516,7 @@
       <c r="X18" s="249"/>
     </row>
     <row r="19" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="314">
+      <c r="A19" s="315">
         <v>2</v>
       </c>
       <c r="B19" s="59" t="s">
@@ -25525,7 +25525,7 @@
       <c r="C19" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="315">
+      <c r="D19" s="316">
         <v>4</v>
       </c>
       <c r="E19" s="59" t="s">
@@ -25534,7 +25534,7 @@
       <c r="F19" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="314">
+      <c r="G19" s="315">
         <v>2</v>
       </c>
       <c r="H19" s="61" t="s">
@@ -25543,7 +25543,7 @@
       <c r="I19" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="J19" s="315">
+      <c r="J19" s="316">
         <v>4</v>
       </c>
       <c r="K19" s="61" t="s">
@@ -25579,35 +25579,35 @@
       <c r="X19" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="Z19" s="281" t="s">
+      <c r="Z19" s="299" t="s">
         <v>61</v>
       </c>
-      <c r="AA19" s="281"/>
-      <c r="AB19" s="281"/>
+      <c r="AA19" s="299"/>
+      <c r="AB19" s="299"/>
     </row>
     <row r="20" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="314"/>
+      <c r="A20" s="315"/>
       <c r="B20" s="63" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="315"/>
+      <c r="D20" s="316"/>
       <c r="E20" s="63" t="s">
         <v>15</v>
       </c>
       <c r="F20" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="314"/>
+      <c r="G20" s="315"/>
       <c r="H20" s="65" t="s">
         <v>16</v>
       </c>
       <c r="I20" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="315"/>
+      <c r="J20" s="316"/>
       <c r="K20" s="65" t="s">
         <v>15</v>
       </c>
@@ -25625,9 +25625,9 @@
       <c r="V20" s="249"/>
       <c r="W20" s="249"/>
       <c r="X20" s="249"/>
-      <c r="Z20" s="281"/>
-      <c r="AA20" s="281"/>
-      <c r="AB20" s="281"/>
+      <c r="Z20" s="299"/>
+      <c r="AA20" s="299"/>
+      <c r="AB20" s="299"/>
     </row>
     <row r="21" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="N21" s="49" t="s">
@@ -25657,46 +25657,46 @@
       <c r="X21" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="Z21" s="281"/>
-      <c r="AA21" s="281"/>
-      <c r="AB21" s="281"/>
+      <c r="Z21" s="299"/>
+      <c r="AA21" s="299"/>
+      <c r="AB21" s="299"/>
     </row>
     <row r="22" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N22" s="301" t="s">
+      <c r="N22" s="331" t="s">
         <v>49</v>
       </c>
-      <c r="O22" s="301"/>
+      <c r="O22" s="331"/>
       <c r="P22" s="249"/>
-      <c r="Q22" s="301" t="s">
+      <c r="Q22" s="331" t="s">
         <v>49</v>
       </c>
-      <c r="R22" s="301"/>
+      <c r="R22" s="331"/>
       <c r="S22" s="249"/>
-      <c r="T22" s="301" t="s">
+      <c r="T22" s="331" t="s">
         <v>63</v>
       </c>
-      <c r="U22" s="301"/>
+      <c r="U22" s="331"/>
       <c r="V22" s="249"/>
-      <c r="W22" s="301" t="s">
+      <c r="W22" s="331" t="s">
         <v>63</v>
       </c>
-      <c r="X22" s="301"/>
+      <c r="X22" s="331"/>
     </row>
     <row r="23" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="317" t="s">
+      <c r="B23" s="318" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="317"/>
-      <c r="D23" s="317"/>
-      <c r="E23" s="317"/>
-      <c r="F23" s="317"/>
-      <c r="H23" s="281" t="s">
+      <c r="C23" s="318"/>
+      <c r="D23" s="318"/>
+      <c r="E23" s="318"/>
+      <c r="F23" s="318"/>
+      <c r="H23" s="299" t="s">
         <v>64</v>
       </c>
-      <c r="I23" s="281"/>
-      <c r="J23" s="281"/>
-      <c r="K23" s="281"/>
-      <c r="L23" s="281"/>
+      <c r="I23" s="299"/>
+      <c r="J23" s="299"/>
+      <c r="K23" s="299"/>
+      <c r="L23" s="299"/>
       <c r="N23" s="53" t="s">
         <v>48</v>
       </c>
@@ -25724,43 +25724,43 @@
       <c r="X23" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="Z23" s="281" t="s">
+      <c r="Z23" s="299" t="s">
         <v>67</v>
       </c>
-      <c r="AA23" s="281"/>
-      <c r="AB23" s="281"/>
+      <c r="AA23" s="299"/>
+      <c r="AB23" s="299"/>
     </row>
     <row r="24" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H24" s="281"/>
-      <c r="I24" s="281"/>
-      <c r="J24" s="281"/>
-      <c r="K24" s="281"/>
-      <c r="L24" s="281"/>
-      <c r="N24" s="302" t="s">
+      <c r="H24" s="299"/>
+      <c r="I24" s="299"/>
+      <c r="J24" s="299"/>
+      <c r="K24" s="299"/>
+      <c r="L24" s="299"/>
+      <c r="N24" s="323" t="s">
         <v>53</v>
       </c>
-      <c r="O24" s="302"/>
+      <c r="O24" s="323"/>
       <c r="P24" s="249"/>
-      <c r="Q24" s="302" t="s">
+      <c r="Q24" s="323" t="s">
         <v>53</v>
       </c>
-      <c r="R24" s="302"/>
+      <c r="R24" s="323"/>
       <c r="S24" s="249"/>
-      <c r="T24" s="302" t="s">
+      <c r="T24" s="323" t="s">
         <v>66</v>
       </c>
-      <c r="U24" s="302"/>
+      <c r="U24" s="323"/>
       <c r="V24" s="249"/>
-      <c r="W24" s="302" t="s">
+      <c r="W24" s="323" t="s">
         <v>66</v>
       </c>
-      <c r="X24" s="302"/>
-      <c r="Z24" s="281"/>
-      <c r="AA24" s="281"/>
-      <c r="AB24" s="281"/>
+      <c r="X24" s="323"/>
+      <c r="Z24" s="299"/>
+      <c r="AA24" s="299"/>
+      <c r="AB24" s="299"/>
     </row>
     <row r="25" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="314">
+      <c r="A25" s="315">
         <v>1</v>
       </c>
       <c r="B25" s="67" t="s">
@@ -25769,7 +25769,7 @@
       <c r="C25" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="315">
+      <c r="D25" s="316">
         <v>3</v>
       </c>
       <c r="E25" s="67" t="s">
@@ -25778,11 +25778,11 @@
       <c r="F25" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="281"/>
-      <c r="I25" s="281"/>
-      <c r="J25" s="281"/>
-      <c r="K25" s="281"/>
-      <c r="L25" s="281"/>
+      <c r="H25" s="299"/>
+      <c r="I25" s="299"/>
+      <c r="J25" s="299"/>
+      <c r="K25" s="299"/>
+      <c r="L25" s="299"/>
       <c r="N25" s="56" t="s">
         <v>47</v>
       </c>
@@ -25810,56 +25810,56 @@
       <c r="X25" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="Z25" s="281"/>
-      <c r="AA25" s="281"/>
-      <c r="AB25" s="281"/>
+      <c r="Z25" s="299"/>
+      <c r="AA25" s="299"/>
+      <c r="AB25" s="299"/>
     </row>
     <row r="26" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="314"/>
+      <c r="A26" s="315"/>
       <c r="B26" s="69" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="315"/>
+      <c r="D26" s="316"/>
       <c r="E26" s="69" t="s">
         <v>15</v>
       </c>
       <c r="F26" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="281"/>
-      <c r="I26" s="281"/>
-      <c r="J26" s="281"/>
-      <c r="K26" s="281"/>
-      <c r="L26" s="281"/>
-      <c r="N26" s="302" t="s">
+      <c r="H26" s="299"/>
+      <c r="I26" s="299"/>
+      <c r="J26" s="299"/>
+      <c r="K26" s="299"/>
+      <c r="L26" s="299"/>
+      <c r="N26" s="323" t="s">
         <v>56</v>
       </c>
-      <c r="O26" s="302"/>
+      <c r="O26" s="323"/>
       <c r="P26" s="249"/>
-      <c r="Q26" s="302" t="s">
+      <c r="Q26" s="323" t="s">
         <v>56</v>
       </c>
-      <c r="R26" s="302"/>
+      <c r="R26" s="323"/>
       <c r="S26" s="249"/>
-      <c r="T26" s="302" t="s">
+      <c r="T26" s="323" t="s">
         <v>68</v>
       </c>
-      <c r="U26" s="302"/>
+      <c r="U26" s="323"/>
       <c r="V26" s="249"/>
-      <c r="W26" s="302" t="s">
+      <c r="W26" s="323" t="s">
         <v>68</v>
       </c>
-      <c r="X26" s="302"/>
+      <c r="X26" s="323"/>
     </row>
     <row r="27" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H27" s="281"/>
-      <c r="I27" s="281"/>
-      <c r="J27" s="281"/>
-      <c r="K27" s="281"/>
-      <c r="L27" s="281"/>
+      <c r="H27" s="299"/>
+      <c r="I27" s="299"/>
+      <c r="J27" s="299"/>
+      <c r="K27" s="299"/>
+      <c r="L27" s="299"/>
       <c r="N27" s="71"/>
       <c r="O27" s="250"/>
       <c r="P27" s="250"/>
@@ -25872,7 +25872,7 @@
       <c r="X27" s="36"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A28" s="314">
+      <c r="A28" s="315">
         <v>2</v>
       </c>
       <c r="B28" s="67" t="s">
@@ -25881,7 +25881,7 @@
       <c r="C28" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="315">
+      <c r="D28" s="316">
         <v>4</v>
       </c>
       <c r="E28" s="67" t="s">
@@ -25890,49 +25890,49 @@
       <c r="F28" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="281"/>
-      <c r="I28" s="281"/>
-      <c r="J28" s="281"/>
-      <c r="K28" s="281"/>
-      <c r="L28" s="281"/>
-      <c r="N28" s="305" t="s">
+      <c r="H28" s="299"/>
+      <c r="I28" s="299"/>
+      <c r="J28" s="299"/>
+      <c r="K28" s="299"/>
+      <c r="L28" s="299"/>
+      <c r="N28" s="329" t="s">
         <v>188</v>
       </c>
-      <c r="O28" s="305"/>
-      <c r="P28" s="305"/>
-      <c r="Q28" s="305"/>
-      <c r="R28" s="305"/>
+      <c r="O28" s="329"/>
+      <c r="P28" s="329"/>
+      <c r="Q28" s="329"/>
+      <c r="R28" s="329"/>
       <c r="S28" s="72"/>
-      <c r="T28" s="306" t="s">
+      <c r="T28" s="330" t="s">
         <v>187</v>
       </c>
-      <c r="U28" s="306"/>
-      <c r="V28" s="306"/>
-      <c r="W28" s="306"/>
-      <c r="X28" s="306"/>
+      <c r="U28" s="330"/>
+      <c r="V28" s="330"/>
+      <c r="W28" s="330"/>
+      <c r="X28" s="330"/>
     </row>
     <row r="29" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="314"/>
+      <c r="A29" s="315"/>
       <c r="B29" s="69" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="315"/>
+      <c r="D29" s="316"/>
       <c r="E29" s="69" t="s">
         <v>15</v>
       </c>
       <c r="F29" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="316" t="s">
+      <c r="H29" s="317" t="s">
         <v>70</v>
       </c>
-      <c r="I29" s="316"/>
-      <c r="J29" s="316"/>
-      <c r="K29" s="316"/>
-      <c r="L29" s="316"/>
+      <c r="I29" s="317"/>
+      <c r="J29" s="317"/>
+      <c r="K29" s="317"/>
+      <c r="L29" s="317"/>
       <c r="N29" s="73"/>
       <c r="O29" s="73"/>
       <c r="P29" s="72"/>
@@ -25963,26 +25963,26 @@
       <c r="V31" s="74"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="B32" s="351"/>
-      <c r="C32" s="349" t="s">
+      <c r="B32" s="276"/>
+      <c r="C32" s="274" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="349" t="s">
+      <c r="D32" s="274" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="350" t="s">
+      <c r="E32" s="275" t="s">
         <v>3</v>
       </c>
-      <c r="G32" s="352"/>
-      <c r="H32" s="349" t="s">
+      <c r="G32" s="277"/>
+      <c r="H32" s="274" t="s">
         <v>3</v>
       </c>
-      <c r="I32" s="350" t="s">
+      <c r="I32" s="275" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B33" s="353" t="s">
+      <c r="B33" s="278" t="s">
         <v>192</v>
       </c>
       <c r="C33" s="254" t="s">
@@ -25991,51 +25991,51 @@
       <c r="D33" s="254" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="341" t="s">
+      <c r="E33" s="266" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="353" t="s">
+      <c r="G33" s="278" t="s">
         <v>12</v>
       </c>
       <c r="H33" s="254" t="s">
         <v>199</v>
       </c>
-      <c r="I33" s="341" t="s">
+      <c r="I33" s="266" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B34" s="344"/>
+      <c r="B34" s="269"/>
       <c r="C34" s="254" t="s">
         <v>7</v>
       </c>
       <c r="D34" s="254" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="341" t="s">
+      <c r="E34" s="266" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="346"/>
+      <c r="G34" s="271"/>
       <c r="H34" s="18"/>
-      <c r="I34" s="347"/>
+      <c r="I34" s="272"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B35" s="346"/>
+      <c r="B35" s="271"/>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
-      <c r="E35" s="347"/>
-      <c r="G35" s="348" t="s">
+      <c r="E35" s="272"/>
+      <c r="G35" s="273" t="s">
         <v>13</v>
       </c>
       <c r="H35" s="254" t="s">
         <v>198</v>
       </c>
-      <c r="I35" s="341" t="s">
+      <c r="I35" s="266" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B36" s="348" t="s">
+      <c r="B36" s="273" t="s">
         <v>193</v>
       </c>
       <c r="C36" s="254" t="s">
@@ -26044,42 +26044,42 @@
       <c r="D36" s="254" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="341" t="s">
+      <c r="E36" s="266" t="s">
         <v>8</v>
       </c>
-      <c r="G36" s="346"/>
+      <c r="G36" s="271"/>
       <c r="H36" s="18"/>
-      <c r="I36" s="347"/>
+      <c r="I36" s="272"/>
     </row>
     <row r="37" spans="2:9" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="344"/>
+      <c r="B37" s="269"/>
       <c r="C37" s="254" t="s">
         <v>7</v>
       </c>
       <c r="D37" s="254" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="341" t="s">
+      <c r="E37" s="266" t="s">
         <v>9</v>
       </c>
-      <c r="G37" s="354" t="s">
+      <c r="G37" s="279" t="s">
         <v>14</v>
       </c>
-      <c r="H37" s="342" t="s">
+      <c r="H37" s="267" t="s">
         <v>198</v>
       </c>
-      <c r="I37" s="343" t="s">
+      <c r="I37" s="268" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B38" s="346"/>
+      <c r="B38" s="271"/>
       <c r="C38" s="18"/>
       <c r="D38" s="18"/>
-      <c r="E38" s="347"/>
+      <c r="E38" s="272"/>
     </row>
     <row r="39" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="348" t="s">
+      <c r="B39" s="273" t="s">
         <v>194</v>
       </c>
       <c r="C39" s="254" t="s">
@@ -26088,41 +26088,41 @@
       <c r="D39" s="254" t="s">
         <v>16</v>
       </c>
-      <c r="E39" s="341" t="s">
+      <c r="E39" s="266" t="s">
         <v>9</v>
       </c>
-      <c r="G39" s="281" t="s">
+      <c r="G39" s="299" t="s">
         <v>200</v>
       </c>
-      <c r="H39" s="281"/>
-      <c r="I39" s="281"/>
+      <c r="H39" s="299"/>
+      <c r="I39" s="299"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B40" s="344"/>
+      <c r="B40" s="269"/>
       <c r="C40" s="254" t="s">
         <v>7</v>
       </c>
       <c r="D40" s="254" t="s">
         <v>15</v>
       </c>
-      <c r="E40" s="341" t="s">
+      <c r="E40" s="266" t="s">
         <v>8</v>
       </c>
-      <c r="G40" s="281"/>
-      <c r="H40" s="281"/>
-      <c r="I40" s="281"/>
+      <c r="G40" s="299"/>
+      <c r="H40" s="299"/>
+      <c r="I40" s="299"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B41" s="346"/>
+      <c r="B41" s="271"/>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
-      <c r="E41" s="347"/>
+      <c r="E41" s="272"/>
       <c r="G41" s="32"/>
       <c r="H41" s="32"/>
       <c r="I41" s="32"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B42" s="348" t="s">
+      <c r="B42" s="273" t="s">
         <v>195</v>
       </c>
       <c r="C42" s="254" t="s">
@@ -26131,7 +26131,7 @@
       <c r="D42" s="254" t="s">
         <v>15</v>
       </c>
-      <c r="E42" s="341" t="s">
+      <c r="E42" s="266" t="s">
         <v>9</v>
       </c>
       <c r="G42" s="32"/>
@@ -26139,14 +26139,14 @@
       <c r="I42" s="32"/>
     </row>
     <row r="43" spans="2:9" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="345"/>
-      <c r="C43" s="342" t="s">
+      <c r="B43" s="270"/>
+      <c r="C43" s="267" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="342" t="s">
+      <c r="D43" s="267" t="s">
         <v>197</v>
       </c>
-      <c r="E43" s="343" t="s">
+      <c r="E43" s="268" t="s">
         <v>8</v>
       </c>
       <c r="G43" s="32"/>
@@ -26155,59 +26155,6 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="G39:I40"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="Z23:AB25"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="H23:L28"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="Z19:AB21"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="H14:L14"/>
-    <mergeCell ref="W13:X13"/>
-    <mergeCell ref="Z15:AB17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="W15:X15"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="W17:X17"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="Z7:AB9"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="Z11:AB13"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="T2:X2"/>
-    <mergeCell ref="Z3:AB5"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="T3:X3"/>
-    <mergeCell ref="N28:R28"/>
-    <mergeCell ref="T28:X28"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="T11:U11"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="T15:U15"/>
     <mergeCell ref="W11:X11"/>
     <mergeCell ref="N22:O22"/>
     <mergeCell ref="N17:O17"/>
@@ -26223,6 +26170,59 @@
     <mergeCell ref="W22:X22"/>
     <mergeCell ref="W24:X24"/>
     <mergeCell ref="W26:X26"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="Z3:AB5"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="T3:X3"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="Z7:AB9"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="Z11:AB13"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="Z15:AB17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="W17:X17"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="Z19:AB21"/>
+    <mergeCell ref="G39:I40"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="Z23:AB25"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="H23:L28"/>
+    <mergeCell ref="N28:R28"/>
+    <mergeCell ref="T28:X28"/>
   </mergeCells>
   <pageMargins left="2.56" right="2.15" top="0.75" bottom="0.75" header="0.61" footer="0.3"/>
   <pageSetup scale="32" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -26251,10 +26251,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B2" s="320" t="s">
+      <c r="B2" s="334" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="320"/>
+      <c r="C2" s="334"/>
       <c r="D2" s="75"/>
       <c r="E2" s="75"/>
       <c r="F2" s="75"/>
@@ -26268,28 +26268,28 @@
       <c r="N2" s="75"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B3" s="279" t="s">
+      <c r="B3" s="293" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="279"/>
-      <c r="D3" s="279"/>
-      <c r="E3" s="279"/>
-      <c r="F3" s="279"/>
-      <c r="G3" s="279"/>
-      <c r="H3" s="279"/>
-      <c r="I3" s="279"/>
-      <c r="J3" s="279"/>
-      <c r="K3" s="279"/>
-      <c r="L3" s="279"/>
-      <c r="M3" s="279"/>
+      <c r="C3" s="293"/>
+      <c r="D3" s="293"/>
+      <c r="E3" s="293"/>
+      <c r="F3" s="293"/>
+      <c r="G3" s="293"/>
+      <c r="H3" s="293"/>
+      <c r="I3" s="293"/>
+      <c r="J3" s="293"/>
+      <c r="K3" s="293"/>
+      <c r="L3" s="293"/>
+      <c r="M3" s="293"/>
       <c r="N3" s="75"/>
-      <c r="O3" s="318" t="s">
+      <c r="O3" s="332" t="s">
         <v>153</v>
       </c>
-      <c r="P3" s="318"/>
-      <c r="Q3" s="318"/>
-      <c r="R3" s="318"/>
-      <c r="S3" s="279"/>
+      <c r="P3" s="332"/>
+      <c r="Q3" s="332"/>
+      <c r="R3" s="332"/>
+      <c r="S3" s="293"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" s="77">
@@ -26329,164 +26329,164 @@
         <v>12</v>
       </c>
       <c r="N4" s="145"/>
-      <c r="O4" s="318"/>
-      <c r="P4" s="318"/>
-      <c r="Q4" s="318"/>
-      <c r="R4" s="318"/>
-      <c r="S4" s="279"/>
+      <c r="O4" s="332"/>
+      <c r="P4" s="332"/>
+      <c r="Q4" s="332"/>
+      <c r="R4" s="332"/>
+      <c r="S4" s="293"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B5" s="321" t="s">
+      <c r="B5" s="335" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="297"/>
-      <c r="D5" s="321" t="s">
+      <c r="C5" s="295"/>
+      <c r="D5" s="335" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="297"/>
-      <c r="F5" s="321" t="s">
+      <c r="E5" s="295"/>
+      <c r="F5" s="335" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="297"/>
-      <c r="H5" s="321" t="s">
+      <c r="G5" s="295"/>
+      <c r="H5" s="335" t="s">
         <v>74</v>
       </c>
-      <c r="I5" s="297"/>
-      <c r="J5" s="321" t="s">
+      <c r="I5" s="295"/>
+      <c r="J5" s="335" t="s">
         <v>73</v>
       </c>
-      <c r="K5" s="322"/>
-      <c r="L5" s="321" t="s">
+      <c r="K5" s="336"/>
+      <c r="L5" s="335" t="s">
         <v>74</v>
       </c>
-      <c r="M5" s="322"/>
+      <c r="M5" s="336"/>
       <c r="N5" s="161"/>
-      <c r="S5" s="279"/>
+      <c r="S5" s="293"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6" s="78"/>
-      <c r="O6" s="281" t="s">
+      <c r="O6" s="299" t="s">
         <v>155</v>
       </c>
-      <c r="P6" s="281"/>
-      <c r="Q6" s="281"/>
-      <c r="R6" s="281"/>
-      <c r="S6" s="279"/>
+      <c r="P6" s="299"/>
+      <c r="Q6" s="299"/>
+      <c r="R6" s="299"/>
+      <c r="S6" s="293"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B7" s="318" t="s">
+      <c r="B7" s="332" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="318"/>
-      <c r="D7" s="318"/>
-      <c r="E7" s="318"/>
-      <c r="F7" s="318"/>
-      <c r="G7" s="318"/>
-      <c r="H7" s="318"/>
-      <c r="I7" s="318"/>
-      <c r="J7" s="318"/>
-      <c r="K7" s="318"/>
-      <c r="L7" s="318"/>
-      <c r="M7" s="318"/>
+      <c r="C7" s="332"/>
+      <c r="D7" s="332"/>
+      <c r="E7" s="332"/>
+      <c r="F7" s="332"/>
+      <c r="G7" s="332"/>
+      <c r="H7" s="332"/>
+      <c r="I7" s="332"/>
+      <c r="J7" s="332"/>
+      <c r="K7" s="332"/>
+      <c r="L7" s="332"/>
+      <c r="M7" s="332"/>
       <c r="N7" s="160"/>
-      <c r="O7" s="281"/>
-      <c r="P7" s="281"/>
-      <c r="Q7" s="281"/>
-      <c r="R7" s="281"/>
-      <c r="S7" s="279"/>
+      <c r="O7" s="299"/>
+      <c r="P7" s="299"/>
+      <c r="Q7" s="299"/>
+      <c r="R7" s="299"/>
+      <c r="S7" s="293"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B8" s="318"/>
-      <c r="C8" s="318"/>
-      <c r="D8" s="318"/>
-      <c r="E8" s="318"/>
-      <c r="F8" s="318"/>
-      <c r="G8" s="318"/>
-      <c r="H8" s="318"/>
-      <c r="I8" s="318"/>
-      <c r="J8" s="318"/>
-      <c r="K8" s="318"/>
-      <c r="L8" s="318"/>
-      <c r="M8" s="318"/>
+      <c r="B8" s="332"/>
+      <c r="C8" s="332"/>
+      <c r="D8" s="332"/>
+      <c r="E8" s="332"/>
+      <c r="F8" s="332"/>
+      <c r="G8" s="332"/>
+      <c r="H8" s="332"/>
+      <c r="I8" s="332"/>
+      <c r="J8" s="332"/>
+      <c r="K8" s="332"/>
+      <c r="L8" s="332"/>
+      <c r="M8" s="332"/>
       <c r="N8" s="160"/>
-      <c r="O8" s="281"/>
-      <c r="P8" s="281"/>
-      <c r="Q8" s="281"/>
-      <c r="R8" s="281"/>
-      <c r="S8" s="279"/>
+      <c r="O8" s="299"/>
+      <c r="P8" s="299"/>
+      <c r="Q8" s="299"/>
+      <c r="R8" s="299"/>
+      <c r="S8" s="293"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B9" s="318"/>
-      <c r="C9" s="318"/>
-      <c r="D9" s="318"/>
-      <c r="E9" s="318"/>
-      <c r="F9" s="318"/>
-      <c r="G9" s="318"/>
-      <c r="H9" s="318"/>
-      <c r="I9" s="318"/>
-      <c r="J9" s="318"/>
-      <c r="K9" s="318"/>
-      <c r="L9" s="318"/>
-      <c r="M9" s="318"/>
+      <c r="B9" s="332"/>
+      <c r="C9" s="332"/>
+      <c r="D9" s="332"/>
+      <c r="E9" s="332"/>
+      <c r="F9" s="332"/>
+      <c r="G9" s="332"/>
+      <c r="H9" s="332"/>
+      <c r="I9" s="332"/>
+      <c r="J9" s="332"/>
+      <c r="K9" s="332"/>
+      <c r="L9" s="332"/>
+      <c r="M9" s="332"/>
       <c r="N9" s="160"/>
-      <c r="O9" s="281"/>
-      <c r="P9" s="281"/>
-      <c r="Q9" s="281"/>
-      <c r="R9" s="281"/>
-      <c r="S9" s="279"/>
+      <c r="O9" s="299"/>
+      <c r="P9" s="299"/>
+      <c r="Q9" s="299"/>
+      <c r="R9" s="299"/>
+      <c r="S9" s="293"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B10" s="318"/>
-      <c r="C10" s="318"/>
-      <c r="D10" s="318"/>
-      <c r="E10" s="318"/>
-      <c r="F10" s="318"/>
-      <c r="G10" s="318"/>
-      <c r="H10" s="318"/>
-      <c r="I10" s="318"/>
-      <c r="J10" s="318"/>
-      <c r="K10" s="318"/>
-      <c r="L10" s="318"/>
-      <c r="M10" s="318"/>
+      <c r="B10" s="332"/>
+      <c r="C10" s="332"/>
+      <c r="D10" s="332"/>
+      <c r="E10" s="332"/>
+      <c r="F10" s="332"/>
+      <c r="G10" s="332"/>
+      <c r="H10" s="332"/>
+      <c r="I10" s="332"/>
+      <c r="J10" s="332"/>
+      <c r="K10" s="332"/>
+      <c r="L10" s="332"/>
+      <c r="M10" s="332"/>
       <c r="N10" s="160"/>
-      <c r="O10" s="281"/>
-      <c r="P10" s="281"/>
-      <c r="Q10" s="281"/>
-      <c r="R10" s="281"/>
-      <c r="S10" s="279"/>
+      <c r="O10" s="299"/>
+      <c r="P10" s="299"/>
+      <c r="Q10" s="299"/>
+      <c r="R10" s="299"/>
+      <c r="S10" s="293"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B11" s="318"/>
-      <c r="C11" s="318"/>
-      <c r="D11" s="318"/>
-      <c r="E11" s="318"/>
-      <c r="F11" s="318"/>
-      <c r="G11" s="318"/>
-      <c r="H11" s="318"/>
-      <c r="I11" s="318"/>
-      <c r="J11" s="318"/>
-      <c r="K11" s="318"/>
-      <c r="L11" s="318"/>
-      <c r="M11" s="318"/>
+      <c r="B11" s="332"/>
+      <c r="C11" s="332"/>
+      <c r="D11" s="332"/>
+      <c r="E11" s="332"/>
+      <c r="F11" s="332"/>
+      <c r="G11" s="332"/>
+      <c r="H11" s="332"/>
+      <c r="I11" s="332"/>
+      <c r="J11" s="332"/>
+      <c r="K11" s="332"/>
+      <c r="L11" s="332"/>
+      <c r="M11" s="332"/>
       <c r="N11" s="160"/>
-      <c r="O11" s="281"/>
-      <c r="P11" s="281"/>
-      <c r="Q11" s="281"/>
-      <c r="R11" s="281"/>
-      <c r="S11" s="279"/>
+      <c r="O11" s="299"/>
+      <c r="P11" s="299"/>
+      <c r="Q11" s="299"/>
+      <c r="R11" s="299"/>
+      <c r="S11" s="293"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="O12" s="281"/>
-      <c r="P12" s="281"/>
-      <c r="Q12" s="281"/>
-      <c r="R12" s="281"/>
-      <c r="S12" s="279"/>
+      <c r="O12" s="299"/>
+      <c r="P12" s="299"/>
+      <c r="Q12" s="299"/>
+      <c r="R12" s="299"/>
+      <c r="S12" s="293"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B13" s="319" t="s">
+      <c r="B13" s="333" t="s">
         <v>161</v>
       </c>
-      <c r="C13" s="319"/>
+      <c r="C13" s="333"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B14" s="75">
@@ -26503,12 +26503,12 @@
       <c r="C15" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="O15" s="281" t="s">
+      <c r="O15" s="299" t="s">
         <v>154</v>
       </c>
-      <c r="P15" s="281"/>
-      <c r="Q15" s="281"/>
-      <c r="R15" s="281"/>
+      <c r="P15" s="299"/>
+      <c r="Q15" s="299"/>
+      <c r="R15" s="299"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B16" s="75">
@@ -26517,10 +26517,10 @@
       <c r="C16" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="O16" s="281"/>
-      <c r="P16" s="281"/>
-      <c r="Q16" s="281"/>
-      <c r="R16" s="281"/>
+      <c r="O16" s="299"/>
+      <c r="P16" s="299"/>
+      <c r="Q16" s="299"/>
+      <c r="R16" s="299"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B17" s="75">
@@ -26537,12 +26537,12 @@
       <c r="C18" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="O18" s="281" t="s">
+      <c r="O18" s="299" t="s">
         <v>156</v>
       </c>
-      <c r="P18" s="281"/>
-      <c r="Q18" s="281"/>
-      <c r="R18" s="281"/>
+      <c r="P18" s="299"/>
+      <c r="Q18" s="299"/>
+      <c r="R18" s="299"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B19" s="75">
@@ -26551,97 +26551,97 @@
       <c r="C19" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="O19" s="281"/>
-      <c r="P19" s="281"/>
-      <c r="Q19" s="281"/>
-      <c r="R19" s="281"/>
+      <c r="O19" s="299"/>
+      <c r="P19" s="299"/>
+      <c r="Q19" s="299"/>
+      <c r="R19" s="299"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O20" s="281"/>
-      <c r="P20" s="281"/>
-      <c r="Q20" s="281"/>
-      <c r="R20" s="281"/>
+      <c r="O20" s="299"/>
+      <c r="P20" s="299"/>
+      <c r="Q20" s="299"/>
+      <c r="R20" s="299"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O21" s="281"/>
-      <c r="P21" s="281"/>
-      <c r="Q21" s="281"/>
-      <c r="R21" s="281"/>
+      <c r="O21" s="299"/>
+      <c r="P21" s="299"/>
+      <c r="Q21" s="299"/>
+      <c r="R21" s="299"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O22" s="281"/>
-      <c r="P22" s="281"/>
-      <c r="Q22" s="281"/>
-      <c r="R22" s="281"/>
+      <c r="O22" s="299"/>
+      <c r="P22" s="299"/>
+      <c r="Q22" s="299"/>
+      <c r="R22" s="299"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O23" s="281"/>
-      <c r="P23" s="281"/>
-      <c r="Q23" s="281"/>
-      <c r="R23" s="281"/>
+      <c r="O23" s="299"/>
+      <c r="P23" s="299"/>
+      <c r="Q23" s="299"/>
+      <c r="R23" s="299"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O27" s="318" t="s">
+      <c r="O27" s="332" t="s">
         <v>152</v>
       </c>
-      <c r="P27" s="318"/>
-      <c r="Q27" s="318"/>
-      <c r="R27" s="318"/>
+      <c r="P27" s="332"/>
+      <c r="Q27" s="332"/>
+      <c r="R27" s="332"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O28" s="318"/>
-      <c r="P28" s="318"/>
-      <c r="Q28" s="318"/>
-      <c r="R28" s="318"/>
+      <c r="O28" s="332"/>
+      <c r="P28" s="332"/>
+      <c r="Q28" s="332"/>
+      <c r="R28" s="332"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O30" s="281" t="s">
+      <c r="O30" s="299" t="s">
         <v>151</v>
       </c>
-      <c r="P30" s="281"/>
-      <c r="Q30" s="281"/>
-      <c r="R30" s="281"/>
+      <c r="P30" s="299"/>
+      <c r="Q30" s="299"/>
+      <c r="R30" s="299"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O31" s="281"/>
-      <c r="P31" s="281"/>
-      <c r="Q31" s="281"/>
-      <c r="R31" s="281"/>
+      <c r="O31" s="299"/>
+      <c r="P31" s="299"/>
+      <c r="Q31" s="299"/>
+      <c r="R31" s="299"/>
     </row>
     <row r="32" spans="2:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M32" s="89"/>
       <c r="N32" s="89"/>
-      <c r="O32" s="281"/>
-      <c r="P32" s="281"/>
-      <c r="Q32" s="281"/>
-      <c r="R32" s="281"/>
+      <c r="O32" s="299"/>
+      <c r="P32" s="299"/>
+      <c r="Q32" s="299"/>
+      <c r="R32" s="299"/>
     </row>
     <row r="33" spans="12:18" x14ac:dyDescent="0.35">
       <c r="L33" s="89"/>
       <c r="M33" s="89"/>
       <c r="N33" s="89"/>
-      <c r="O33" s="281"/>
-      <c r="P33" s="281"/>
-      <c r="Q33" s="281"/>
-      <c r="R33" s="281"/>
+      <c r="O33" s="299"/>
+      <c r="P33" s="299"/>
+      <c r="Q33" s="299"/>
+      <c r="R33" s="299"/>
     </row>
     <row r="34" spans="12:18" x14ac:dyDescent="0.35">
       <c r="L34" s="89"/>
       <c r="M34" s="89"/>
       <c r="N34" s="89"/>
-      <c r="O34" s="281"/>
-      <c r="P34" s="281"/>
-      <c r="Q34" s="281"/>
-      <c r="R34" s="281"/>
+      <c r="O34" s="299"/>
+      <c r="P34" s="299"/>
+      <c r="Q34" s="299"/>
+      <c r="R34" s="299"/>
     </row>
     <row r="35" spans="12:18" x14ac:dyDescent="0.35">
       <c r="L35" s="89"/>
       <c r="M35" s="89"/>
       <c r="N35" s="89"/>
-      <c r="O35" s="281"/>
-      <c r="P35" s="281"/>
-      <c r="Q35" s="281"/>
-      <c r="R35" s="281"/>
+      <c r="O35" s="299"/>
+      <c r="P35" s="299"/>
+      <c r="Q35" s="299"/>
+      <c r="R35" s="299"/>
     </row>
     <row r="36" spans="12:18" x14ac:dyDescent="0.35">
       <c r="L36" s="89"/>
@@ -26669,11 +26669,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="O30:R35"/>
-    <mergeCell ref="O15:R16"/>
-    <mergeCell ref="O3:R4"/>
-    <mergeCell ref="O18:R23"/>
-    <mergeCell ref="O6:R12"/>
     <mergeCell ref="B7:M11"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="S3:S12"/>
@@ -26686,6 +26681,11 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
+    <mergeCell ref="O30:R35"/>
+    <mergeCell ref="O15:R16"/>
+    <mergeCell ref="O3:R4"/>
+    <mergeCell ref="O18:R23"/>
+    <mergeCell ref="O6:R12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="55" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -26700,8 +26700,8 @@
   </sheetPr>
   <dimension ref="B3:R23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="81" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="81" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -26713,57 +26713,57 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="329" t="s">
+      <c r="B3" s="340" t="s">
         <v>162</v>
       </c>
-      <c r="C3" s="333"/>
-      <c r="D3" s="333"/>
-      <c r="E3" s="333"/>
-      <c r="F3" s="329" t="s">
+      <c r="C3" s="344"/>
+      <c r="D3" s="344"/>
+      <c r="E3" s="344"/>
+      <c r="F3" s="340" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="329"/>
-      <c r="H3" s="329"/>
-      <c r="I3" s="329"/>
-      <c r="J3" s="329"/>
-      <c r="K3" s="329"/>
-      <c r="L3" s="329"/>
-      <c r="M3" s="329"/>
-      <c r="N3" s="329"/>
-      <c r="O3" s="329"/>
-      <c r="P3" s="329"/>
-      <c r="Q3" s="329"/>
+      <c r="G3" s="340"/>
+      <c r="H3" s="340"/>
+      <c r="I3" s="340"/>
+      <c r="J3" s="340"/>
+      <c r="K3" s="340"/>
+      <c r="L3" s="340"/>
+      <c r="M3" s="340"/>
+      <c r="N3" s="340"/>
+      <c r="O3" s="340"/>
+      <c r="P3" s="340"/>
+      <c r="Q3" s="340"/>
     </row>
     <row r="4" spans="2:18" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="337" t="s">
+      <c r="B4" s="348" t="s">
         <v>170</v>
       </c>
-      <c r="C4" s="337"/>
-      <c r="D4" s="337"/>
-      <c r="E4" s="337"/>
-      <c r="F4" s="338" t="s">
+      <c r="C4" s="348"/>
+      <c r="D4" s="348"/>
+      <c r="E4" s="348"/>
+      <c r="F4" s="349" t="s">
         <v>171</v>
       </c>
-      <c r="G4" s="338"/>
-      <c r="H4" s="338"/>
-      <c r="I4" s="338"/>
-      <c r="J4" s="338"/>
-      <c r="K4" s="338"/>
-      <c r="L4" s="338"/>
-      <c r="M4" s="338"/>
-      <c r="N4" s="338"/>
-      <c r="O4" s="338"/>
-      <c r="P4" s="338"/>
-      <c r="Q4" s="338"/>
+      <c r="G4" s="349"/>
+      <c r="H4" s="349"/>
+      <c r="I4" s="349"/>
+      <c r="J4" s="349"/>
+      <c r="K4" s="349"/>
+      <c r="L4" s="349"/>
+      <c r="M4" s="349"/>
+      <c r="N4" s="349"/>
+      <c r="O4" s="349"/>
+      <c r="P4" s="349"/>
+      <c r="Q4" s="349"/>
       <c r="R4" s="206"/>
     </row>
     <row r="5" spans="2:18" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="334">
+      <c r="B5" s="345">
         <v>80</v>
       </c>
-      <c r="C5" s="335"/>
-      <c r="D5" s="335"/>
-      <c r="E5" s="336"/>
+      <c r="C5" s="346"/>
+      <c r="D5" s="346"/>
+      <c r="E5" s="347"/>
       <c r="F5" s="205">
         <v>6</v>
       </c>
@@ -26842,29 +26842,29 @@
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B8" s="207"/>
-      <c r="C8" s="332" t="s">
+      <c r="C8" s="343" t="s">
         <v>165</v>
       </c>
-      <c r="D8" s="332"/>
+      <c r="D8" s="343"/>
       <c r="E8" s="197"/>
       <c r="F8" s="212"/>
       <c r="G8" s="213"/>
-      <c r="H8" s="327" t="s">
+      <c r="H8" s="338" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="328"/>
+      <c r="I8" s="339"/>
       <c r="J8" s="212"/>
       <c r="K8" s="213"/>
-      <c r="L8" s="327" t="s">
+      <c r="L8" s="338" t="s">
         <v>74</v>
       </c>
-      <c r="M8" s="328"/>
+      <c r="M8" s="339"/>
       <c r="N8" s="212"/>
       <c r="O8" s="213"/>
-      <c r="P8" s="330" t="s">
+      <c r="P8" s="341" t="s">
         <v>74</v>
       </c>
-      <c r="Q8" s="331"/>
+      <c r="Q8" s="342"/>
       <c r="R8" s="196"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.35">
@@ -26876,22 +26876,22 @@
         <v>20</v>
       </c>
       <c r="E9" s="199"/>
-      <c r="F9" s="326" t="s">
+      <c r="F9" s="354" t="s">
         <v>73</v>
       </c>
-      <c r="G9" s="326"/>
+      <c r="G9" s="354"/>
       <c r="H9" s="216"/>
       <c r="I9" s="217"/>
-      <c r="J9" s="326" t="s">
+      <c r="J9" s="354" t="s">
         <v>73</v>
       </c>
-      <c r="K9" s="326"/>
+      <c r="K9" s="354"/>
       <c r="L9" s="218"/>
       <c r="M9" s="218"/>
-      <c r="N9" s="326" t="s">
+      <c r="N9" s="354" t="s">
         <v>73</v>
       </c>
-      <c r="O9" s="326"/>
+      <c r="O9" s="354"/>
       <c r="P9" s="218"/>
       <c r="Q9" s="218"/>
       <c r="R9" s="196"/>
@@ -26924,28 +26924,28 @@
       <c r="C11" s="201"/>
       <c r="D11" s="201"/>
       <c r="E11" s="201"/>
-      <c r="F11" s="339" t="s">
+      <c r="F11" s="350" t="s">
         <v>174</v>
       </c>
-      <c r="G11" s="339"/>
-      <c r="H11" s="339"/>
-      <c r="I11" s="339"/>
-      <c r="J11" s="339"/>
-      <c r="K11" s="339"/>
-      <c r="L11" s="339"/>
-      <c r="M11" s="339"/>
-      <c r="N11" s="339"/>
-      <c r="O11" s="339"/>
-      <c r="P11" s="339"/>
-      <c r="Q11" s="339"/>
+      <c r="G11" s="350"/>
+      <c r="H11" s="350"/>
+      <c r="I11" s="350"/>
+      <c r="J11" s="350"/>
+      <c r="K11" s="350"/>
+      <c r="L11" s="350"/>
+      <c r="M11" s="350"/>
+      <c r="N11" s="350"/>
+      <c r="O11" s="350"/>
+      <c r="P11" s="350"/>
+      <c r="Q11" s="350"/>
       <c r="R11" s="196"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B12" s="202"/>
-      <c r="C12" s="332" t="s">
+      <c r="C12" s="343" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="332"/>
+      <c r="D12" s="343"/>
       <c r="E12" s="202"/>
       <c r="F12" s="226"/>
       <c r="G12" s="226"/>
@@ -26973,15 +26973,15 @@
       <c r="F13" s="227"/>
       <c r="G13" s="228"/>
       <c r="H13" s="227"/>
-      <c r="I13" s="325" t="s">
+      <c r="I13" s="353" t="s">
         <v>176</v>
       </c>
-      <c r="J13" s="325"/>
-      <c r="K13" s="325"/>
-      <c r="L13" s="325"/>
-      <c r="M13" s="325"/>
-      <c r="N13" s="325"/>
-      <c r="O13" s="325"/>
+      <c r="J13" s="353"/>
+      <c r="K13" s="353"/>
+      <c r="L13" s="353"/>
+      <c r="M13" s="353"/>
+      <c r="N13" s="353"/>
+      <c r="O13" s="353"/>
       <c r="P13" s="229"/>
       <c r="Q13" s="229"/>
       <c r="R13" s="196"/>
@@ -27002,9 +27002,9 @@
       <c r="J14" s="244" t="s">
         <v>177</v>
       </c>
-      <c r="K14" s="324"/>
-      <c r="L14" s="324"/>
-      <c r="M14" s="324"/>
+      <c r="K14" s="352"/>
+      <c r="L14" s="352"/>
+      <c r="M14" s="352"/>
       <c r="N14" s="244" t="s">
         <v>178</v>
       </c>
@@ -27084,13 +27084,13 @@
       <c r="G17" s="227"/>
       <c r="H17" s="227"/>
       <c r="I17" s="237"/>
-      <c r="J17" s="323" t="s">
+      <c r="J17" s="351" t="s">
         <v>175</v>
       </c>
-      <c r="K17" s="323"/>
-      <c r="L17" s="323"/>
-      <c r="M17" s="323"/>
-      <c r="N17" s="323"/>
+      <c r="K17" s="351"/>
+      <c r="L17" s="351"/>
+      <c r="M17" s="351"/>
+      <c r="N17" s="351"/>
       <c r="O17" s="238"/>
       <c r="P17" s="227"/>
       <c r="Q17" s="227"/>
@@ -27132,63 +27132,65 @@
       <c r="Q19" s="227"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B21" s="340" t="s">
+      <c r="B21" s="337" t="s">
         <v>191</v>
       </c>
-      <c r="C21" s="340"/>
-      <c r="D21" s="340"/>
-      <c r="E21" s="340"/>
-      <c r="F21" s="340"/>
-      <c r="G21" s="340"/>
-      <c r="H21" s="340"/>
-      <c r="I21" s="340"/>
-      <c r="J21" s="340"/>
-      <c r="K21" s="340"/>
-      <c r="L21" s="340"/>
-      <c r="M21" s="340"/>
-      <c r="N21" s="340"/>
-      <c r="O21" s="340"/>
-      <c r="P21" s="340"/>
-      <c r="Q21" s="340"/>
+      <c r="C21" s="337"/>
+      <c r="D21" s="337"/>
+      <c r="E21" s="337"/>
+      <c r="F21" s="337"/>
+      <c r="G21" s="337"/>
+      <c r="H21" s="337"/>
+      <c r="I21" s="337"/>
+      <c r="J21" s="337"/>
+      <c r="K21" s="337"/>
+      <c r="L21" s="337"/>
+      <c r="M21" s="337"/>
+      <c r="N21" s="337"/>
+      <c r="O21" s="337"/>
+      <c r="P21" s="337"/>
+      <c r="Q21" s="337"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B22" s="340"/>
-      <c r="C22" s="340"/>
-      <c r="D22" s="340"/>
-      <c r="E22" s="340"/>
-      <c r="F22" s="340"/>
-      <c r="G22" s="340"/>
-      <c r="H22" s="340"/>
-      <c r="I22" s="340"/>
-      <c r="J22" s="340"/>
-      <c r="K22" s="340"/>
-      <c r="L22" s="340"/>
-      <c r="M22" s="340"/>
-      <c r="N22" s="340"/>
-      <c r="O22" s="340"/>
-      <c r="P22" s="340"/>
-      <c r="Q22" s="340"/>
+      <c r="B22" s="337"/>
+      <c r="C22" s="337"/>
+      <c r="D22" s="337"/>
+      <c r="E22" s="337"/>
+      <c r="F22" s="337"/>
+      <c r="G22" s="337"/>
+      <c r="H22" s="337"/>
+      <c r="I22" s="337"/>
+      <c r="J22" s="337"/>
+      <c r="K22" s="337"/>
+      <c r="L22" s="337"/>
+      <c r="M22" s="337"/>
+      <c r="N22" s="337"/>
+      <c r="O22" s="337"/>
+      <c r="P22" s="337"/>
+      <c r="Q22" s="337"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B23" s="340"/>
-      <c r="C23" s="340"/>
-      <c r="D23" s="340"/>
-      <c r="E23" s="340"/>
-      <c r="F23" s="340"/>
-      <c r="G23" s="340"/>
-      <c r="H23" s="340"/>
-      <c r="I23" s="340"/>
-      <c r="J23" s="340"/>
-      <c r="K23" s="340"/>
-      <c r="L23" s="340"/>
-      <c r="M23" s="340"/>
-      <c r="N23" s="340"/>
-      <c r="O23" s="340"/>
-      <c r="P23" s="340"/>
-      <c r="Q23" s="340"/>
+      <c r="B23" s="337"/>
+      <c r="C23" s="337"/>
+      <c r="D23" s="337"/>
+      <c r="E23" s="337"/>
+      <c r="F23" s="337"/>
+      <c r="G23" s="337"/>
+      <c r="H23" s="337"/>
+      <c r="I23" s="337"/>
+      <c r="J23" s="337"/>
+      <c r="K23" s="337"/>
+      <c r="L23" s="337"/>
+      <c r="M23" s="337"/>
+      <c r="N23" s="337"/>
+      <c r="O23" s="337"/>
+      <c r="P23" s="337"/>
+      <c r="Q23" s="337"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="N9:O9"/>
     <mergeCell ref="B21:Q23"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="F3:Q3"/>
@@ -27205,8 +27207,6 @@
     <mergeCell ref="K14:M14"/>
     <mergeCell ref="I13:O13"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="N9:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>